<commit_message>
Add numbers of events and patients to HR forest plot panels
</commit_message>
<xml_diff>
--- a/products/Exported Data.xlsx
+++ b/products/Exported Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14994" uniqueCount="8755">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15614" uniqueCount="9115">
   <si>
     <t>Study</t>
   </si>
@@ -19313,6 +19313,1086 @@
   </si>
   <si>
     <t>Study</t>
+  </si>
+  <si>
+    <t>Attal 2019 (ICARIA-MM): IsPd vs Pd</t>
+  </si>
+  <si>
+    <t>Bahlis 2020 (POLLUX): DRd vs Rd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2013 (VANTAGE 088): VorV vs V</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2016 (ENDEAVOR): Kd vs Vd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2018 (ELOQUENT-3): EPd vs Pd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2021 (APOLLO): DPd vs Pd</t>
+  </si>
+  <si>
+    <t>Hou 2017 (China Cont.): IRd vs Rd</t>
+  </si>
+  <si>
+    <t>Jakubowiak 2016 (NCT01478048): EVd vs Vd</t>
+  </si>
+  <si>
+    <t>Kumar 2020 (BELLINI): VeVd vs Vd</t>
+  </si>
+  <si>
+    <t>Lonial 2015 (ELOQUENT-2): ELd vs Ld</t>
+  </si>
+  <si>
+    <t>Lu 2021 (LEPUS): DVd vs Vd</t>
+  </si>
+  <si>
+    <t>Mateos 2020 (CASTOR): DVd vs Vd</t>
+  </si>
+  <si>
+    <t>Moreau 2021 (IKEMA): IsKd vs Kd</t>
+  </si>
+  <si>
+    <t>Orlowski 2007 (NCT00103506): V vs DoxV</t>
+  </si>
+  <si>
+    <t>Orlowski 2016 (NCT00103506): V vs DoxV</t>
+  </si>
+  <si>
+    <t>Orlowski 2019 (ENDEAVOR): Kd vs Vd</t>
+  </si>
+  <si>
+    <t>Richardson 2019 (OPTIMISMM): PVd vs Vd</t>
+  </si>
+  <si>
+    <t>Richardson 2021 (TOURMALINE-MM1): IRd vs Rd</t>
+  </si>
+  <si>
+    <t>San-Miguel 2016 (PANORAMA 1): FVd vs Vd</t>
+  </si>
+  <si>
+    <t>Stewart 2015 (ASPIRE): KRd vs Rd</t>
+  </si>
+  <si>
+    <t>Usmani 2022 (CANDOR): DKd vs Kd</t>
+  </si>
+  <si>
+    <t>refract</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Previous R use</t>
+  </si>
+  <si>
+    <t>No previous R use</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No IMiD use</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Ref. to R and a PI</t>
+  </si>
+  <si>
+    <t>Not ref. to R and a PI</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No IMiD use</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No IMiD use</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No IMiD use</t>
+  </si>
+  <si>
+    <t>Naive</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Naive</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Previous R use</t>
+  </si>
+  <si>
+    <t>No previous R use</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Not refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Not refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Previous R or T use</t>
+  </si>
+  <si>
+    <t>No previous R or T use</t>
+  </si>
+  <si>
+    <t>Previous R or T use</t>
+  </si>
+  <si>
+    <t>No previous R or T use</t>
+  </si>
+  <si>
+    <t>Previous R use</t>
+  </si>
+  <si>
+    <t>No previous R use</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Refractory to T</t>
+  </si>
+  <si>
+    <t>Not refractory to T</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No previous IMiD use</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Not refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Outcome</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Lower 95% CI Bound on HR</t>
+  </si>
+  <si>
+    <t>Upper 95% CI Bound on HR</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0230</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .       Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tab. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      p. 808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. S3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. S4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t>Data Extraction Errors</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Study: Treatment 1 vs Treatment 2</t>
+  </si>
+  <si>
+    <t>Attal 2019 (ICARIA-MM): IsPd vs Pd</t>
+  </si>
+  <si>
+    <t>Bahlis 2020 (POLLUX): DRd vs Rd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2013 (VANTAGE 088): VorV vs V</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2016 (ENDEAVOR): Kd vs Vd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2018 (ELOQUENT-3): EPd vs Pd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2018 (ELOQUENT-2): ELd vs Ld</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2020 (ELOQUENT-2): ELd vs Ld</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2021 (APOLLO): DPd vs Pd</t>
+  </si>
+  <si>
+    <t>Grosicki 2020 (BOSTON): SeVd vs Vd</t>
+  </si>
+  <si>
+    <t>Hou 2017 (China Cont.): IRd vs Rd</t>
+  </si>
+  <si>
+    <t>Jakubowiak 2016 (NCT01478048): EVd vs Vd</t>
+  </si>
+  <si>
+    <t>Kumar 2020 (BELLINI): VeVd vs Vd</t>
+  </si>
+  <si>
+    <t>Lu 2021 (LEPUS): DVd vs Vd</t>
+  </si>
+  <si>
+    <t>Mateos 2020 (CASTOR): DVd vs Vd</t>
+  </si>
+  <si>
+    <t>Moreau 2021 (IKEMA): IsKd vs Kd</t>
+  </si>
+  <si>
+    <t>Orlowski 2019 (ENDEAVOR): Kd vs Vd</t>
+  </si>
+  <si>
+    <t>Richardson 2019 (OPTIMISMM): PVd vs Vd</t>
+  </si>
+  <si>
+    <t>Richardson 2021 (TOURMALINE-MM1): IRd vs Rd</t>
+  </si>
+  <si>
+    <t>San-Miguel 2014 (PANORAMA-1): FVd vs Vd</t>
+  </si>
+  <si>
+    <t>San-Miguel 2016 (PANORAMA 1): FVd vs Vd</t>
+  </si>
+  <si>
+    <t>San-Miguel 2013 (MM-003): Pd vs GC</t>
+  </si>
+  <si>
+    <t>Siegel 2018 (ASPIRE): KRd vs Rd</t>
+  </si>
+  <si>
+    <t>Usamani 2022 (CANDOR): DKd vs Kd</t>
+  </si>
+  <si>
+    <t>lot</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>&gt;3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>&gt;3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>&gt;=4</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>&gt;=4</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>&gt;3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>&gt;3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>&gt;1</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>&gt;2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>&gt;=3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>&gt;2</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>&gt;2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>&gt;=2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>Outcome</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Lower 95% CI Bound on HR</t>
+  </si>
+  <si>
+    <t>Upper 95% CI Bound on HR</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t>Tab. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tab. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      p. 808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. S3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. S4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      AT 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      p. 730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t>Data Extraction Errors</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Study: Treatment 1 vs Treatment 2</t>
   </si>
   <si>
     <t>Attal 2019 (ICARIA-MM): IsPd vs Pd</t>
@@ -26329,42 +27409,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>8395</v>
+        <v>8755</v>
       </c>
       <c r="B1" t="s">
-        <v>8419</v>
+        <v>8779</v>
       </c>
       <c r="C1" t="s">
-        <v>8483</v>
+        <v>8843</v>
       </c>
       <c r="D1" t="s">
-        <v>8499</v>
+        <v>8859</v>
       </c>
       <c r="E1" t="s">
-        <v>8500</v>
+        <v>8860</v>
       </c>
       <c r="F1" t="s">
-        <v>8501</v>
+        <v>8861</v>
       </c>
       <c r="G1" t="s">
-        <v>8502</v>
+        <v>8862</v>
       </c>
       <c r="H1" t="s">
-        <v>8503</v>
+        <v>8863</v>
       </c>
       <c r="I1" t="s">
-        <v>8527</v>
+        <v>8887</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>8396</v>
+        <v>8756</v>
       </c>
       <c r="B2" t="s">
-        <v>8420</v>
+        <v>8780</v>
       </c>
       <c r="C2" t="s">
-        <v>8484</v>
+        <v>8844</v>
       </c>
       <c r="D2" s="1">
         <v>0.5899999737739563</v>
@@ -26377,21 +27457,21 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" t="s">
-        <v>8504</v>
+        <v>8864</v>
       </c>
       <c r="I2" t="s">
-        <v>8528</v>
+        <v>8888</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8396</v>
+        <v>8756</v>
       </c>
       <c r="B3" t="s">
-        <v>8421</v>
+        <v>8781</v>
       </c>
       <c r="C3" t="s">
-        <v>8484</v>
+        <v>8844</v>
       </c>
       <c r="D3" s="1">
         <v>0.5899999737739563</v>
@@ -26404,21 +27484,21 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" t="s">
-        <v>8504</v>
+        <v>8864</v>
       </c>
       <c r="I3" t="s">
-        <v>8529</v>
+        <v>8889</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>8397</v>
+        <v>8757</v>
       </c>
       <c r="B4" t="s">
-        <v>8422</v>
+        <v>8782</v>
       </c>
       <c r="C4" t="s">
-        <v>8484</v>
+        <v>8844</v>
       </c>
       <c r="D4" s="1">
         <v>0.41999998688697815</v>
@@ -26431,21 +27511,21 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" t="s">
-        <v>8505</v>
+        <v>8865</v>
       </c>
       <c r="I4" t="s">
-        <v>8530</v>
+        <v>8890</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8397</v>
+        <v>8757</v>
       </c>
       <c r="B5" t="s">
-        <v>8423</v>
+        <v>8783</v>
       </c>
       <c r="C5" t="s">
-        <v>8484</v>
+        <v>8844</v>
       </c>
       <c r="D5" s="1">
         <v>0.38999998569488525</v>
@@ -26458,21 +27538,21 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" t="s">
-        <v>8505</v>
+        <v>8865</v>
       </c>
       <c r="I5" t="s">
-        <v>8531</v>
+        <v>8891</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8397</v>
+        <v>8757</v>
       </c>
       <c r="B6" t="s">
-        <v>8424</v>
+        <v>8784</v>
       </c>
       <c r="C6" t="s">
-        <v>8484</v>
+        <v>8844</v>
       </c>
       <c r="D6" s="1">
         <v>0.47999998927116394</v>
@@ -26485,21 +27565,21 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" t="s">
-        <v>8505</v>
+        <v>8865</v>
       </c>
       <c r="I6" t="s">
-        <v>8532</v>
+        <v>8892</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>8397</v>
+        <v>8757</v>
       </c>
       <c r="B7" t="s">
-        <v>8425</v>
+        <v>8785</v>
       </c>
       <c r="C7" t="s">
-        <v>8484</v>
+        <v>8844</v>
       </c>
       <c r="D7" s="1">
         <v>0.74000000953674316</v>
@@ -26512,21 +27592,21 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" t="s">
-        <v>8505</v>
+        <v>8865</v>
       </c>
       <c r="I7" t="s">
-        <v>8533</v>
+        <v>8893</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>8398</v>
+        <v>8758</v>
       </c>
       <c r="B8" t="s">
-        <v>8426</v>
+        <v>8786</v>
       </c>
       <c r="C8" t="s">
-        <v>8484</v>
+        <v>8844</v>
       </c>
       <c r="D8" s="1">
         <v>0.68699997663497925</v>
@@ -26541,21 +27621,21 @@
         <v>0.015200000256299973</v>
       </c>
       <c r="H8" t="s">
-        <v>8506</v>
+        <v>8866</v>
       </c>
       <c r="I8" t="s">
-        <v>8534</v>
+        <v>8894</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8398</v>
+        <v>8758</v>
       </c>
       <c r="B9" t="s">
-        <v>8427</v>
+        <v>8787</v>
       </c>
       <c r="C9" t="s">
-        <v>8484</v>
+        <v>8844</v>
       </c>
       <c r="D9" s="1">
         <v>0.91600000858306885</v>
@@ -26570,21 +27650,21 @@
         <v>0.48710000514984131</v>
       </c>
       <c r="H9" t="s">
-        <v>8507</v>
+        <v>8867</v>
       </c>
       <c r="I9" t="s">
-        <v>8535</v>
+        <v>8895</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>8399</v>
+        <v>8759</v>
       </c>
       <c r="B10" t="s">
-        <v>8428</v>
+        <v>8788</v>
       </c>
       <c r="C10" t="s">
-        <v>8484</v>
+        <v>8844</v>
       </c>
       <c r="D10" s="1">
         <v>0.44999998807907104</v>
@@ -26597,21 +27677,21 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" t="s">
-        <v>8508</v>
+        <v>8868</v>
       </c>
       <c r="I10" t="s">
-        <v>8536</v>
+        <v>8896</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>8399</v>
+        <v>8759</v>
       </c>
       <c r="B11" t="s">
-        <v>8429</v>
+        <v>8789</v>
       </c>
       <c r="C11" t="s">
-        <v>8484</v>
+        <v>8844</v>
       </c>
       <c r="D11" s="1">
         <v>0.60000002384185791</v>
@@ -26624,21 +27704,21 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" t="s">
-        <v>8508</v>
+        <v>8868</v>
       </c>
       <c r="I11" t="s">
-        <v>8537</v>
+        <v>8897</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>8400</v>
+        <v>8760</v>
       </c>
       <c r="B12" t="s">
-        <v>8429</v>
+        <v>8789</v>
       </c>
       <c r="C12" t="s">
-        <v>8484</v>
+        <v>8844</v>
       </c>
       <c r="D12" s="1">
         <v>0.55000001192092896</v>
@@ -26651,21 +27731,21 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" t="s">
-        <v>8509</v>
+        <v>8869</v>
       </c>
       <c r="I12" t="s">
-        <v>8538</v>
+        <v>8898</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>8400</v>
+        <v>8760</v>
       </c>
       <c r="B13" t="s">
-        <v>8430</v>
+        <v>8790</v>
       </c>
       <c r="C13" t="s">
-        <v>8484</v>
+        <v>8844</v>
       </c>
       <c r="D13" s="1">
         <v>0.50999999046325684</v>
@@ -26678,21 +27758,21 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" t="s">
-        <v>8509</v>
+        <v>8869</v>
       </c>
       <c r="I13" t="s">
-        <v>8539</v>
+        <v>8899</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>8401</v>
+        <v>8761</v>
       </c>
       <c r="B14" t="s">
-        <v>8431</v>
+        <v>8791</v>
       </c>
       <c r="C14" t="s">
-        <v>8484</v>
+        <v>8844</v>
       </c>
       <c r="D14" s="1">
         <v>0.76999998092651367</v>
@@ -26705,21 +27785,21 @@
       </c>
       <c r="G14" s="1"/>
       <c r="H14" t="s">
-        <v>8510</v>
+        <v>8870</v>
       </c>
       <c r="I14" t="s">
-        <v>8540</v>
+        <v>8900</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>8401</v>
+        <v>8761</v>
       </c>
       <c r="B15" t="s">
-        <v>8432</v>
+        <v>8792</v>
       </c>
       <c r="C15" t="s">
-        <v>8484</v>
+        <v>8844</v>
       </c>
       <c r="D15" s="1">
         <v>0.68000000715255737</v>
@@ -26732,21 +27812,21 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15" t="s">
-        <v>8510</v>
+        <v>8870</v>
       </c>
       <c r="I15" t="s">
-        <v>8541</v>
+        <v>8901</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>8402</v>
+        <v>8762</v>
       </c>
       <c r="B16" t="s">
-        <v>8433</v>
+        <v>8793</v>
       </c>
       <c r="C16" t="s">
-        <v>8485</v>
+        <v>8845</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
@@ -26759,21 +27839,21 @@
       </c>
       <c r="G16" s="1"/>
       <c r="H16" t="s">
-        <v>8510</v>
+        <v>8870</v>
       </c>
       <c r="I16" t="s">
-        <v>8542</v>
+        <v>8902</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>8402</v>
+        <v>8762</v>
       </c>
       <c r="B17" t="s">
-        <v>8434</v>
+        <v>8794</v>
       </c>
       <c r="C17" t="s">
-        <v>8485</v>
+        <v>8845</v>
       </c>
       <c r="D17" s="1">
         <v>0.70999997854232788</v>
@@ -26786,21 +27866,21 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" t="s">
-        <v>8510</v>
+        <v>8870</v>
       </c>
       <c r="I17" t="s">
-        <v>8543</v>
+        <v>8903</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>8403</v>
+        <v>8763</v>
       </c>
       <c r="B18" t="s">
-        <v>8435</v>
+        <v>8795</v>
       </c>
       <c r="C18" t="s">
-        <v>8486</v>
+        <v>8846</v>
       </c>
       <c r="D18" s="1">
         <v>0.69999998807907104</v>
@@ -26813,21 +27893,21 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" t="s">
-        <v>8511</v>
+        <v>8871</v>
       </c>
       <c r="I18" t="s">
-        <v>8544</v>
+        <v>8904</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>8403</v>
+        <v>8763</v>
       </c>
       <c r="B19" t="s">
-        <v>8436</v>
+        <v>8796</v>
       </c>
       <c r="C19" t="s">
-        <v>8486</v>
+        <v>8846</v>
       </c>
       <c r="D19" s="1">
         <v>0.6600000262260437</v>
@@ -26840,21 +27920,21 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19" t="s">
-        <v>8511</v>
+        <v>8871</v>
       </c>
       <c r="I19" t="s">
-        <v>8545</v>
+        <v>8905</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>8403</v>
+        <v>8763</v>
       </c>
       <c r="B20" t="s">
-        <v>8437</v>
+        <v>8797</v>
       </c>
       <c r="C20" t="s">
-        <v>8486</v>
+        <v>8846</v>
       </c>
       <c r="D20" s="1">
         <v>0.40000000596046448</v>
@@ -26867,21 +27947,21 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" t="s">
-        <v>8511</v>
+        <v>8871</v>
       </c>
       <c r="I20" t="s">
-        <v>8546</v>
+        <v>8906</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>8404</v>
+        <v>8764</v>
       </c>
       <c r="B21" t="s">
-        <v>8438</v>
+        <v>8798</v>
       </c>
       <c r="C21" t="s">
-        <v>8486</v>
+        <v>8846</v>
       </c>
       <c r="D21" s="1">
         <v>0.62999999523162842</v>
@@ -26894,21 +27974,21 @@
       </c>
       <c r="G21" s="1"/>
       <c r="H21" t="s">
-        <v>8512</v>
+        <v>8872</v>
       </c>
       <c r="I21" t="s">
-        <v>8547</v>
+        <v>8907</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>8404</v>
+        <v>8764</v>
       </c>
       <c r="B22" t="s">
-        <v>8439</v>
+        <v>8799</v>
       </c>
       <c r="C22" t="s">
-        <v>8486</v>
+        <v>8846</v>
       </c>
       <c r="D22" s="1">
         <v>0.64999997615814209</v>
@@ -26921,21 +28001,21 @@
       </c>
       <c r="G22" s="1"/>
       <c r="H22" t="s">
-        <v>8512</v>
+        <v>8872</v>
       </c>
       <c r="I22" t="s">
-        <v>8548</v>
+        <v>8908</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>8404</v>
+        <v>8764</v>
       </c>
       <c r="B23" t="s">
-        <v>8440</v>
+        <v>8800</v>
       </c>
       <c r="C23" t="s">
-        <v>8486</v>
+        <v>8846</v>
       </c>
       <c r="D23" s="1">
         <v>0.81999999284744263</v>
@@ -26948,21 +28028,21 @@
       </c>
       <c r="G23" s="1"/>
       <c r="H23" t="s">
-        <v>8512</v>
+        <v>8872</v>
       </c>
       <c r="I23" t="s">
-        <v>8549</v>
+        <v>8909</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>8405</v>
+        <v>8765</v>
       </c>
       <c r="B24" t="s">
-        <v>8441</v>
+        <v>8801</v>
       </c>
       <c r="C24" t="s">
-        <v>8486</v>
+        <v>8846</v>
       </c>
       <c r="D24" s="1">
         <v>0.84700000286102295</v>
@@ -26975,21 +28055,21 @@
       </c>
       <c r="G24" s="1"/>
       <c r="H24" t="s">
-        <v>8513</v>
+        <v>8873</v>
       </c>
       <c r="I24" t="s">
-        <v>8550</v>
+        <v>8910</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>8405</v>
+        <v>8765</v>
       </c>
       <c r="B25" t="s">
-        <v>8442</v>
+        <v>8802</v>
       </c>
       <c r="C25" t="s">
-        <v>8486</v>
+        <v>8846</v>
       </c>
       <c r="D25" s="1">
         <v>0.37000000476837158</v>
@@ -27002,21 +28082,21 @@
       </c>
       <c r="G25" s="1"/>
       <c r="H25" t="s">
-        <v>8513</v>
+        <v>8873</v>
       </c>
       <c r="I25" t="s">
-        <v>8551</v>
+        <v>8911</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>8405</v>
+        <v>8765</v>
       </c>
       <c r="B26" t="s">
-        <v>8443</v>
+        <v>8803</v>
       </c>
       <c r="C26" t="s">
-        <v>8486</v>
+        <v>8846</v>
       </c>
       <c r="D26" s="1">
         <v>0.70200002193450928</v>
@@ -27029,21 +28109,21 @@
       </c>
       <c r="G26" s="1"/>
       <c r="H26" t="s">
-        <v>8513</v>
+        <v>8873</v>
       </c>
       <c r="I26" t="s">
-        <v>8552</v>
+        <v>8912</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>8405</v>
+        <v>8765</v>
       </c>
       <c r="B27" t="s">
-        <v>8444</v>
+        <v>8804</v>
       </c>
       <c r="C27" t="s">
-        <v>8487</v>
+        <v>8847</v>
       </c>
       <c r="D27" s="1">
         <v>0.52100002765655518</v>
@@ -27056,21 +28136,21 @@
       </c>
       <c r="G27" s="1"/>
       <c r="H27" t="s">
-        <v>8514</v>
+        <v>8874</v>
       </c>
       <c r="I27" t="s">
-        <v>8553</v>
+        <v>8913</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>8405</v>
+        <v>8765</v>
       </c>
       <c r="B28" t="s">
-        <v>8445</v>
+        <v>8805</v>
       </c>
       <c r="C28" t="s">
-        <v>8487</v>
+        <v>8847</v>
       </c>
       <c r="D28" s="1">
         <v>0.38600000739097595</v>
@@ -27083,21 +28163,21 @@
       </c>
       <c r="G28" s="1"/>
       <c r="H28" t="s">
-        <v>8514</v>
+        <v>8874</v>
       </c>
       <c r="I28" t="s">
-        <v>8554</v>
+        <v>8914</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>8405</v>
+        <v>8765</v>
       </c>
       <c r="B29" t="s">
-        <v>8446</v>
+        <v>8806</v>
       </c>
       <c r="C29" t="s">
-        <v>8487</v>
+        <v>8847</v>
       </c>
       <c r="D29" s="1">
         <v>0.335999995470047</v>
@@ -27110,21 +28190,21 @@
       </c>
       <c r="G29" s="1"/>
       <c r="H29" t="s">
-        <v>8514</v>
+        <v>8874</v>
       </c>
       <c r="I29" t="s">
-        <v>8555</v>
+        <v>8915</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>8406</v>
+        <v>8766</v>
       </c>
       <c r="B30" t="s">
-        <v>8447</v>
+        <v>8807</v>
       </c>
       <c r="C30" t="s">
-        <v>8488</v>
+        <v>8848</v>
       </c>
       <c r="D30" s="1">
         <v>0.74000000953674316</v>
@@ -27137,21 +28217,21 @@
       </c>
       <c r="G30" s="1"/>
       <c r="H30" t="s">
-        <v>8515</v>
+        <v>8875</v>
       </c>
       <c r="I30" t="s">
-        <v>8556</v>
+        <v>8916</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>8406</v>
+        <v>8766</v>
       </c>
       <c r="B31" t="s">
-        <v>8448</v>
+        <v>8808</v>
       </c>
       <c r="C31" t="s">
-        <v>8488</v>
+        <v>8848</v>
       </c>
       <c r="D31" s="1">
         <v>0.75999999046325684</v>
@@ -27164,21 +28244,21 @@
       </c>
       <c r="G31" s="1"/>
       <c r="H31" t="s">
-        <v>8515</v>
+        <v>8875</v>
       </c>
       <c r="I31" t="s">
-        <v>8557</v>
+        <v>8917</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>8407</v>
+        <v>8767</v>
       </c>
       <c r="B32" t="s">
-        <v>8449</v>
+        <v>8809</v>
       </c>
       <c r="C32" t="s">
-        <v>8488</v>
+        <v>8848</v>
       </c>
       <c r="D32" s="1">
         <v>0.75</v>
@@ -27191,21 +28271,21 @@
       </c>
       <c r="G32" s="1"/>
       <c r="H32" t="s">
-        <v>8516</v>
+        <v>8876</v>
       </c>
       <c r="I32" t="s">
-        <v>8558</v>
+        <v>8918</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>8407</v>
+        <v>8767</v>
       </c>
       <c r="B33" t="s">
-        <v>8450</v>
+        <v>8810</v>
       </c>
       <c r="C33" t="s">
-        <v>8488</v>
+        <v>8848</v>
       </c>
       <c r="D33" s="1">
         <v>0.54000002145767212</v>
@@ -27218,21 +28298,21 @@
       </c>
       <c r="G33" s="1"/>
       <c r="H33" t="s">
-        <v>8516</v>
+        <v>8876</v>
       </c>
       <c r="I33" t="s">
-        <v>8559</v>
+        <v>8919</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>8407</v>
+        <v>8767</v>
       </c>
       <c r="B34" t="s">
-        <v>8451</v>
+        <v>8811</v>
       </c>
       <c r="C34" t="s">
-        <v>8489</v>
+        <v>8849</v>
       </c>
       <c r="D34" s="1">
         <v>1.6699999570846558</v>
@@ -27245,21 +28325,21 @@
       </c>
       <c r="G34" s="1"/>
       <c r="H34" t="s">
-        <v>8517</v>
+        <v>8877</v>
       </c>
       <c r="I34" t="s">
-        <v>8560</v>
+        <v>8920</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>8407</v>
+        <v>8767</v>
       </c>
       <c r="B35" t="s">
-        <v>8452</v>
+        <v>8812</v>
       </c>
       <c r="C35" t="s">
-        <v>8489</v>
+        <v>8849</v>
       </c>
       <c r="D35" s="1">
         <v>2.3299999237060547</v>
@@ -27272,21 +28352,21 @@
       </c>
       <c r="G35" s="1"/>
       <c r="H35" t="s">
-        <v>8517</v>
+        <v>8877</v>
       </c>
       <c r="I35" t="s">
-        <v>8561</v>
+        <v>8921</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>8408</v>
+        <v>8768</v>
       </c>
       <c r="B36" t="s">
-        <v>8453</v>
+        <v>8813</v>
       </c>
       <c r="C36" t="s">
-        <v>8490</v>
+        <v>8850</v>
       </c>
       <c r="D36" s="1">
         <v>0.15999999642372131</v>
@@ -27299,21 +28379,21 @@
       </c>
       <c r="G36" s="1"/>
       <c r="H36" t="s">
-        <v>8518</v>
+        <v>8878</v>
       </c>
       <c r="I36" t="s">
-        <v>8562</v>
+        <v>8922</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>8408</v>
+        <v>8768</v>
       </c>
       <c r="B37" t="s">
-        <v>8454</v>
+        <v>8814</v>
       </c>
       <c r="C37" t="s">
-        <v>8490</v>
+        <v>8850</v>
       </c>
       <c r="D37" s="1">
         <v>0.51999998092651367</v>
@@ -27326,21 +28406,21 @@
       </c>
       <c r="G37" s="1"/>
       <c r="H37" t="s">
-        <v>8518</v>
+        <v>8878</v>
       </c>
       <c r="I37" t="s">
-        <v>8563</v>
+        <v>8923</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>8408</v>
+        <v>8768</v>
       </c>
       <c r="B38" t="s">
-        <v>8455</v>
+        <v>8815</v>
       </c>
       <c r="C38" t="s">
-        <v>8490</v>
+        <v>8850</v>
       </c>
       <c r="D38" s="1">
         <v>0.62999999523162842</v>
@@ -27353,21 +28433,21 @@
       </c>
       <c r="G38" s="1"/>
       <c r="H38" t="s">
-        <v>8518</v>
+        <v>8878</v>
       </c>
       <c r="I38" t="s">
-        <v>8564</v>
+        <v>8924</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>8408</v>
+        <v>8768</v>
       </c>
       <c r="B39" t="s">
-        <v>8456</v>
+        <v>8816</v>
       </c>
       <c r="C39" t="s">
-        <v>8490</v>
+        <v>8850</v>
       </c>
       <c r="D39" s="1">
         <v>0.25999999046325684</v>
@@ -27380,21 +28460,21 @@
       </c>
       <c r="G39" s="1"/>
       <c r="H39" t="s">
-        <v>8518</v>
+        <v>8878</v>
       </c>
       <c r="I39" t="s">
-        <v>8565</v>
+        <v>8925</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>8409</v>
+        <v>8769</v>
       </c>
       <c r="B40" t="s">
-        <v>8457</v>
+        <v>8817</v>
       </c>
       <c r="C40" t="s">
-        <v>8490</v>
+        <v>8850</v>
       </c>
       <c r="D40" s="1">
         <v>0.2199999988079071</v>
@@ -27407,21 +28487,21 @@
       </c>
       <c r="G40" s="1"/>
       <c r="H40" t="s">
-        <v>8518</v>
+        <v>8878</v>
       </c>
       <c r="I40" t="s">
-        <v>8566</v>
+        <v>8926</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>8409</v>
+        <v>8769</v>
       </c>
       <c r="B41" t="s">
-        <v>8458</v>
+        <v>8818</v>
       </c>
       <c r="C41" t="s">
-        <v>8490</v>
+        <v>8850</v>
       </c>
       <c r="D41" s="1">
         <v>0.46000000834465027</v>
@@ -27434,21 +28514,21 @@
       </c>
       <c r="G41" s="1"/>
       <c r="H41" t="s">
-        <v>8518</v>
+        <v>8878</v>
       </c>
       <c r="I41" t="s">
-        <v>8567</v>
+        <v>8927</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>8409</v>
+        <v>8769</v>
       </c>
       <c r="B42" t="s">
-        <v>8459</v>
+        <v>8819</v>
       </c>
       <c r="C42" t="s">
-        <v>8490</v>
+        <v>8850</v>
       </c>
       <c r="D42" s="1">
         <v>0.60000002384185791</v>
@@ -27461,21 +28541,21 @@
       </c>
       <c r="G42" s="1"/>
       <c r="H42" t="s">
-        <v>8518</v>
+        <v>8878</v>
       </c>
       <c r="I42" t="s">
-        <v>8568</v>
+        <v>8928</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>8409</v>
+        <v>8769</v>
       </c>
       <c r="B43" t="s">
-        <v>8460</v>
+        <v>8820</v>
       </c>
       <c r="C43" t="s">
-        <v>8490</v>
+        <v>8850</v>
       </c>
       <c r="D43" s="1">
         <v>0.37000000476837158</v>
@@ -27488,21 +28568,21 @@
       </c>
       <c r="G43" s="1"/>
       <c r="H43" t="s">
-        <v>8518</v>
+        <v>8878</v>
       </c>
       <c r="I43" t="s">
-        <v>8569</v>
+        <v>8929</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>8410</v>
+        <v>8770</v>
       </c>
       <c r="B44" t="s">
-        <v>8461</v>
+        <v>8821</v>
       </c>
       <c r="C44" t="s">
-        <v>8490</v>
+        <v>8850</v>
       </c>
       <c r="D44" s="1">
         <v>0.5899999737739563</v>
@@ -27515,21 +28595,21 @@
       </c>
       <c r="G44" s="1"/>
       <c r="H44" t="s">
-        <v>8519</v>
+        <v>8879</v>
       </c>
       <c r="I44" t="s">
-        <v>8570</v>
+        <v>8930</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>8410</v>
+        <v>8770</v>
       </c>
       <c r="B45" t="s">
-        <v>8462</v>
+        <v>8822</v>
       </c>
       <c r="C45" t="s">
-        <v>8490</v>
+        <v>8850</v>
       </c>
       <c r="D45" s="1">
         <v>0.47999998927116394</v>
@@ -27542,21 +28622,21 @@
       </c>
       <c r="G45" s="1"/>
       <c r="H45" t="s">
-        <v>8519</v>
+        <v>8879</v>
       </c>
       <c r="I45" t="s">
-        <v>8571</v>
+        <v>8931</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>8411</v>
+        <v>8771</v>
       </c>
       <c r="B46" t="s">
-        <v>8463</v>
+        <v>8823</v>
       </c>
       <c r="C46" t="s">
-        <v>8491</v>
+        <v>8851</v>
       </c>
       <c r="D46" s="1">
         <v>0.77100002765655518</v>
@@ -27569,21 +28649,21 @@
       </c>
       <c r="G46" s="1"/>
       <c r="H46" t="s">
-        <v>8519</v>
+        <v>8879</v>
       </c>
       <c r="I46" t="s">
-        <v>8572</v>
+        <v>8932</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>8411</v>
+        <v>8771</v>
       </c>
       <c r="B47" t="s">
-        <v>8464</v>
+        <v>8824</v>
       </c>
       <c r="C47" t="s">
-        <v>8491</v>
+        <v>8851</v>
       </c>
       <c r="D47" s="1">
         <v>0.75199997425079346</v>
@@ -27596,21 +28676,21 @@
       </c>
       <c r="G47" s="1"/>
       <c r="H47" t="s">
-        <v>8519</v>
+        <v>8879</v>
       </c>
       <c r="I47" t="s">
-        <v>8573</v>
+        <v>8933</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>8412</v>
+        <v>8772</v>
       </c>
       <c r="B48" t="s">
-        <v>8465</v>
+        <v>8825</v>
       </c>
       <c r="C48" t="s">
-        <v>8492</v>
+        <v>8852</v>
       </c>
       <c r="D48" s="1">
         <v>0.54000002145767212</v>
@@ -27623,21 +28703,21 @@
       </c>
       <c r="G48" s="1"/>
       <c r="H48" t="s">
-        <v>8519</v>
+        <v>8879</v>
       </c>
       <c r="I48" t="s">
-        <v>8574</v>
+        <v>8934</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>8412</v>
+        <v>8772</v>
       </c>
       <c r="B49" t="s">
-        <v>8466</v>
+        <v>8826</v>
       </c>
       <c r="C49" t="s">
-        <v>8492</v>
+        <v>8852</v>
       </c>
       <c r="D49" s="1">
         <v>0.67000001668930054</v>
@@ -27650,21 +28730,21 @@
       </c>
       <c r="G49" s="1"/>
       <c r="H49" t="s">
-        <v>8519</v>
+        <v>8879</v>
       </c>
       <c r="I49" t="s">
-        <v>8575</v>
+        <v>8935</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>8412</v>
+        <v>8772</v>
       </c>
       <c r="B50" t="s">
-        <v>8467</v>
+        <v>8827</v>
       </c>
       <c r="C50" t="s">
-        <v>8492</v>
+        <v>8852</v>
       </c>
       <c r="D50" s="1">
         <v>0.60000002384185791</v>
@@ -27677,21 +28757,21 @@
       </c>
       <c r="G50" s="1"/>
       <c r="H50" t="s">
-        <v>8519</v>
+        <v>8879</v>
       </c>
       <c r="I50" t="s">
-        <v>8576</v>
+        <v>8936</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>8413</v>
+        <v>8773</v>
       </c>
       <c r="B51" t="s">
-        <v>8468</v>
+        <v>8828</v>
       </c>
       <c r="C51" t="s">
-        <v>8493</v>
+        <v>8853</v>
       </c>
       <c r="D51" s="1">
         <v>0.97600001096725464</v>
@@ -27704,21 +28784,21 @@
       </c>
       <c r="G51" s="1"/>
       <c r="H51" t="s">
-        <v>8520</v>
+        <v>8880</v>
       </c>
       <c r="I51" t="s">
-        <v>8577</v>
+        <v>8937</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>8413</v>
+        <v>8773</v>
       </c>
       <c r="B52" t="s">
-        <v>8469</v>
+        <v>8829</v>
       </c>
       <c r="C52" t="s">
-        <v>8493</v>
+        <v>8853</v>
       </c>
       <c r="D52" s="1">
         <v>0.92599999904632568</v>
@@ -27731,21 +28811,21 @@
       </c>
       <c r="G52" s="1"/>
       <c r="H52" t="s">
-        <v>8520</v>
+        <v>8880</v>
       </c>
       <c r="I52" t="s">
-        <v>8578</v>
+        <v>8938</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>8413</v>
+        <v>8773</v>
       </c>
       <c r="B53" t="s">
-        <v>8470</v>
+        <v>8830</v>
       </c>
       <c r="C53" t="s">
-        <v>8493</v>
+        <v>8853</v>
       </c>
       <c r="D53" s="1">
         <v>0.88300001621246338</v>
@@ -27758,21 +28838,21 @@
       </c>
       <c r="G53" s="1"/>
       <c r="H53" t="s">
-        <v>8520</v>
+        <v>8880</v>
       </c>
       <c r="I53" t="s">
-        <v>8579</v>
+        <v>8939</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>8414</v>
+        <v>8774</v>
       </c>
       <c r="B54" t="s">
-        <v>8471</v>
+        <v>8831</v>
       </c>
       <c r="C54" t="s">
-        <v>8494</v>
+        <v>8854</v>
       </c>
       <c r="D54" s="1">
         <v>0.6600000262260437</v>
@@ -27785,21 +28865,21 @@
       </c>
       <c r="G54" s="1"/>
       <c r="H54" t="s">
-        <v>8521</v>
+        <v>8881</v>
       </c>
       <c r="I54" t="s">
-        <v>8580</v>
+        <v>8940</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>8414</v>
+        <v>8774</v>
       </c>
       <c r="B55" t="s">
-        <v>8472</v>
+        <v>8832</v>
       </c>
       <c r="C55" t="s">
-        <v>8494</v>
+        <v>8854</v>
       </c>
       <c r="D55" s="1">
         <v>0.63999998569488525</v>
@@ -27812,21 +28892,21 @@
       </c>
       <c r="G55" s="1"/>
       <c r="H55" t="s">
-        <v>8521</v>
+        <v>8881</v>
       </c>
       <c r="I55" t="s">
-        <v>8581</v>
+        <v>8941</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>8415</v>
+        <v>8775</v>
       </c>
       <c r="B56" t="s">
-        <v>8473</v>
+        <v>8833</v>
       </c>
       <c r="C56" t="s">
-        <v>8495</v>
+        <v>8855</v>
       </c>
       <c r="D56" s="1">
         <v>0.89999997615814209</v>
@@ -27839,21 +28919,21 @@
       </c>
       <c r="G56" s="1"/>
       <c r="H56" t="s">
-        <v>8522</v>
+        <v>8882</v>
       </c>
       <c r="I56" t="s">
-        <v>8582</v>
+        <v>8942</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>8415</v>
+        <v>8775</v>
       </c>
       <c r="B57" t="s">
-        <v>8474</v>
+        <v>8834</v>
       </c>
       <c r="C57" t="s">
-        <v>8495</v>
+        <v>8855</v>
       </c>
       <c r="D57" s="1">
         <v>0.95999997854232788</v>
@@ -27866,21 +28946,21 @@
       </c>
       <c r="G57" s="1"/>
       <c r="H57" t="s">
-        <v>8522</v>
+        <v>8882</v>
       </c>
       <c r="I57" t="s">
-        <v>8583</v>
+        <v>8943</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>8416</v>
+        <v>8776</v>
       </c>
       <c r="B58" t="s">
-        <v>8475</v>
+        <v>8835</v>
       </c>
       <c r="C58" t="s">
-        <v>8496</v>
+        <v>8856</v>
       </c>
       <c r="D58" s="1">
         <v>0.4699999988079071</v>
@@ -27893,21 +28973,21 @@
       </c>
       <c r="G58" s="1"/>
       <c r="H58" t="s">
-        <v>8523</v>
+        <v>8883</v>
       </c>
       <c r="I58" t="s">
-        <v>8584</v>
+        <v>8944</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>8416</v>
+        <v>8776</v>
       </c>
       <c r="B59" t="s">
-        <v>8476</v>
+        <v>8836</v>
       </c>
       <c r="C59" t="s">
-        <v>8496</v>
+        <v>8856</v>
       </c>
       <c r="D59" s="1">
         <v>0.47999998927116394</v>
@@ -27920,21 +29000,21 @@
       </c>
       <c r="G59" s="1"/>
       <c r="H59" t="s">
-        <v>8523</v>
+        <v>8883</v>
       </c>
       <c r="I59" t="s">
-        <v>8585</v>
+        <v>8945</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>8416</v>
+        <v>8776</v>
       </c>
       <c r="B60" t="s">
-        <v>8477</v>
+        <v>8837</v>
       </c>
       <c r="C60" t="s">
-        <v>8497</v>
+        <v>8857</v>
       </c>
       <c r="D60" s="1">
         <v>0.43999999761581421</v>
@@ -27947,21 +29027,21 @@
       </c>
       <c r="G60" s="1"/>
       <c r="H60" t="s">
-        <v>8524</v>
+        <v>8884</v>
       </c>
       <c r="I60" t="s">
-        <v>8586</v>
+        <v>8946</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>8416</v>
+        <v>8776</v>
       </c>
       <c r="B61" t="s">
-        <v>8478</v>
+        <v>8838</v>
       </c>
       <c r="C61" t="s">
-        <v>8497</v>
+        <v>8857</v>
       </c>
       <c r="D61" s="1">
         <v>0.75999999046325684</v>
@@ -27974,21 +29054,21 @@
       </c>
       <c r="G61" s="1"/>
       <c r="H61" t="s">
-        <v>8524</v>
+        <v>8884</v>
       </c>
       <c r="I61" t="s">
-        <v>8587</v>
+        <v>8947</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>8417</v>
+        <v>8777</v>
       </c>
       <c r="B62" t="s">
-        <v>8479</v>
+        <v>8839</v>
       </c>
       <c r="C62" t="s">
-        <v>8497</v>
+        <v>8857</v>
       </c>
       <c r="D62" s="1">
         <v>0.81000000238418579</v>
@@ -28001,21 +29081,21 @@
       </c>
       <c r="G62" s="1"/>
       <c r="H62" t="s">
-        <v>8525</v>
+        <v>8885</v>
       </c>
       <c r="I62" t="s">
-        <v>8588</v>
+        <v>8948</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>8417</v>
+        <v>8777</v>
       </c>
       <c r="B63" t="s">
-        <v>8480</v>
+        <v>8840</v>
       </c>
       <c r="C63" t="s">
-        <v>8497</v>
+        <v>8857</v>
       </c>
       <c r="D63" s="1">
         <v>0.79000002145767212</v>
@@ -28028,21 +29108,21 @@
       </c>
       <c r="G63" s="1"/>
       <c r="H63" t="s">
-        <v>8525</v>
+        <v>8885</v>
       </c>
       <c r="I63" t="s">
-        <v>8589</v>
+        <v>8949</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>8418</v>
+        <v>8778</v>
       </c>
       <c r="B64" t="s">
-        <v>8481</v>
+        <v>8841</v>
       </c>
       <c r="C64" t="s">
-        <v>8498</v>
+        <v>8858</v>
       </c>
       <c r="D64" s="1">
         <v>0.6600000262260437</v>
@@ -28055,21 +29135,21 @@
       </c>
       <c r="G64" s="1"/>
       <c r="H64" t="s">
-        <v>8526</v>
+        <v>8886</v>
       </c>
       <c r="I64" t="s">
-        <v>8590</v>
+        <v>8950</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>8418</v>
+        <v>8778</v>
       </c>
       <c r="B65" t="s">
-        <v>8482</v>
+        <v>8842</v>
       </c>
       <c r="C65" t="s">
-        <v>8498</v>
+        <v>8858</v>
       </c>
       <c r="D65" s="1">
         <v>0.55000001192092896</v>
@@ -28082,10 +29162,10 @@
       </c>
       <c r="G65" s="1"/>
       <c r="H65" t="s">
-        <v>8526</v>
+        <v>8886</v>
       </c>
       <c r="I65" t="s">
-        <v>8591</v>
+        <v>8951</v>
       </c>
     </row>
   </sheetData>
@@ -28099,42 +29179,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>8592</v>
+        <v>8952</v>
       </c>
       <c r="B1" t="s">
-        <v>8614</v>
+        <v>8974</v>
       </c>
       <c r="C1" t="s">
-        <v>8661</v>
+        <v>9021</v>
       </c>
       <c r="D1" t="s">
-        <v>8671</v>
+        <v>9031</v>
       </c>
       <c r="E1" t="s">
-        <v>8672</v>
+        <v>9032</v>
       </c>
       <c r="F1" t="s">
-        <v>8673</v>
+        <v>9033</v>
       </c>
       <c r="G1" t="s">
-        <v>8674</v>
+        <v>9034</v>
       </c>
       <c r="H1" t="s">
-        <v>8686</v>
+        <v>9046</v>
       </c>
       <c r="I1" t="s">
-        <v>8707</v>
+        <v>9067</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>8593</v>
+        <v>8953</v>
       </c>
       <c r="B2" t="s">
-        <v>8615</v>
+        <v>8975</v>
       </c>
       <c r="C2" t="s">
-        <v>8662</v>
+        <v>9022</v>
       </c>
       <c r="D2" s="1">
         <v>0.5899999737739563</v>
@@ -28146,24 +29226,24 @@
         <v>0.81999999284744263</v>
       </c>
       <c r="G2" t="s">
-        <v>8675</v>
+        <v>9035</v>
       </c>
       <c r="H2" t="s">
-        <v>8687</v>
+        <v>9047</v>
       </c>
       <c r="I2" t="s">
-        <v>8708</v>
+        <v>9068</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8593</v>
+        <v>8953</v>
       </c>
       <c r="B3" t="s">
-        <v>8616</v>
+        <v>8976</v>
       </c>
       <c r="C3" t="s">
-        <v>8662</v>
+        <v>9022</v>
       </c>
       <c r="D3" s="1">
         <v>0.18000000715255737</v>
@@ -28175,24 +29255,24 @@
         <v>1.4900000095367432</v>
       </c>
       <c r="G3" t="s">
-        <v>8675</v>
+        <v>9035</v>
       </c>
       <c r="H3" t="s">
-        <v>8687</v>
+        <v>9047</v>
       </c>
       <c r="I3" t="s">
-        <v>8709</v>
+        <v>9069</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>8594</v>
+        <v>8954</v>
       </c>
       <c r="B4" t="s">
-        <v>8617</v>
+        <v>8977</v>
       </c>
       <c r="C4" t="s">
-        <v>8662</v>
+        <v>9022</v>
       </c>
       <c r="D4" s="1">
         <v>0.37999999523162842</v>
@@ -28204,24 +29284,24 @@
         <v>0.6600000262260437</v>
       </c>
       <c r="G4" t="s">
-        <v>8675</v>
+        <v>9035</v>
       </c>
       <c r="H4" t="s">
-        <v>8688</v>
+        <v>9048</v>
       </c>
       <c r="I4" t="s">
-        <v>8710</v>
+        <v>9070</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8594</v>
+        <v>8954</v>
       </c>
       <c r="B5" t="s">
-        <v>8618</v>
+        <v>8978</v>
       </c>
       <c r="C5" t="s">
-        <v>8662</v>
+        <v>9022</v>
       </c>
       <c r="D5" s="1">
         <v>0.44999998807907104</v>
@@ -28233,24 +29313,24 @@
         <v>0.57999998331069946</v>
       </c>
       <c r="G5" t="s">
-        <v>8675</v>
+        <v>9035</v>
       </c>
       <c r="H5" t="s">
-        <v>8688</v>
+        <v>9048</v>
       </c>
       <c r="I5" t="s">
-        <v>8711</v>
+        <v>9071</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8595</v>
+        <v>8955</v>
       </c>
       <c r="B6" t="s">
-        <v>8619</v>
+        <v>8979</v>
       </c>
       <c r="C6" t="s">
-        <v>8662</v>
+        <v>9022</v>
       </c>
       <c r="D6" s="1">
         <v>0.75700002908706665</v>
@@ -28262,24 +29342,24 @@
         <v>0.96299999952316284</v>
       </c>
       <c r="G6" t="s">
-        <v>8676</v>
+        <v>9036</v>
       </c>
       <c r="H6" t="s">
-        <v>8689</v>
+        <v>9049</v>
       </c>
       <c r="I6" t="s">
-        <v>8712</v>
+        <v>9072</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>8595</v>
+        <v>8955</v>
       </c>
       <c r="B7" t="s">
-        <v>8620</v>
+        <v>8980</v>
       </c>
       <c r="C7" t="s">
-        <v>8662</v>
+        <v>9022</v>
       </c>
       <c r="D7" s="1">
         <v>0.92599999904632568</v>
@@ -28291,24 +29371,24 @@
         <v>1.2790000438690186</v>
       </c>
       <c r="G7" t="s">
-        <v>8677</v>
+        <v>9037</v>
       </c>
       <c r="H7" t="s">
-        <v>8689</v>
+        <v>9049</v>
       </c>
       <c r="I7" t="s">
-        <v>8713</v>
+        <v>9073</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>8596</v>
+        <v>8956</v>
       </c>
       <c r="B8" t="s">
-        <v>8621</v>
+        <v>8981</v>
       </c>
       <c r="C8" t="s">
-        <v>8662</v>
+        <v>9022</v>
       </c>
       <c r="D8" s="1">
         <v>0.43999999761581421</v>
@@ -28320,24 +29400,24 @@
         <v>0.56000000238418579</v>
       </c>
       <c r="G8" t="s">
-        <v>8678</v>
+        <v>9038</v>
       </c>
       <c r="H8" t="s">
-        <v>8690</v>
+        <v>9050</v>
       </c>
       <c r="I8" t="s">
-        <v>8714</v>
+        <v>9074</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8596</v>
+        <v>8956</v>
       </c>
       <c r="B9" t="s">
-        <v>8622</v>
+        <v>8982</v>
       </c>
       <c r="C9" t="s">
-        <v>8662</v>
+        <v>9022</v>
       </c>
       <c r="D9" s="1">
         <v>0.80000001192092896</v>
@@ -28349,24 +29429,24 @@
         <v>1.1100000143051147</v>
       </c>
       <c r="G9" t="s">
-        <v>8678</v>
+        <v>9038</v>
       </c>
       <c r="H9" t="s">
-        <v>8690</v>
+        <v>9050</v>
       </c>
       <c r="I9" t="s">
-        <v>8715</v>
+        <v>9075</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>8597</v>
+        <v>8957</v>
       </c>
       <c r="B10" t="s">
-        <v>8623</v>
+        <v>8983</v>
       </c>
       <c r="C10" t="s">
-        <v>8662</v>
+        <v>9022</v>
       </c>
       <c r="D10" s="1">
         <v>0.56000000238418579</v>
@@ -28378,24 +29458,24 @@
         <v>0.97000002861022949</v>
       </c>
       <c r="G10" t="s">
-        <v>8678</v>
+        <v>9038</v>
       </c>
       <c r="H10" t="s">
-        <v>8691</v>
+        <v>9051</v>
       </c>
       <c r="I10" t="s">
-        <v>8716</v>
+        <v>9076</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>8597</v>
+        <v>8957</v>
       </c>
       <c r="B11" t="s">
-        <v>8624</v>
+        <v>8984</v>
       </c>
       <c r="C11" t="s">
-        <v>8662</v>
+        <v>9022</v>
       </c>
       <c r="D11" s="1">
         <v>0.50999999046325684</v>
@@ -28407,24 +29487,24 @@
         <v>1.190000057220459</v>
       </c>
       <c r="G11" t="s">
-        <v>8678</v>
+        <v>9038</v>
       </c>
       <c r="H11" t="s">
-        <v>8691</v>
+        <v>9051</v>
       </c>
       <c r="I11" t="s">
-        <v>8717</v>
+        <v>9077</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>8598</v>
+        <v>8958</v>
       </c>
       <c r="B12" t="s">
-        <v>8625</v>
+        <v>8985</v>
       </c>
       <c r="C12" t="s">
-        <v>8662</v>
+        <v>9022</v>
       </c>
       <c r="D12" s="1">
         <v>0.36000001430511475</v>
@@ -28436,24 +29516,24 @@
         <v>0.82999998331069946</v>
       </c>
       <c r="G12" t="s">
-        <v>8678</v>
+        <v>9038</v>
       </c>
       <c r="H12" t="s">
-        <v>8692</v>
+        <v>9052</v>
       </c>
       <c r="I12" t="s">
-        <v>8718</v>
+        <v>9078</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>8598</v>
+        <v>8958</v>
       </c>
       <c r="B13" t="s">
-        <v>8626</v>
+        <v>8986</v>
       </c>
       <c r="C13" t="s">
-        <v>8662</v>
+        <v>9022</v>
       </c>
       <c r="D13" s="1">
         <v>0.6600000262260437</v>
@@ -28465,24 +29545,24 @@
         <v>0.89999997615814209</v>
       </c>
       <c r="G13" t="s">
-        <v>8678</v>
+        <v>9038</v>
       </c>
       <c r="H13" t="s">
-        <v>8692</v>
+        <v>9052</v>
       </c>
       <c r="I13" t="s">
-        <v>8719</v>
+        <v>9079</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>8599</v>
+        <v>8959</v>
       </c>
       <c r="B14" t="s">
-        <v>8627</v>
+        <v>8987</v>
       </c>
       <c r="C14" t="s">
-        <v>8662</v>
+        <v>9022</v>
       </c>
       <c r="D14" s="1">
         <v>0.55299997329711914</v>
@@ -28494,24 +29574,24 @@
         <v>0.9309999942779541</v>
       </c>
       <c r="G14" t="s">
-        <v>8679</v>
+        <v>9039</v>
       </c>
       <c r="H14" t="s">
-        <v>8693</v>
+        <v>9053</v>
       </c>
       <c r="I14" t="s">
-        <v>8720</v>
+        <v>9080</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>8599</v>
+        <v>8959</v>
       </c>
       <c r="B15" t="s">
-        <v>8628</v>
+        <v>8988</v>
       </c>
       <c r="C15" t="s">
-        <v>8662</v>
+        <v>9022</v>
       </c>
       <c r="D15" s="1">
         <v>0.76599997282028198</v>
@@ -28523,24 +29603,24 @@
         <v>3.9639999866485596</v>
       </c>
       <c r="G15" t="s">
-        <v>8679</v>
+        <v>9039</v>
       </c>
       <c r="H15" t="s">
-        <v>8693</v>
+        <v>9053</v>
       </c>
       <c r="I15" t="s">
-        <v>8721</v>
+        <v>9081</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>8599</v>
+        <v>8959</v>
       </c>
       <c r="B16" t="s">
-        <v>8629</v>
+        <v>8989</v>
       </c>
       <c r="C16" t="s">
-        <v>8663</v>
+        <v>9023</v>
       </c>
       <c r="D16" s="1">
         <v>0.39800000190734863</v>
@@ -28552,24 +29632,24 @@
         <v>0.71899998188018799</v>
       </c>
       <c r="G16" t="s">
-        <v>8679</v>
+        <v>9039</v>
       </c>
       <c r="H16" t="s">
-        <v>8694</v>
+        <v>9054</v>
       </c>
       <c r="I16" t="s">
-        <v>8722</v>
+        <v>9082</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>8599</v>
+        <v>8959</v>
       </c>
       <c r="B17" t="s">
-        <v>8630</v>
+        <v>8990</v>
       </c>
       <c r="C17" t="s">
-        <v>8663</v>
+        <v>9023</v>
       </c>
       <c r="D17" s="1">
         <v>0.49799999594688416</v>
@@ -28581,24 +29661,24 @@
         <v>2.4030001163482666</v>
       </c>
       <c r="G17" t="s">
-        <v>8679</v>
+        <v>9039</v>
       </c>
       <c r="H17" t="s">
-        <v>8694</v>
+        <v>9054</v>
       </c>
       <c r="I17" t="s">
-        <v>8723</v>
+        <v>9083</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>8600</v>
+        <v>8960</v>
       </c>
       <c r="B18" t="s">
-        <v>8631</v>
+        <v>8991</v>
       </c>
       <c r="C18" t="s">
-        <v>8664</v>
+        <v>9024</v>
       </c>
       <c r="D18" s="1">
         <v>0.87000000476837158</v>
@@ -28610,24 +29690,24 @@
         <v>1.2899999618530273</v>
       </c>
       <c r="G18" t="s">
-        <v>8680</v>
+        <v>9040</v>
       </c>
       <c r="H18" t="s">
-        <v>8695</v>
+        <v>9055</v>
       </c>
       <c r="I18" t="s">
-        <v>8724</v>
+        <v>9084</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>8600</v>
+        <v>8960</v>
       </c>
       <c r="B19" t="s">
-        <v>8632</v>
+        <v>8992</v>
       </c>
       <c r="C19" t="s">
-        <v>8664</v>
+        <v>9024</v>
       </c>
       <c r="D19" s="1">
         <v>0.38999998569488525</v>
@@ -28639,24 +29719,24 @@
         <v>0.80000001192092896</v>
       </c>
       <c r="G19" t="s">
-        <v>8680</v>
+        <v>9040</v>
       </c>
       <c r="H19" t="s">
-        <v>8695</v>
+        <v>9055</v>
       </c>
       <c r="I19" t="s">
-        <v>8725</v>
+        <v>9085</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>8601</v>
+        <v>8961</v>
       </c>
       <c r="B20" t="s">
-        <v>8633</v>
+        <v>8993</v>
       </c>
       <c r="C20" t="s">
-        <v>8664</v>
+        <v>9024</v>
       </c>
       <c r="D20" s="1">
         <v>0.61000001430511475</v>
@@ -28668,24 +29748,24 @@
         <v>1.1699999570846558</v>
       </c>
       <c r="G20" t="s">
-        <v>8680</v>
+        <v>9040</v>
       </c>
       <c r="H20" t="s">
-        <v>8696</v>
+        <v>9056</v>
       </c>
       <c r="I20" t="s">
-        <v>8726</v>
+        <v>9086</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>8601</v>
+        <v>8961</v>
       </c>
       <c r="B21" t="s">
-        <v>8634</v>
+        <v>8994</v>
       </c>
       <c r="C21" t="s">
-        <v>8664</v>
+        <v>9024</v>
       </c>
       <c r="D21" s="1">
         <v>0.75</v>
@@ -28697,24 +29777,24 @@
         <v>1.3600000143051147</v>
       </c>
       <c r="G21" t="s">
-        <v>8680</v>
+        <v>9040</v>
       </c>
       <c r="H21" t="s">
-        <v>8696</v>
+        <v>9056</v>
       </c>
       <c r="I21" t="s">
-        <v>8727</v>
+        <v>9087</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>8601</v>
+        <v>8961</v>
       </c>
       <c r="B22" t="s">
-        <v>8635</v>
+        <v>8995</v>
       </c>
       <c r="C22" t="s">
-        <v>8665</v>
+        <v>9025</v>
       </c>
       <c r="D22" s="1">
         <v>5.9000000953674316</v>
@@ -28726,24 +29806,24 @@
         <v>46.099998474121094</v>
       </c>
       <c r="G22" t="s">
-        <v>8680</v>
+        <v>9040</v>
       </c>
       <c r="H22" t="s">
-        <v>8697</v>
+        <v>9057</v>
       </c>
       <c r="I22" t="s">
-        <v>8728</v>
+        <v>9088</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>8601</v>
+        <v>8961</v>
       </c>
       <c r="B23" t="s">
-        <v>8636</v>
+        <v>8996</v>
       </c>
       <c r="C23" t="s">
-        <v>8665</v>
+        <v>9025</v>
       </c>
       <c r="D23" s="1">
         <v>1.8200000524520874</v>
@@ -28755,24 +29835,24 @@
         <v>5.1399998664855957</v>
       </c>
       <c r="G23" t="s">
-        <v>8680</v>
+        <v>9040</v>
       </c>
       <c r="H23" t="s">
-        <v>8697</v>
+        <v>9057</v>
       </c>
       <c r="I23" t="s">
-        <v>8729</v>
+        <v>9089</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>8602</v>
+        <v>8962</v>
       </c>
       <c r="B24" t="s">
-        <v>8637</v>
+        <v>8997</v>
       </c>
       <c r="C24" t="s">
-        <v>8666</v>
+        <v>9026</v>
       </c>
       <c r="D24" s="1">
         <v>0.5899999737739563</v>
@@ -28784,24 +29864,24 @@
         <v>1.3999999761581421</v>
       </c>
       <c r="G24" t="s">
-        <v>8680</v>
+        <v>9040</v>
       </c>
       <c r="H24" t="s">
-        <v>8698</v>
+        <v>9058</v>
       </c>
       <c r="I24" t="s">
-        <v>8730</v>
+        <v>9090</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>8602</v>
+        <v>8962</v>
       </c>
       <c r="B25" t="s">
-        <v>8638</v>
+        <v>8998</v>
       </c>
       <c r="C25" t="s">
-        <v>8666</v>
+        <v>9026</v>
       </c>
       <c r="D25" s="1">
         <v>0.69999998807907104</v>
@@ -28813,24 +29893,24 @@
         <v>0.87000000476837158</v>
       </c>
       <c r="G25" t="s">
-        <v>8680</v>
+        <v>9040</v>
       </c>
       <c r="H25" t="s">
-        <v>8698</v>
+        <v>9058</v>
       </c>
       <c r="I25" t="s">
-        <v>8731</v>
+        <v>9091</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>8603</v>
+        <v>8963</v>
       </c>
       <c r="B26" t="s">
-        <v>8639</v>
+        <v>8999</v>
       </c>
       <c r="C26" t="s">
-        <v>8666</v>
+        <v>9026</v>
       </c>
       <c r="D26" s="1">
         <v>0.38999998569488525</v>
@@ -28842,24 +29922,24 @@
         <v>0.68999999761581421</v>
       </c>
       <c r="G26" t="s">
-        <v>8680</v>
+        <v>9040</v>
       </c>
       <c r="H26" t="s">
-        <v>8699</v>
+        <v>9059</v>
       </c>
       <c r="I26" t="s">
-        <v>8732</v>
+        <v>9092</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>8603</v>
+        <v>8963</v>
       </c>
       <c r="B27" t="s">
-        <v>8640</v>
+        <v>9000</v>
       </c>
       <c r="C27" t="s">
-        <v>8666</v>
+        <v>9026</v>
       </c>
       <c r="D27" s="1">
         <v>0.15999999642372131</v>
@@ -28871,24 +29951,24 @@
         <v>0.40000000596046448</v>
       </c>
       <c r="G27" t="s">
-        <v>8680</v>
+        <v>9040</v>
       </c>
       <c r="H27" t="s">
-        <v>8699</v>
+        <v>9059</v>
       </c>
       <c r="I27" t="s">
-        <v>8733</v>
+        <v>9093</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>8604</v>
+        <v>8964</v>
       </c>
       <c r="B28" t="s">
-        <v>8641</v>
+        <v>9001</v>
       </c>
       <c r="C28" t="s">
-        <v>8666</v>
+        <v>9026</v>
       </c>
       <c r="D28" s="1">
         <v>0.46000000834465027</v>
@@ -28900,24 +29980,24 @@
         <v>0.6600000262260437</v>
       </c>
       <c r="G28" t="s">
-        <v>8680</v>
+        <v>9040</v>
       </c>
       <c r="H28" t="s">
-        <v>8699</v>
+        <v>9059</v>
       </c>
       <c r="I28" t="s">
-        <v>8734</v>
+        <v>9094</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>8604</v>
+        <v>8964</v>
       </c>
       <c r="B29" t="s">
-        <v>8642</v>
+        <v>9002</v>
       </c>
       <c r="C29" t="s">
-        <v>8666</v>
+        <v>9026</v>
       </c>
       <c r="D29" s="1">
         <v>0.30000001192092896</v>
@@ -28929,24 +30009,24 @@
         <v>0.44999998807907104</v>
       </c>
       <c r="G29" t="s">
-        <v>8680</v>
+        <v>9040</v>
       </c>
       <c r="H29" t="s">
-        <v>8699</v>
+        <v>9059</v>
       </c>
       <c r="I29" t="s">
-        <v>8735</v>
+        <v>9095</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>8605</v>
+        <v>8965</v>
       </c>
       <c r="B30" t="s">
-        <v>8643</v>
+        <v>9003</v>
       </c>
       <c r="C30" t="s">
-        <v>8666</v>
+        <v>9026</v>
       </c>
       <c r="D30" s="1">
         <v>0.5</v>
@@ -28958,24 +30038,24 @@
         <v>1.059999942779541</v>
       </c>
       <c r="G30" t="s">
-        <v>8680</v>
+        <v>9040</v>
       </c>
       <c r="H30" t="s">
-        <v>8700</v>
+        <v>9060</v>
       </c>
       <c r="I30" t="s">
-        <v>8736</v>
+        <v>9096</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>8605</v>
+        <v>8965</v>
       </c>
       <c r="B31" t="s">
-        <v>8644</v>
+        <v>9004</v>
       </c>
       <c r="C31" t="s">
-        <v>8666</v>
+        <v>9026</v>
       </c>
       <c r="D31" s="1">
         <v>0.47999998927116394</v>
@@ -28987,24 +30067,24 @@
         <v>0.76999998092651367</v>
       </c>
       <c r="G31" t="s">
-        <v>8680</v>
+        <v>9040</v>
       </c>
       <c r="H31" t="s">
-        <v>8700</v>
+        <v>9060</v>
       </c>
       <c r="I31" t="s">
-        <v>8737</v>
+        <v>9097</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>8606</v>
+        <v>8966</v>
       </c>
       <c r="B32" t="s">
-        <v>8645</v>
+        <v>9005</v>
       </c>
       <c r="C32" t="s">
-        <v>8666</v>
+        <v>9026</v>
       </c>
       <c r="D32" s="1">
         <v>1.6200000047683716</v>
@@ -29016,24 +30096,24 @@
         <v>2.4100000858306885</v>
       </c>
       <c r="G32" t="s">
-        <v>8680</v>
+        <v>9040</v>
       </c>
       <c r="H32" t="s">
-        <v>8700</v>
+        <v>9060</v>
       </c>
       <c r="I32" t="s">
-        <v>8738</v>
+        <v>9098</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>8606</v>
+        <v>8966</v>
       </c>
       <c r="B33" t="s">
-        <v>8646</v>
+        <v>9006</v>
       </c>
       <c r="C33" t="s">
-        <v>8666</v>
+        <v>9026</v>
       </c>
       <c r="D33" s="1">
         <v>2.0099999904632568</v>
@@ -29045,24 +30125,24 @@
         <v>2.8399999141693115</v>
       </c>
       <c r="G33" t="s">
-        <v>8680</v>
+        <v>9040</v>
       </c>
       <c r="H33" t="s">
-        <v>8700</v>
+        <v>9060</v>
       </c>
       <c r="I33" t="s">
-        <v>8739</v>
+        <v>9099</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>8607</v>
+        <v>8967</v>
       </c>
       <c r="B34" t="s">
-        <v>8647</v>
+        <v>9007</v>
       </c>
       <c r="C34" t="s">
-        <v>8667</v>
+        <v>9027</v>
       </c>
       <c r="D34" s="1">
         <v>0.95999997854232788</v>
@@ -29074,24 +30154,24 @@
         <v>1.2560000419616699</v>
       </c>
       <c r="G34" t="s">
-        <v>8681</v>
+        <v>9041</v>
       </c>
       <c r="H34" t="s">
-        <v>8701</v>
+        <v>9061</v>
       </c>
       <c r="I34" t="s">
-        <v>8740</v>
+        <v>9100</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>8607</v>
+        <v>8967</v>
       </c>
       <c r="B35" t="s">
-        <v>8648</v>
+        <v>9008</v>
       </c>
       <c r="C35" t="s">
-        <v>8667</v>
+        <v>9027</v>
       </c>
       <c r="D35" s="1">
         <v>1.0800000429153442</v>
@@ -29103,24 +30183,24 @@
         <v>1.3609999418258667</v>
       </c>
       <c r="G35" t="s">
-        <v>8681</v>
+        <v>9041</v>
       </c>
       <c r="H35" t="s">
-        <v>8701</v>
+        <v>9061</v>
       </c>
       <c r="I35" t="s">
-        <v>8741</v>
+        <v>9101</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>8608</v>
+        <v>8968</v>
       </c>
       <c r="B36" t="s">
-        <v>8649</v>
+        <v>9009</v>
       </c>
       <c r="C36" t="s">
-        <v>8667</v>
+        <v>9027</v>
       </c>
       <c r="D36" s="1">
         <v>0.87699997425079346</v>
@@ -29132,24 +30212,24 @@
         <v>1.156000018119812</v>
       </c>
       <c r="G36" t="s">
-        <v>8682</v>
+        <v>9042</v>
       </c>
       <c r="H36" t="s">
-        <v>8702</v>
+        <v>9062</v>
       </c>
       <c r="I36" t="s">
-        <v>8742</v>
+        <v>9102</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>8608</v>
+        <v>8968</v>
       </c>
       <c r="B37" t="s">
-        <v>8650</v>
+        <v>9010</v>
       </c>
       <c r="C37" t="s">
-        <v>8667</v>
+        <v>9027</v>
       </c>
       <c r="D37" s="1">
         <v>0.68400001525878906</v>
@@ -29161,24 +30241,24 @@
         <v>0.875</v>
       </c>
       <c r="G37" t="s">
-        <v>8682</v>
+        <v>9042</v>
       </c>
       <c r="H37" t="s">
-        <v>8702</v>
+        <v>9062</v>
       </c>
       <c r="I37" t="s">
-        <v>8743</v>
+        <v>9103</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>8608</v>
+        <v>8968</v>
       </c>
       <c r="B38" t="s">
-        <v>8651</v>
+        <v>9011</v>
       </c>
       <c r="C38" t="s">
-        <v>8667</v>
+        <v>9027</v>
       </c>
       <c r="D38" s="1">
         <v>0.85699999332427979</v>
@@ -29190,24 +30270,24 @@
         <v>1.1779999732971191</v>
       </c>
       <c r="G38" t="s">
-        <v>8682</v>
+        <v>9042</v>
       </c>
       <c r="H38" t="s">
-        <v>8702</v>
+        <v>9062</v>
       </c>
       <c r="I38" t="s">
-        <v>8744</v>
+        <v>9104</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>8609</v>
+        <v>8969</v>
       </c>
       <c r="B39" t="s">
-        <v>8651</v>
+        <v>9011</v>
       </c>
       <c r="C39" t="s">
-        <v>8668</v>
+        <v>9028</v>
       </c>
       <c r="D39" s="1">
         <v>0.64999997615814209</v>
@@ -29219,24 +30299,24 @@
         <v>0.8399999737739563</v>
       </c>
       <c r="G39" t="s">
-        <v>8683</v>
+        <v>9043</v>
       </c>
       <c r="H39" t="s">
-        <v>8702</v>
+        <v>9062</v>
       </c>
       <c r="I39" t="s">
-        <v>8745</v>
+        <v>9105</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>8609</v>
+        <v>8969</v>
       </c>
       <c r="B40" t="s">
-        <v>8652</v>
+        <v>9012</v>
       </c>
       <c r="C40" t="s">
-        <v>8668</v>
+        <v>9028</v>
       </c>
       <c r="D40" s="1">
         <v>0.47999998927116394</v>
@@ -29248,24 +30328,24 @@
         <v>0.75</v>
       </c>
       <c r="G40" t="s">
-        <v>8683</v>
+        <v>9043</v>
       </c>
       <c r="H40" t="s">
-        <v>8702</v>
+        <v>9062</v>
       </c>
       <c r="I40" t="s">
-        <v>8746</v>
+        <v>9106</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>8610</v>
+        <v>8970</v>
       </c>
       <c r="B41" t="s">
-        <v>8653</v>
+        <v>9013</v>
       </c>
       <c r="C41" t="s">
-        <v>8669</v>
+        <v>9029</v>
       </c>
       <c r="D41" s="1">
         <v>0.78100001811981201</v>
@@ -29277,24 +30357,24 @@
         <v>1.3220000267028809</v>
       </c>
       <c r="G41" t="s">
-        <v>8684</v>
+        <v>9044</v>
       </c>
       <c r="H41" t="s">
-        <v>8703</v>
+        <v>9063</v>
       </c>
       <c r="I41" t="s">
-        <v>8747</v>
+        <v>9107</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>8610</v>
+        <v>8970</v>
       </c>
       <c r="B42" t="s">
-        <v>8654</v>
+        <v>9014</v>
       </c>
       <c r="C42" t="s">
-        <v>8669</v>
+        <v>9029</v>
       </c>
       <c r="D42" s="1">
         <v>0.97500002384185791</v>
@@ -29306,24 +30386,24 @@
         <v>1.1829999685287476</v>
       </c>
       <c r="G42" t="s">
-        <v>8684</v>
+        <v>9044</v>
       </c>
       <c r="H42" t="s">
-        <v>8703</v>
+        <v>9063</v>
       </c>
       <c r="I42" t="s">
-        <v>8748</v>
+        <v>9108</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>8611</v>
+        <v>8971</v>
       </c>
       <c r="B43" t="s">
-        <v>8655</v>
+        <v>9015</v>
       </c>
       <c r="C43" t="s">
-        <v>8669</v>
+        <v>9029</v>
       </c>
       <c r="D43" s="1">
         <v>0.93000000715255737</v>
@@ -29335,24 +30415,24 @@
         <v>1.309999942779541</v>
       </c>
       <c r="G43" t="s">
-        <v>8685</v>
+        <v>9045</v>
       </c>
       <c r="H43" t="s">
-        <v>8704</v>
+        <v>9064</v>
       </c>
       <c r="I43" t="s">
-        <v>8749</v>
+        <v>9109</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>8611</v>
+        <v>8971</v>
       </c>
       <c r="B44" t="s">
-        <v>8656</v>
+        <v>9016</v>
       </c>
       <c r="C44" t="s">
-        <v>8669</v>
+        <v>9029</v>
       </c>
       <c r="D44" s="1">
         <v>0.93999999761581421</v>
@@ -29364,24 +30444,24 @@
         <v>1.190000057220459</v>
       </c>
       <c r="G44" t="s">
-        <v>8685</v>
+        <v>9045</v>
       </c>
       <c r="H44" t="s">
-        <v>8704</v>
+        <v>9064</v>
       </c>
       <c r="I44" t="s">
-        <v>8750</v>
+        <v>9110</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>8612</v>
+        <v>8972</v>
       </c>
       <c r="B45" t="s">
-        <v>8657</v>
+        <v>9017</v>
       </c>
       <c r="C45" t="s">
-        <v>8670</v>
+        <v>9030</v>
       </c>
       <c r="D45" s="1">
         <v>0.63999998569488525</v>
@@ -29393,24 +30473,24 @@
         <v>0.9100000262260437</v>
       </c>
       <c r="G45" t="s">
-        <v>8685</v>
+        <v>9045</v>
       </c>
       <c r="H45" t="s">
-        <v>8705</v>
+        <v>9065</v>
       </c>
       <c r="I45" t="s">
-        <v>8751</v>
+        <v>9111</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>8612</v>
+        <v>8972</v>
       </c>
       <c r="B46" t="s">
-        <v>8658</v>
+        <v>9018</v>
       </c>
       <c r="C46" t="s">
-        <v>8670</v>
+        <v>9030</v>
       </c>
       <c r="D46" s="1">
         <v>0.72000002861022949</v>
@@ -29422,24 +30502,24 @@
         <v>0.89999997615814209</v>
       </c>
       <c r="G46" t="s">
-        <v>8685</v>
+        <v>9045</v>
       </c>
       <c r="H46" t="s">
-        <v>8705</v>
+        <v>9065</v>
       </c>
       <c r="I46" t="s">
-        <v>8752</v>
+        <v>9112</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>8613</v>
+        <v>8973</v>
       </c>
       <c r="B47" t="s">
-        <v>8659</v>
+        <v>9019</v>
       </c>
       <c r="C47" t="s">
-        <v>8670</v>
+        <v>9030</v>
       </c>
       <c r="D47" s="1">
         <v>0.46000000834465027</v>
@@ -29451,24 +30531,24 @@
         <v>0.73000001907348633</v>
       </c>
       <c r="G47" t="s">
-        <v>8685</v>
+        <v>9045</v>
       </c>
       <c r="H47" t="s">
-        <v>8706</v>
+        <v>9066</v>
       </c>
       <c r="I47" t="s">
-        <v>8753</v>
+        <v>9113</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>8613</v>
+        <v>8973</v>
       </c>
       <c r="B48" t="s">
-        <v>8660</v>
+        <v>9020</v>
       </c>
       <c r="C48" t="s">
-        <v>8670</v>
+        <v>9030</v>
       </c>
       <c r="D48" s="1">
         <v>0.62999999523162842</v>
@@ -29480,13 +30560,13 @@
         <v>0.89999997615814209</v>
       </c>
       <c r="G48" t="s">
-        <v>8685</v>
+        <v>9045</v>
       </c>
       <c r="H48" t="s">
-        <v>8706</v>
+        <v>9066</v>
       </c>
       <c r="I48" t="s">
-        <v>8754</v>
+        <v>9114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct data for San-Miguel 2016 (PANORAMA 1)
</commit_message>
<xml_diff>
--- a/products/Exported Data.xlsx
+++ b/products/Exported Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63975" uniqueCount="37488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64595" uniqueCount="37848">
   <si>
     <t>Study</t>
   </si>
@@ -101537,6 +101537,1086 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Study: Treatment 1 vs Treatment 2</t>
+  </si>
+  <si>
+    <t>Attal 2019 (ICARIA-MM): IsPd vs Pd</t>
+  </si>
+  <si>
+    <t>Bahlis 2020 (POLLUX): DRd vs Rd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2013 (VANTAGE 088): VorV vs V</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2016 (ENDEAVOR): Kd vs Vd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2018 (ELOQUENT-3): EPd vs Pd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2018 (ELOQUENT-2): ELd vs Ld</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2020 (ELOQUENT-2): ELd vs Ld</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2021 (APOLLO): DPd vs Pd</t>
+  </si>
+  <si>
+    <t>Grosicki 2020 (BOSTON): SeVd vs Vd</t>
+  </si>
+  <si>
+    <t>Hou 2017 (China Cont.): IRd vs Rd</t>
+  </si>
+  <si>
+    <t>Jakubowiak 2016 (NCT01478048): EVd vs Vd</t>
+  </si>
+  <si>
+    <t>Kumar 2020 (BELLINI): VeVd vs Vd</t>
+  </si>
+  <si>
+    <t>Lu 2021 (LEPUS): DVd vs Vd</t>
+  </si>
+  <si>
+    <t>Mateos 2020 (CASTOR): DVd vs Vd</t>
+  </si>
+  <si>
+    <t>Moreau 2021 (IKEMA): IsKd vs Kd</t>
+  </si>
+  <si>
+    <t>Orlowski 2019 (ENDEAVOR): Kd vs Vd</t>
+  </si>
+  <si>
+    <t>Richardson 2019 (OPTIMISMM): PVd vs Vd</t>
+  </si>
+  <si>
+    <t>Richardson 2021 (TOURMALINE-MM1): IRd vs Rd</t>
+  </si>
+  <si>
+    <t>San-Miguel 2014 (PANORAMA-1): FVd vs Vd</t>
+  </si>
+  <si>
+    <t>San-Miguel 2016 (PANORAMA 1): FVd vs Vd</t>
+  </si>
+  <si>
+    <t>San-Miguel 2013 (MM-003): Pd vs GC</t>
+  </si>
+  <si>
+    <t>Siegel 2018 (ASPIRE): KRd vs Rd</t>
+  </si>
+  <si>
+    <t>Usamani 2022 (CANDOR): DKd vs Kd</t>
+  </si>
+  <si>
+    <t>lot</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>&gt;3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>&gt;3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>&gt;=4</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>&gt;=4</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>&gt;3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>&gt;3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>&gt;1</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>&gt;2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>&gt;=3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>&gt;2</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>&gt;2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>&gt;=2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>Outcome</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Lower 95% CI Bound on HR</t>
+  </si>
+  <si>
+    <t>Upper 95% CI Bound on HR</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t>Tab. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tab. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      p. 808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. S3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. S4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      AT 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      p. 730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t>Data Extraction Errors</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Study: Treatment 1 vs Treatment 2</t>
+  </si>
+  <si>
+    <t>Attal 2019 (ICARIA-MM): IsPd vs Pd</t>
+  </si>
+  <si>
+    <t>Bahlis 2020 (POLLUX): DRd vs Rd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2013 (VANTAGE 088): VorV vs V</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2016 (ENDEAVOR): Kd vs Vd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2018 (ELOQUENT-3): EPd vs Pd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2021 (APOLLO): DPd vs Pd</t>
+  </si>
+  <si>
+    <t>Hou 2017 (China Cont.): IRd vs Rd</t>
+  </si>
+  <si>
+    <t>Jakubowiak 2016 (NCT01478048): EVd vs Vd</t>
+  </si>
+  <si>
+    <t>Kumar 2020 (BELLINI): VeVd vs Vd</t>
+  </si>
+  <si>
+    <t>Lonial 2015 (ELOQUENT-2): ELd vs Ld</t>
+  </si>
+  <si>
+    <t>Lu 2021 (LEPUS): DVd vs Vd</t>
+  </si>
+  <si>
+    <t>Mateos 2020 (CASTOR): DVd vs Vd</t>
+  </si>
+  <si>
+    <t>Moreau 2021 (IKEMA): IsKd vs Kd</t>
+  </si>
+  <si>
+    <t>Orlowski 2007 (NCT00103506): V vs DoxV</t>
+  </si>
+  <si>
+    <t>Orlowski 2016 (NCT00103506): V vs DoxV</t>
+  </si>
+  <si>
+    <t>Orlowski 2019 (ENDEAVOR): Kd vs Vd</t>
+  </si>
+  <si>
+    <t>Richardson 2019 (OPTIMISMM): PVd vs Vd</t>
+  </si>
+  <si>
+    <t>Richardson 2021 (TOURMALINE-MM1): IRd vs Rd</t>
+  </si>
+  <si>
+    <t>San-Miguel 2016 (PANORAMA 1): FVd vs Vd</t>
+  </si>
+  <si>
+    <t>Stewart 2015 (ASPIRE): KRd vs Rd</t>
+  </si>
+  <si>
+    <t>Usmani 2022 (CANDOR): DKd vs Kd</t>
+  </si>
+  <si>
+    <t>refract</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Previous R use</t>
+  </si>
+  <si>
+    <t>No previous R use</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No IMiD use</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Ref. to R and a PI</t>
+  </si>
+  <si>
+    <t>Not ref. to R and a PI</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No IMiD use</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No IMiD use</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No IMiD use</t>
+  </si>
+  <si>
+    <t>Naive</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Naive</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Previous R use</t>
+  </si>
+  <si>
+    <t>No previous R use</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Not refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Not refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Previous R or T use</t>
+  </si>
+  <si>
+    <t>No previous R or T use</t>
+  </si>
+  <si>
+    <t>Previous R or T use</t>
+  </si>
+  <si>
+    <t>No previous R or T use</t>
+  </si>
+  <si>
+    <t>Previous R use</t>
+  </si>
+  <si>
+    <t>No previous R use</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Refractory to T</t>
+  </si>
+  <si>
+    <t>Not refractory to T</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No previous IMiD use</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Not refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Outcome</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Lower 95% CI Bound on HR</t>
+  </si>
+  <si>
+    <t>Upper 95% CI Bound on HR</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0230</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .       Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tab. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      p. 808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. S3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. S4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t>Data Extraction Errors</t>
   </si>
   <si>
     <t/>
@@ -112528,42 +113608,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>37128</v>
+        <v>37488</v>
       </c>
       <c r="B1" t="s">
-        <v>37152</v>
+        <v>37512</v>
       </c>
       <c r="C1" t="s">
-        <v>37216</v>
+        <v>37576</v>
       </c>
       <c r="D1" t="s">
-        <v>37232</v>
+        <v>37592</v>
       </c>
       <c r="E1" t="s">
-        <v>37233</v>
+        <v>37593</v>
       </c>
       <c r="F1" t="s">
-        <v>37234</v>
+        <v>37594</v>
       </c>
       <c r="G1" t="s">
-        <v>37235</v>
+        <v>37595</v>
       </c>
       <c r="H1" t="s">
-        <v>37236</v>
+        <v>37596</v>
       </c>
       <c r="I1" t="s">
-        <v>37260</v>
+        <v>37620</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>37129</v>
+        <v>37489</v>
       </c>
       <c r="B2" t="s">
-        <v>37153</v>
+        <v>37513</v>
       </c>
       <c r="C2" t="s">
-        <v>37217</v>
+        <v>37577</v>
       </c>
       <c r="D2" s="1">
         <v>0.5899999737739563</v>
@@ -112576,21 +113656,21 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" t="s">
-        <v>37237</v>
+        <v>37597</v>
       </c>
       <c r="I2" t="s">
-        <v>37261</v>
+        <v>37621</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>37129</v>
+        <v>37489</v>
       </c>
       <c r="B3" t="s">
-        <v>37154</v>
+        <v>37514</v>
       </c>
       <c r="C3" t="s">
-        <v>37217</v>
+        <v>37577</v>
       </c>
       <c r="D3" s="1">
         <v>0.5899999737739563</v>
@@ -112603,21 +113683,21 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" t="s">
-        <v>37237</v>
+        <v>37597</v>
       </c>
       <c r="I3" t="s">
-        <v>37262</v>
+        <v>37622</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>37130</v>
+        <v>37490</v>
       </c>
       <c r="B4" t="s">
-        <v>37155</v>
+        <v>37515</v>
       </c>
       <c r="C4" t="s">
-        <v>37217</v>
+        <v>37577</v>
       </c>
       <c r="D4" s="1">
         <v>0.41999998688697815</v>
@@ -112630,21 +113710,21 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" t="s">
-        <v>37238</v>
+        <v>37598</v>
       </c>
       <c r="I4" t="s">
-        <v>37263</v>
+        <v>37623</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>37130</v>
+        <v>37490</v>
       </c>
       <c r="B5" t="s">
-        <v>37156</v>
+        <v>37516</v>
       </c>
       <c r="C5" t="s">
-        <v>37217</v>
+        <v>37577</v>
       </c>
       <c r="D5" s="1">
         <v>0.38999998569488525</v>
@@ -112657,21 +113737,21 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" t="s">
-        <v>37238</v>
+        <v>37598</v>
       </c>
       <c r="I5" t="s">
-        <v>37264</v>
+        <v>37624</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>37130</v>
+        <v>37490</v>
       </c>
       <c r="B6" t="s">
-        <v>37157</v>
+        <v>37517</v>
       </c>
       <c r="C6" t="s">
-        <v>37217</v>
+        <v>37577</v>
       </c>
       <c r="D6" s="1">
         <v>0.47999998927116394</v>
@@ -112684,21 +113764,21 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" t="s">
-        <v>37238</v>
+        <v>37598</v>
       </c>
       <c r="I6" t="s">
-        <v>37265</v>
+        <v>37625</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>37130</v>
+        <v>37490</v>
       </c>
       <c r="B7" t="s">
-        <v>37158</v>
+        <v>37518</v>
       </c>
       <c r="C7" t="s">
-        <v>37217</v>
+        <v>37577</v>
       </c>
       <c r="D7" s="1">
         <v>0.74000000953674316</v>
@@ -112711,21 +113791,21 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" t="s">
-        <v>37238</v>
+        <v>37598</v>
       </c>
       <c r="I7" t="s">
-        <v>37266</v>
+        <v>37626</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>37131</v>
+        <v>37491</v>
       </c>
       <c r="B8" t="s">
-        <v>37159</v>
+        <v>37519</v>
       </c>
       <c r="C8" t="s">
-        <v>37217</v>
+        <v>37577</v>
       </c>
       <c r="D8" s="1">
         <v>0.68699997663497925</v>
@@ -112740,21 +113820,21 @@
         <v>0.015200000256299973</v>
       </c>
       <c r="H8" t="s">
-        <v>37239</v>
+        <v>37599</v>
       </c>
       <c r="I8" t="s">
-        <v>37267</v>
+        <v>37627</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>37131</v>
+        <v>37491</v>
       </c>
       <c r="B9" t="s">
-        <v>37160</v>
+        <v>37520</v>
       </c>
       <c r="C9" t="s">
-        <v>37217</v>
+        <v>37577</v>
       </c>
       <c r="D9" s="1">
         <v>0.91600000858306885</v>
@@ -112769,21 +113849,21 @@
         <v>0.48710000514984131</v>
       </c>
       <c r="H9" t="s">
-        <v>37240</v>
+        <v>37600</v>
       </c>
       <c r="I9" t="s">
-        <v>37268</v>
+        <v>37628</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>37132</v>
+        <v>37492</v>
       </c>
       <c r="B10" t="s">
-        <v>37161</v>
+        <v>37521</v>
       </c>
       <c r="C10" t="s">
-        <v>37217</v>
+        <v>37577</v>
       </c>
       <c r="D10" s="1">
         <v>0.44999998807907104</v>
@@ -112796,21 +113876,21 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" t="s">
-        <v>37241</v>
+        <v>37601</v>
       </c>
       <c r="I10" t="s">
-        <v>37269</v>
+        <v>37629</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>37132</v>
+        <v>37492</v>
       </c>
       <c r="B11" t="s">
-        <v>37162</v>
+        <v>37522</v>
       </c>
       <c r="C11" t="s">
-        <v>37217</v>
+        <v>37577</v>
       </c>
       <c r="D11" s="1">
         <v>0.60000002384185791</v>
@@ -112823,21 +113903,21 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" t="s">
-        <v>37241</v>
+        <v>37601</v>
       </c>
       <c r="I11" t="s">
-        <v>37270</v>
+        <v>37630</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>37133</v>
+        <v>37493</v>
       </c>
       <c r="B12" t="s">
-        <v>37162</v>
+        <v>37522</v>
       </c>
       <c r="C12" t="s">
-        <v>37217</v>
+        <v>37577</v>
       </c>
       <c r="D12" s="1">
         <v>0.55000001192092896</v>
@@ -112850,21 +113930,21 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" t="s">
-        <v>37242</v>
+        <v>37602</v>
       </c>
       <c r="I12" t="s">
-        <v>37271</v>
+        <v>37631</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>37133</v>
+        <v>37493</v>
       </c>
       <c r="B13" t="s">
-        <v>37163</v>
+        <v>37523</v>
       </c>
       <c r="C13" t="s">
-        <v>37217</v>
+        <v>37577</v>
       </c>
       <c r="D13" s="1">
         <v>0.50999999046325684</v>
@@ -112877,21 +113957,21 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" t="s">
-        <v>37242</v>
+        <v>37602</v>
       </c>
       <c r="I13" t="s">
-        <v>37272</v>
+        <v>37632</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>37134</v>
+        <v>37494</v>
       </c>
       <c r="B14" t="s">
-        <v>37164</v>
+        <v>37524</v>
       </c>
       <c r="C14" t="s">
-        <v>37217</v>
+        <v>37577</v>
       </c>
       <c r="D14" s="1">
         <v>0.76999998092651367</v>
@@ -112904,21 +113984,21 @@
       </c>
       <c r="G14" s="1"/>
       <c r="H14" t="s">
-        <v>37243</v>
+        <v>37603</v>
       </c>
       <c r="I14" t="s">
-        <v>37273</v>
+        <v>37633</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>37134</v>
+        <v>37494</v>
       </c>
       <c r="B15" t="s">
-        <v>37165</v>
+        <v>37525</v>
       </c>
       <c r="C15" t="s">
-        <v>37217</v>
+        <v>37577</v>
       </c>
       <c r="D15" s="1">
         <v>0.68000000715255737</v>
@@ -112931,21 +114011,21 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15" t="s">
-        <v>37243</v>
+        <v>37603</v>
       </c>
       <c r="I15" t="s">
-        <v>37274</v>
+        <v>37634</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>37135</v>
+        <v>37495</v>
       </c>
       <c r="B16" t="s">
-        <v>37166</v>
+        <v>37526</v>
       </c>
       <c r="C16" t="s">
-        <v>37218</v>
+        <v>37578</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
@@ -112958,21 +114038,21 @@
       </c>
       <c r="G16" s="1"/>
       <c r="H16" t="s">
-        <v>37243</v>
+        <v>37603</v>
       </c>
       <c r="I16" t="s">
-        <v>37275</v>
+        <v>37635</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>37135</v>
+        <v>37495</v>
       </c>
       <c r="B17" t="s">
-        <v>37167</v>
+        <v>37527</v>
       </c>
       <c r="C17" t="s">
-        <v>37218</v>
+        <v>37578</v>
       </c>
       <c r="D17" s="1">
         <v>0.70999997854232788</v>
@@ -112985,21 +114065,21 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" t="s">
-        <v>37243</v>
+        <v>37603</v>
       </c>
       <c r="I17" t="s">
-        <v>37276</v>
+        <v>37636</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>37136</v>
+        <v>37496</v>
       </c>
       <c r="B18" t="s">
-        <v>37168</v>
+        <v>37528</v>
       </c>
       <c r="C18" t="s">
-        <v>37219</v>
+        <v>37579</v>
       </c>
       <c r="D18" s="1">
         <v>0.69999998807907104</v>
@@ -113012,21 +114092,21 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" t="s">
-        <v>37244</v>
+        <v>37604</v>
       </c>
       <c r="I18" t="s">
-        <v>37277</v>
+        <v>37637</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>37136</v>
+        <v>37496</v>
       </c>
       <c r="B19" t="s">
-        <v>37169</v>
+        <v>37529</v>
       </c>
       <c r="C19" t="s">
-        <v>37219</v>
+        <v>37579</v>
       </c>
       <c r="D19" s="1">
         <v>0.6600000262260437</v>
@@ -113039,21 +114119,21 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19" t="s">
-        <v>37244</v>
+        <v>37604</v>
       </c>
       <c r="I19" t="s">
-        <v>37278</v>
+        <v>37638</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>37136</v>
+        <v>37496</v>
       </c>
       <c r="B20" t="s">
-        <v>37170</v>
+        <v>37530</v>
       </c>
       <c r="C20" t="s">
-        <v>37219</v>
+        <v>37579</v>
       </c>
       <c r="D20" s="1">
         <v>0.40000000596046448</v>
@@ -113066,21 +114146,21 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" t="s">
-        <v>37244</v>
+        <v>37604</v>
       </c>
       <c r="I20" t="s">
-        <v>37279</v>
+        <v>37639</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>37137</v>
+        <v>37497</v>
       </c>
       <c r="B21" t="s">
-        <v>37171</v>
+        <v>37531</v>
       </c>
       <c r="C21" t="s">
-        <v>37219</v>
+        <v>37579</v>
       </c>
       <c r="D21" s="1">
         <v>0.62999999523162842</v>
@@ -113093,21 +114173,21 @@
       </c>
       <c r="G21" s="1"/>
       <c r="H21" t="s">
-        <v>37245</v>
+        <v>37605</v>
       </c>
       <c r="I21" t="s">
-        <v>37280</v>
+        <v>37640</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>37137</v>
+        <v>37497</v>
       </c>
       <c r="B22" t="s">
-        <v>37172</v>
+        <v>37532</v>
       </c>
       <c r="C22" t="s">
-        <v>37219</v>
+        <v>37579</v>
       </c>
       <c r="D22" s="1">
         <v>0.64999997615814209</v>
@@ -113120,21 +114200,21 @@
       </c>
       <c r="G22" s="1"/>
       <c r="H22" t="s">
-        <v>37245</v>
+        <v>37605</v>
       </c>
       <c r="I22" t="s">
-        <v>37281</v>
+        <v>37641</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>37137</v>
+        <v>37497</v>
       </c>
       <c r="B23" t="s">
-        <v>37173</v>
+        <v>37533</v>
       </c>
       <c r="C23" t="s">
-        <v>37219</v>
+        <v>37579</v>
       </c>
       <c r="D23" s="1">
         <v>0.81999999284744263</v>
@@ -113147,21 +114227,21 @@
       </c>
       <c r="G23" s="1"/>
       <c r="H23" t="s">
-        <v>37245</v>
+        <v>37605</v>
       </c>
       <c r="I23" t="s">
-        <v>37282</v>
+        <v>37642</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>37138</v>
+        <v>37498</v>
       </c>
       <c r="B24" t="s">
-        <v>37174</v>
+        <v>37534</v>
       </c>
       <c r="C24" t="s">
-        <v>37219</v>
+        <v>37579</v>
       </c>
       <c r="D24" s="1">
         <v>0.84700000286102295</v>
@@ -113174,21 +114254,21 @@
       </c>
       <c r="G24" s="1"/>
       <c r="H24" t="s">
-        <v>37246</v>
+        <v>37606</v>
       </c>
       <c r="I24" t="s">
-        <v>37283</v>
+        <v>37643</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>37138</v>
+        <v>37498</v>
       </c>
       <c r="B25" t="s">
-        <v>37175</v>
+        <v>37535</v>
       </c>
       <c r="C25" t="s">
-        <v>37219</v>
+        <v>37579</v>
       </c>
       <c r="D25" s="1">
         <v>0.37000000476837158</v>
@@ -113201,21 +114281,21 @@
       </c>
       <c r="G25" s="1"/>
       <c r="H25" t="s">
-        <v>37246</v>
+        <v>37606</v>
       </c>
       <c r="I25" t="s">
-        <v>37284</v>
+        <v>37644</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>37138</v>
+        <v>37498</v>
       </c>
       <c r="B26" t="s">
-        <v>37176</v>
+        <v>37536</v>
       </c>
       <c r="C26" t="s">
-        <v>37219</v>
+        <v>37579</v>
       </c>
       <c r="D26" s="1">
         <v>0.70200002193450928</v>
@@ -113228,21 +114308,21 @@
       </c>
       <c r="G26" s="1"/>
       <c r="H26" t="s">
-        <v>37246</v>
+        <v>37606</v>
       </c>
       <c r="I26" t="s">
-        <v>37285</v>
+        <v>37645</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>37138</v>
+        <v>37498</v>
       </c>
       <c r="B27" t="s">
-        <v>37177</v>
+        <v>37537</v>
       </c>
       <c r="C27" t="s">
-        <v>37220</v>
+        <v>37580</v>
       </c>
       <c r="D27" s="1">
         <v>0.52100002765655518</v>
@@ -113255,21 +114335,21 @@
       </c>
       <c r="G27" s="1"/>
       <c r="H27" t="s">
-        <v>37247</v>
+        <v>37607</v>
       </c>
       <c r="I27" t="s">
-        <v>37286</v>
+        <v>37646</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>37138</v>
+        <v>37498</v>
       </c>
       <c r="B28" t="s">
-        <v>37178</v>
+        <v>37538</v>
       </c>
       <c r="C28" t="s">
-        <v>37220</v>
+        <v>37580</v>
       </c>
       <c r="D28" s="1">
         <v>0.38600000739097595</v>
@@ -113282,21 +114362,21 @@
       </c>
       <c r="G28" s="1"/>
       <c r="H28" t="s">
-        <v>37247</v>
+        <v>37607</v>
       </c>
       <c r="I28" t="s">
-        <v>37287</v>
+        <v>37647</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>37138</v>
+        <v>37498</v>
       </c>
       <c r="B29" t="s">
-        <v>37179</v>
+        <v>37539</v>
       </c>
       <c r="C29" t="s">
-        <v>37220</v>
+        <v>37580</v>
       </c>
       <c r="D29" s="1">
         <v>0.335999995470047</v>
@@ -113309,21 +114389,21 @@
       </c>
       <c r="G29" s="1"/>
       <c r="H29" t="s">
-        <v>37247</v>
+        <v>37607</v>
       </c>
       <c r="I29" t="s">
-        <v>37288</v>
+        <v>37648</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>37139</v>
+        <v>37499</v>
       </c>
       <c r="B30" t="s">
-        <v>37180</v>
+        <v>37540</v>
       </c>
       <c r="C30" t="s">
-        <v>37221</v>
+        <v>37581</v>
       </c>
       <c r="D30" s="1">
         <v>0.74000000953674316</v>
@@ -113336,21 +114416,21 @@
       </c>
       <c r="G30" s="1"/>
       <c r="H30" t="s">
-        <v>37248</v>
+        <v>37608</v>
       </c>
       <c r="I30" t="s">
-        <v>37289</v>
+        <v>37649</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>37139</v>
+        <v>37499</v>
       </c>
       <c r="B31" t="s">
-        <v>37181</v>
+        <v>37541</v>
       </c>
       <c r="C31" t="s">
-        <v>37221</v>
+        <v>37581</v>
       </c>
       <c r="D31" s="1">
         <v>0.75999999046325684</v>
@@ -113363,21 +114443,21 @@
       </c>
       <c r="G31" s="1"/>
       <c r="H31" t="s">
-        <v>37248</v>
+        <v>37608</v>
       </c>
       <c r="I31" t="s">
-        <v>37290</v>
+        <v>37650</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>37140</v>
+        <v>37500</v>
       </c>
       <c r="B32" t="s">
-        <v>37182</v>
+        <v>37542</v>
       </c>
       <c r="C32" t="s">
-        <v>37221</v>
+        <v>37581</v>
       </c>
       <c r="D32" s="1">
         <v>0.75</v>
@@ -113390,21 +114470,21 @@
       </c>
       <c r="G32" s="1"/>
       <c r="H32" t="s">
-        <v>37249</v>
+        <v>37609</v>
       </c>
       <c r="I32" t="s">
-        <v>37291</v>
+        <v>37651</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>37140</v>
+        <v>37500</v>
       </c>
       <c r="B33" t="s">
-        <v>37183</v>
+        <v>37543</v>
       </c>
       <c r="C33" t="s">
-        <v>37221</v>
+        <v>37581</v>
       </c>
       <c r="D33" s="1">
         <v>0.54000002145767212</v>
@@ -113417,21 +114497,21 @@
       </c>
       <c r="G33" s="1"/>
       <c r="H33" t="s">
-        <v>37249</v>
+        <v>37609</v>
       </c>
       <c r="I33" t="s">
-        <v>37292</v>
+        <v>37652</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>37140</v>
+        <v>37500</v>
       </c>
       <c r="B34" t="s">
-        <v>37184</v>
+        <v>37544</v>
       </c>
       <c r="C34" t="s">
-        <v>37222</v>
+        <v>37582</v>
       </c>
       <c r="D34" s="1">
         <v>1.6699999570846558</v>
@@ -113444,21 +114524,21 @@
       </c>
       <c r="G34" s="1"/>
       <c r="H34" t="s">
-        <v>37250</v>
+        <v>37610</v>
       </c>
       <c r="I34" t="s">
-        <v>37293</v>
+        <v>37653</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>37140</v>
+        <v>37500</v>
       </c>
       <c r="B35" t="s">
-        <v>37185</v>
+        <v>37545</v>
       </c>
       <c r="C35" t="s">
-        <v>37222</v>
+        <v>37582</v>
       </c>
       <c r="D35" s="1">
         <v>2.3299999237060547</v>
@@ -113471,21 +114551,21 @@
       </c>
       <c r="G35" s="1"/>
       <c r="H35" t="s">
-        <v>37250</v>
+        <v>37610</v>
       </c>
       <c r="I35" t="s">
-        <v>37294</v>
+        <v>37654</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>37141</v>
+        <v>37501</v>
       </c>
       <c r="B36" t="s">
-        <v>37186</v>
+        <v>37546</v>
       </c>
       <c r="C36" t="s">
-        <v>37223</v>
+        <v>37583</v>
       </c>
       <c r="D36" s="1">
         <v>0.15999999642372131</v>
@@ -113498,21 +114578,21 @@
       </c>
       <c r="G36" s="1"/>
       <c r="H36" t="s">
-        <v>37251</v>
+        <v>37611</v>
       </c>
       <c r="I36" t="s">
-        <v>37295</v>
+        <v>37655</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>37141</v>
+        <v>37501</v>
       </c>
       <c r="B37" t="s">
-        <v>37187</v>
+        <v>37547</v>
       </c>
       <c r="C37" t="s">
-        <v>37223</v>
+        <v>37583</v>
       </c>
       <c r="D37" s="1">
         <v>0.51999998092651367</v>
@@ -113525,21 +114605,21 @@
       </c>
       <c r="G37" s="1"/>
       <c r="H37" t="s">
-        <v>37251</v>
+        <v>37611</v>
       </c>
       <c r="I37" t="s">
-        <v>37296</v>
+        <v>37656</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>37141</v>
+        <v>37501</v>
       </c>
       <c r="B38" t="s">
-        <v>37188</v>
+        <v>37548</v>
       </c>
       <c r="C38" t="s">
-        <v>37223</v>
+        <v>37583</v>
       </c>
       <c r="D38" s="1">
         <v>0.62999999523162842</v>
@@ -113552,21 +114632,21 @@
       </c>
       <c r="G38" s="1"/>
       <c r="H38" t="s">
-        <v>37251</v>
+        <v>37611</v>
       </c>
       <c r="I38" t="s">
-        <v>37297</v>
+        <v>37657</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>37141</v>
+        <v>37501</v>
       </c>
       <c r="B39" t="s">
-        <v>37189</v>
+        <v>37549</v>
       </c>
       <c r="C39" t="s">
-        <v>37223</v>
+        <v>37583</v>
       </c>
       <c r="D39" s="1">
         <v>0.25999999046325684</v>
@@ -113579,21 +114659,21 @@
       </c>
       <c r="G39" s="1"/>
       <c r="H39" t="s">
-        <v>37251</v>
+        <v>37611</v>
       </c>
       <c r="I39" t="s">
-        <v>37298</v>
+        <v>37658</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>37142</v>
+        <v>37502</v>
       </c>
       <c r="B40" t="s">
-        <v>37190</v>
+        <v>37550</v>
       </c>
       <c r="C40" t="s">
-        <v>37223</v>
+        <v>37583</v>
       </c>
       <c r="D40" s="1">
         <v>0.2199999988079071</v>
@@ -113606,21 +114686,21 @@
       </c>
       <c r="G40" s="1"/>
       <c r="H40" t="s">
-        <v>37251</v>
+        <v>37611</v>
       </c>
       <c r="I40" t="s">
-        <v>37299</v>
+        <v>37659</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>37142</v>
+        <v>37502</v>
       </c>
       <c r="B41" t="s">
-        <v>37191</v>
+        <v>37551</v>
       </c>
       <c r="C41" t="s">
-        <v>37223</v>
+        <v>37583</v>
       </c>
       <c r="D41" s="1">
         <v>0.46000000834465027</v>
@@ -113633,21 +114713,21 @@
       </c>
       <c r="G41" s="1"/>
       <c r="H41" t="s">
-        <v>37251</v>
+        <v>37611</v>
       </c>
       <c r="I41" t="s">
-        <v>37300</v>
+        <v>37660</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>37142</v>
+        <v>37502</v>
       </c>
       <c r="B42" t="s">
-        <v>37192</v>
+        <v>37552</v>
       </c>
       <c r="C42" t="s">
-        <v>37223</v>
+        <v>37583</v>
       </c>
       <c r="D42" s="1">
         <v>0.60000002384185791</v>
@@ -113660,21 +114740,21 @@
       </c>
       <c r="G42" s="1"/>
       <c r="H42" t="s">
-        <v>37251</v>
+        <v>37611</v>
       </c>
       <c r="I42" t="s">
-        <v>37301</v>
+        <v>37661</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>37142</v>
+        <v>37502</v>
       </c>
       <c r="B43" t="s">
-        <v>37193</v>
+        <v>37553</v>
       </c>
       <c r="C43" t="s">
-        <v>37223</v>
+        <v>37583</v>
       </c>
       <c r="D43" s="1">
         <v>0.37000000476837158</v>
@@ -113687,21 +114767,21 @@
       </c>
       <c r="G43" s="1"/>
       <c r="H43" t="s">
-        <v>37251</v>
+        <v>37611</v>
       </c>
       <c r="I43" t="s">
-        <v>37302</v>
+        <v>37662</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>37143</v>
+        <v>37503</v>
       </c>
       <c r="B44" t="s">
-        <v>37194</v>
+        <v>37554</v>
       </c>
       <c r="C44" t="s">
-        <v>37223</v>
+        <v>37583</v>
       </c>
       <c r="D44" s="1">
         <v>0.5899999737739563</v>
@@ -113714,21 +114794,21 @@
       </c>
       <c r="G44" s="1"/>
       <c r="H44" t="s">
-        <v>37252</v>
+        <v>37612</v>
       </c>
       <c r="I44" t="s">
-        <v>37303</v>
+        <v>37663</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>37143</v>
+        <v>37503</v>
       </c>
       <c r="B45" t="s">
-        <v>37195</v>
+        <v>37555</v>
       </c>
       <c r="C45" t="s">
-        <v>37223</v>
+        <v>37583</v>
       </c>
       <c r="D45" s="1">
         <v>0.47999998927116394</v>
@@ -113741,21 +114821,21 @@
       </c>
       <c r="G45" s="1"/>
       <c r="H45" t="s">
-        <v>37252</v>
+        <v>37612</v>
       </c>
       <c r="I45" t="s">
-        <v>37304</v>
+        <v>37664</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>37144</v>
+        <v>37504</v>
       </c>
       <c r="B46" t="s">
-        <v>37196</v>
+        <v>37556</v>
       </c>
       <c r="C46" t="s">
-        <v>37224</v>
+        <v>37584</v>
       </c>
       <c r="D46" s="1">
         <v>0.77100002765655518</v>
@@ -113768,21 +114848,21 @@
       </c>
       <c r="G46" s="1"/>
       <c r="H46" t="s">
-        <v>37252</v>
+        <v>37612</v>
       </c>
       <c r="I46" t="s">
-        <v>37305</v>
+        <v>37665</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>37144</v>
+        <v>37504</v>
       </c>
       <c r="B47" t="s">
-        <v>37197</v>
+        <v>37557</v>
       </c>
       <c r="C47" t="s">
-        <v>37224</v>
+        <v>37584</v>
       </c>
       <c r="D47" s="1">
         <v>0.75199997425079346</v>
@@ -113795,21 +114875,21 @@
       </c>
       <c r="G47" s="1"/>
       <c r="H47" t="s">
-        <v>37252</v>
+        <v>37612</v>
       </c>
       <c r="I47" t="s">
-        <v>37306</v>
+        <v>37666</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>37145</v>
+        <v>37505</v>
       </c>
       <c r="B48" t="s">
-        <v>37198</v>
+        <v>37558</v>
       </c>
       <c r="C48" t="s">
-        <v>37225</v>
+        <v>37585</v>
       </c>
       <c r="D48" s="1">
         <v>0.54000002145767212</v>
@@ -113822,21 +114902,21 @@
       </c>
       <c r="G48" s="1"/>
       <c r="H48" t="s">
-        <v>37252</v>
+        <v>37612</v>
       </c>
       <c r="I48" t="s">
-        <v>37307</v>
+        <v>37667</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>37145</v>
+        <v>37505</v>
       </c>
       <c r="B49" t="s">
-        <v>37199</v>
+        <v>37559</v>
       </c>
       <c r="C49" t="s">
-        <v>37225</v>
+        <v>37585</v>
       </c>
       <c r="D49" s="1">
         <v>0.67000001668930054</v>
@@ -113849,21 +114929,21 @@
       </c>
       <c r="G49" s="1"/>
       <c r="H49" t="s">
-        <v>37252</v>
+        <v>37612</v>
       </c>
       <c r="I49" t="s">
-        <v>37308</v>
+        <v>37668</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>37145</v>
+        <v>37505</v>
       </c>
       <c r="B50" t="s">
-        <v>37200</v>
+        <v>37560</v>
       </c>
       <c r="C50" t="s">
-        <v>37225</v>
+        <v>37585</v>
       </c>
       <c r="D50" s="1">
         <v>0.60000002384185791</v>
@@ -113876,21 +114956,21 @@
       </c>
       <c r="G50" s="1"/>
       <c r="H50" t="s">
-        <v>37252</v>
+        <v>37612</v>
       </c>
       <c r="I50" t="s">
-        <v>37309</v>
+        <v>37669</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>37146</v>
+        <v>37506</v>
       </c>
       <c r="B51" t="s">
-        <v>37201</v>
+        <v>37561</v>
       </c>
       <c r="C51" t="s">
-        <v>37226</v>
+        <v>37586</v>
       </c>
       <c r="D51" s="1">
         <v>0.97600001096725464</v>
@@ -113903,21 +114983,21 @@
       </c>
       <c r="G51" s="1"/>
       <c r="H51" t="s">
-        <v>37253</v>
+        <v>37613</v>
       </c>
       <c r="I51" t="s">
-        <v>37310</v>
+        <v>37670</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>37146</v>
+        <v>37506</v>
       </c>
       <c r="B52" t="s">
-        <v>37202</v>
+        <v>37562</v>
       </c>
       <c r="C52" t="s">
-        <v>37226</v>
+        <v>37586</v>
       </c>
       <c r="D52" s="1">
         <v>0.92599999904632568</v>
@@ -113930,21 +115010,21 @@
       </c>
       <c r="G52" s="1"/>
       <c r="H52" t="s">
-        <v>37253</v>
+        <v>37613</v>
       </c>
       <c r="I52" t="s">
-        <v>37311</v>
+        <v>37671</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>37146</v>
+        <v>37506</v>
       </c>
       <c r="B53" t="s">
-        <v>37203</v>
+        <v>37563</v>
       </c>
       <c r="C53" t="s">
-        <v>37226</v>
+        <v>37586</v>
       </c>
       <c r="D53" s="1">
         <v>0.88300001621246338</v>
@@ -113957,21 +115037,21 @@
       </c>
       <c r="G53" s="1"/>
       <c r="H53" t="s">
-        <v>37253</v>
+        <v>37613</v>
       </c>
       <c r="I53" t="s">
-        <v>37312</v>
+        <v>37672</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>37147</v>
+        <v>37507</v>
       </c>
       <c r="B54" t="s">
-        <v>37204</v>
+        <v>37564</v>
       </c>
       <c r="C54" t="s">
-        <v>37227</v>
+        <v>37587</v>
       </c>
       <c r="D54" s="1">
         <v>0.6600000262260437</v>
@@ -113984,21 +115064,21 @@
       </c>
       <c r="G54" s="1"/>
       <c r="H54" t="s">
-        <v>37254</v>
+        <v>37614</v>
       </c>
       <c r="I54" t="s">
-        <v>37313</v>
+        <v>37673</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>37147</v>
+        <v>37507</v>
       </c>
       <c r="B55" t="s">
-        <v>37205</v>
+        <v>37565</v>
       </c>
       <c r="C55" t="s">
-        <v>37227</v>
+        <v>37587</v>
       </c>
       <c r="D55" s="1">
         <v>0.63999998569488525</v>
@@ -114011,21 +115091,21 @@
       </c>
       <c r="G55" s="1"/>
       <c r="H55" t="s">
-        <v>37254</v>
+        <v>37614</v>
       </c>
       <c r="I55" t="s">
-        <v>37314</v>
+        <v>37674</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>37148</v>
+        <v>37508</v>
       </c>
       <c r="B56" t="s">
-        <v>37206</v>
+        <v>37566</v>
       </c>
       <c r="C56" t="s">
-        <v>37228</v>
+        <v>37588</v>
       </c>
       <c r="D56" s="1">
         <v>0.89999997615814209</v>
@@ -114038,21 +115118,21 @@
       </c>
       <c r="G56" s="1"/>
       <c r="H56" t="s">
-        <v>37255</v>
+        <v>37615</v>
       </c>
       <c r="I56" t="s">
-        <v>37315</v>
+        <v>37675</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>37148</v>
+        <v>37508</v>
       </c>
       <c r="B57" t="s">
-        <v>37207</v>
+        <v>37567</v>
       </c>
       <c r="C57" t="s">
-        <v>37228</v>
+        <v>37588</v>
       </c>
       <c r="D57" s="1">
         <v>0.95999997854232788</v>
@@ -114065,21 +115145,21 @@
       </c>
       <c r="G57" s="1"/>
       <c r="H57" t="s">
-        <v>37255</v>
+        <v>37615</v>
       </c>
       <c r="I57" t="s">
-        <v>37316</v>
+        <v>37676</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>37149</v>
+        <v>37509</v>
       </c>
       <c r="B58" t="s">
-        <v>37208</v>
+        <v>37568</v>
       </c>
       <c r="C58" t="s">
-        <v>37229</v>
+        <v>37589</v>
       </c>
       <c r="D58" s="1">
         <v>0.4699999988079071</v>
@@ -114092,21 +115172,21 @@
       </c>
       <c r="G58" s="1"/>
       <c r="H58" t="s">
-        <v>37256</v>
+        <v>37616</v>
       </c>
       <c r="I58" t="s">
-        <v>37317</v>
+        <v>37677</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>37149</v>
+        <v>37509</v>
       </c>
       <c r="B59" t="s">
-        <v>37209</v>
+        <v>37569</v>
       </c>
       <c r="C59" t="s">
-        <v>37229</v>
+        <v>37589</v>
       </c>
       <c r="D59" s="1">
         <v>0.47999998927116394</v>
@@ -114119,21 +115199,21 @@
       </c>
       <c r="G59" s="1"/>
       <c r="H59" t="s">
-        <v>37256</v>
+        <v>37616</v>
       </c>
       <c r="I59" t="s">
-        <v>37318</v>
+        <v>37678</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>37149</v>
+        <v>37509</v>
       </c>
       <c r="B60" t="s">
-        <v>37210</v>
+        <v>37570</v>
       </c>
       <c r="C60" t="s">
-        <v>37230</v>
+        <v>37590</v>
       </c>
       <c r="D60" s="1">
         <v>0.43999999761581421</v>
@@ -114146,21 +115226,21 @@
       </c>
       <c r="G60" s="1"/>
       <c r="H60" t="s">
-        <v>37257</v>
+        <v>37617</v>
       </c>
       <c r="I60" t="s">
-        <v>37319</v>
+        <v>37679</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>37149</v>
+        <v>37509</v>
       </c>
       <c r="B61" t="s">
-        <v>37211</v>
+        <v>37571</v>
       </c>
       <c r="C61" t="s">
-        <v>37230</v>
+        <v>37590</v>
       </c>
       <c r="D61" s="1">
         <v>0.75999999046325684</v>
@@ -114173,21 +115253,21 @@
       </c>
       <c r="G61" s="1"/>
       <c r="H61" t="s">
-        <v>37257</v>
+        <v>37617</v>
       </c>
       <c r="I61" t="s">
-        <v>37320</v>
+        <v>37680</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>37150</v>
+        <v>37510</v>
       </c>
       <c r="B62" t="s">
-        <v>37212</v>
+        <v>37572</v>
       </c>
       <c r="C62" t="s">
-        <v>37230</v>
+        <v>37590</v>
       </c>
       <c r="D62" s="1">
         <v>0.81000000238418579</v>
@@ -114200,21 +115280,21 @@
       </c>
       <c r="G62" s="1"/>
       <c r="H62" t="s">
-        <v>37258</v>
+        <v>37618</v>
       </c>
       <c r="I62" t="s">
-        <v>37321</v>
+        <v>37681</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>37150</v>
+        <v>37510</v>
       </c>
       <c r="B63" t="s">
-        <v>37213</v>
+        <v>37573</v>
       </c>
       <c r="C63" t="s">
-        <v>37230</v>
+        <v>37590</v>
       </c>
       <c r="D63" s="1">
         <v>0.79000002145767212</v>
@@ -114227,21 +115307,21 @@
       </c>
       <c r="G63" s="1"/>
       <c r="H63" t="s">
-        <v>37258</v>
+        <v>37618</v>
       </c>
       <c r="I63" t="s">
-        <v>37322</v>
+        <v>37682</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>37151</v>
+        <v>37511</v>
       </c>
       <c r="B64" t="s">
-        <v>37214</v>
+        <v>37574</v>
       </c>
       <c r="C64" t="s">
-        <v>37231</v>
+        <v>37591</v>
       </c>
       <c r="D64" s="1">
         <v>0.6600000262260437</v>
@@ -114254,21 +115334,21 @@
       </c>
       <c r="G64" s="1"/>
       <c r="H64" t="s">
-        <v>37259</v>
+        <v>37619</v>
       </c>
       <c r="I64" t="s">
-        <v>37323</v>
+        <v>37683</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>37151</v>
+        <v>37511</v>
       </c>
       <c r="B65" t="s">
-        <v>37215</v>
+        <v>37575</v>
       </c>
       <c r="C65" t="s">
-        <v>37231</v>
+        <v>37591</v>
       </c>
       <c r="D65" s="1">
         <v>0.55000001192092896</v>
@@ -114281,10 +115361,10 @@
       </c>
       <c r="G65" s="1"/>
       <c r="H65" t="s">
-        <v>37259</v>
+        <v>37619</v>
       </c>
       <c r="I65" t="s">
-        <v>37324</v>
+        <v>37684</v>
       </c>
     </row>
   </sheetData>
@@ -114298,42 +115378,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>37325</v>
+        <v>37685</v>
       </c>
       <c r="B1" t="s">
-        <v>37347</v>
+        <v>37707</v>
       </c>
       <c r="C1" t="s">
-        <v>37394</v>
+        <v>37754</v>
       </c>
       <c r="D1" t="s">
-        <v>37404</v>
+        <v>37764</v>
       </c>
       <c r="E1" t="s">
-        <v>37405</v>
+        <v>37765</v>
       </c>
       <c r="F1" t="s">
-        <v>37406</v>
+        <v>37766</v>
       </c>
       <c r="G1" t="s">
-        <v>37407</v>
+        <v>37767</v>
       </c>
       <c r="H1" t="s">
-        <v>37419</v>
+        <v>37779</v>
       </c>
       <c r="I1" t="s">
-        <v>37440</v>
+        <v>37800</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>37326</v>
+        <v>37686</v>
       </c>
       <c r="B2" t="s">
-        <v>37348</v>
+        <v>37708</v>
       </c>
       <c r="C2" t="s">
-        <v>37395</v>
+        <v>37755</v>
       </c>
       <c r="D2" s="1">
         <v>0.5899999737739563</v>
@@ -114345,24 +115425,24 @@
         <v>0.81999999284744263</v>
       </c>
       <c r="G2" t="s">
-        <v>37408</v>
+        <v>37768</v>
       </c>
       <c r="H2" t="s">
-        <v>37420</v>
+        <v>37780</v>
       </c>
       <c r="I2" t="s">
-        <v>37441</v>
+        <v>37801</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>37326</v>
+        <v>37686</v>
       </c>
       <c r="B3" t="s">
-        <v>37349</v>
+        <v>37709</v>
       </c>
       <c r="C3" t="s">
-        <v>37395</v>
+        <v>37755</v>
       </c>
       <c r="D3" s="1">
         <v>0.18000000715255737</v>
@@ -114374,24 +115454,24 @@
         <v>1.4900000095367432</v>
       </c>
       <c r="G3" t="s">
-        <v>37408</v>
+        <v>37768</v>
       </c>
       <c r="H3" t="s">
-        <v>37420</v>
+        <v>37780</v>
       </c>
       <c r="I3" t="s">
-        <v>37442</v>
+        <v>37802</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>37327</v>
+        <v>37687</v>
       </c>
       <c r="B4" t="s">
-        <v>37350</v>
+        <v>37710</v>
       </c>
       <c r="C4" t="s">
-        <v>37395</v>
+        <v>37755</v>
       </c>
       <c r="D4" s="1">
         <v>0.37999999523162842</v>
@@ -114403,24 +115483,24 @@
         <v>0.6600000262260437</v>
       </c>
       <c r="G4" t="s">
-        <v>37408</v>
+        <v>37768</v>
       </c>
       <c r="H4" t="s">
-        <v>37421</v>
+        <v>37781</v>
       </c>
       <c r="I4" t="s">
-        <v>37443</v>
+        <v>37803</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>37327</v>
+        <v>37687</v>
       </c>
       <c r="B5" t="s">
-        <v>37351</v>
+        <v>37711</v>
       </c>
       <c r="C5" t="s">
-        <v>37395</v>
+        <v>37755</v>
       </c>
       <c r="D5" s="1">
         <v>0.44999998807907104</v>
@@ -114432,24 +115512,24 @@
         <v>0.57999998331069946</v>
       </c>
       <c r="G5" t="s">
-        <v>37408</v>
+        <v>37768</v>
       </c>
       <c r="H5" t="s">
-        <v>37421</v>
+        <v>37781</v>
       </c>
       <c r="I5" t="s">
-        <v>37444</v>
+        <v>37804</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>37328</v>
+        <v>37688</v>
       </c>
       <c r="B6" t="s">
-        <v>37352</v>
+        <v>37712</v>
       </c>
       <c r="C6" t="s">
-        <v>37395</v>
+        <v>37755</v>
       </c>
       <c r="D6" s="1">
         <v>0.75700002908706665</v>
@@ -114461,24 +115541,24 @@
         <v>0.96299999952316284</v>
       </c>
       <c r="G6" t="s">
-        <v>37409</v>
+        <v>37769</v>
       </c>
       <c r="H6" t="s">
-        <v>37422</v>
+        <v>37782</v>
       </c>
       <c r="I6" t="s">
-        <v>37445</v>
+        <v>37805</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>37328</v>
+        <v>37688</v>
       </c>
       <c r="B7" t="s">
-        <v>37353</v>
+        <v>37713</v>
       </c>
       <c r="C7" t="s">
-        <v>37395</v>
+        <v>37755</v>
       </c>
       <c r="D7" s="1">
         <v>0.92599999904632568</v>
@@ -114490,24 +115570,24 @@
         <v>1.2790000438690186</v>
       </c>
       <c r="G7" t="s">
-        <v>37410</v>
+        <v>37770</v>
       </c>
       <c r="H7" t="s">
-        <v>37422</v>
+        <v>37782</v>
       </c>
       <c r="I7" t="s">
-        <v>37446</v>
+        <v>37806</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>37329</v>
+        <v>37689</v>
       </c>
       <c r="B8" t="s">
-        <v>37354</v>
+        <v>37714</v>
       </c>
       <c r="C8" t="s">
-        <v>37395</v>
+        <v>37755</v>
       </c>
       <c r="D8" s="1">
         <v>0.43999999761581421</v>
@@ -114519,24 +115599,24 @@
         <v>0.56000000238418579</v>
       </c>
       <c r="G8" t="s">
-        <v>37411</v>
+        <v>37771</v>
       </c>
       <c r="H8" t="s">
-        <v>37423</v>
+        <v>37783</v>
       </c>
       <c r="I8" t="s">
-        <v>37447</v>
+        <v>37807</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>37329</v>
+        <v>37689</v>
       </c>
       <c r="B9" t="s">
-        <v>37355</v>
+        <v>37715</v>
       </c>
       <c r="C9" t="s">
-        <v>37395</v>
+        <v>37755</v>
       </c>
       <c r="D9" s="1">
         <v>0.80000001192092896</v>
@@ -114548,24 +115628,24 @@
         <v>1.1100000143051147</v>
       </c>
       <c r="G9" t="s">
-        <v>37411</v>
+        <v>37771</v>
       </c>
       <c r="H9" t="s">
-        <v>37423</v>
+        <v>37783</v>
       </c>
       <c r="I9" t="s">
-        <v>37448</v>
+        <v>37808</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>37330</v>
+        <v>37690</v>
       </c>
       <c r="B10" t="s">
-        <v>37356</v>
+        <v>37716</v>
       </c>
       <c r="C10" t="s">
-        <v>37395</v>
+        <v>37755</v>
       </c>
       <c r="D10" s="1">
         <v>0.56000000238418579</v>
@@ -114577,24 +115657,24 @@
         <v>0.97000002861022949</v>
       </c>
       <c r="G10" t="s">
-        <v>37411</v>
+        <v>37771</v>
       </c>
       <c r="H10" t="s">
-        <v>37424</v>
+        <v>37784</v>
       </c>
       <c r="I10" t="s">
-        <v>37449</v>
+        <v>37809</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>37330</v>
+        <v>37690</v>
       </c>
       <c r="B11" t="s">
-        <v>37357</v>
+        <v>37717</v>
       </c>
       <c r="C11" t="s">
-        <v>37395</v>
+        <v>37755</v>
       </c>
       <c r="D11" s="1">
         <v>0.50999999046325684</v>
@@ -114606,24 +115686,24 @@
         <v>1.190000057220459</v>
       </c>
       <c r="G11" t="s">
-        <v>37411</v>
+        <v>37771</v>
       </c>
       <c r="H11" t="s">
-        <v>37424</v>
+        <v>37784</v>
       </c>
       <c r="I11" t="s">
-        <v>37450</v>
+        <v>37810</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>37331</v>
+        <v>37691</v>
       </c>
       <c r="B12" t="s">
-        <v>37358</v>
+        <v>37718</v>
       </c>
       <c r="C12" t="s">
-        <v>37395</v>
+        <v>37755</v>
       </c>
       <c r="D12" s="1">
         <v>0.6600000262260437</v>
@@ -114635,24 +115715,24 @@
         <v>0.89999997615814209</v>
       </c>
       <c r="G12" t="s">
-        <v>37411</v>
+        <v>37771</v>
       </c>
       <c r="H12" t="s">
-        <v>37425</v>
+        <v>37785</v>
       </c>
       <c r="I12" t="s">
-        <v>37451</v>
+        <v>37811</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>37331</v>
+        <v>37691</v>
       </c>
       <c r="B13" t="s">
-        <v>37359</v>
+        <v>37719</v>
       </c>
       <c r="C13" t="s">
-        <v>37395</v>
+        <v>37755</v>
       </c>
       <c r="D13" s="1">
         <v>0.36000001430511475</v>
@@ -114664,24 +115744,24 @@
         <v>0.82999998331069946</v>
       </c>
       <c r="G13" t="s">
-        <v>37411</v>
+        <v>37771</v>
       </c>
       <c r="H13" t="s">
-        <v>37425</v>
+        <v>37785</v>
       </c>
       <c r="I13" t="s">
-        <v>37452</v>
+        <v>37812</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>37332</v>
+        <v>37692</v>
       </c>
       <c r="B14" t="s">
-        <v>37360</v>
+        <v>37720</v>
       </c>
       <c r="C14" t="s">
-        <v>37395</v>
+        <v>37755</v>
       </c>
       <c r="D14" s="1">
         <v>0.55299997329711914</v>
@@ -114693,24 +115773,24 @@
         <v>0.9309999942779541</v>
       </c>
       <c r="G14" t="s">
-        <v>37412</v>
+        <v>37772</v>
       </c>
       <c r="H14" t="s">
-        <v>37426</v>
+        <v>37786</v>
       </c>
       <c r="I14" t="s">
-        <v>37453</v>
+        <v>37813</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>37332</v>
+        <v>37692</v>
       </c>
       <c r="B15" t="s">
-        <v>37361</v>
+        <v>37721</v>
       </c>
       <c r="C15" t="s">
-        <v>37395</v>
+        <v>37755</v>
       </c>
       <c r="D15" s="1">
         <v>0.76599997282028198</v>
@@ -114722,24 +115802,24 @@
         <v>3.9639999866485596</v>
       </c>
       <c r="G15" t="s">
-        <v>37412</v>
+        <v>37772</v>
       </c>
       <c r="H15" t="s">
-        <v>37426</v>
+        <v>37786</v>
       </c>
       <c r="I15" t="s">
-        <v>37454</v>
+        <v>37814</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>37332</v>
+        <v>37692</v>
       </c>
       <c r="B16" t="s">
-        <v>37362</v>
+        <v>37722</v>
       </c>
       <c r="C16" t="s">
-        <v>37396</v>
+        <v>37756</v>
       </c>
       <c r="D16" s="1">
         <v>0.39800000190734863</v>
@@ -114751,24 +115831,24 @@
         <v>0.71899998188018799</v>
       </c>
       <c r="G16" t="s">
-        <v>37412</v>
+        <v>37772</v>
       </c>
       <c r="H16" t="s">
-        <v>37427</v>
+        <v>37787</v>
       </c>
       <c r="I16" t="s">
-        <v>37455</v>
+        <v>37815</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>37332</v>
+        <v>37692</v>
       </c>
       <c r="B17" t="s">
-        <v>37363</v>
+        <v>37723</v>
       </c>
       <c r="C17" t="s">
-        <v>37396</v>
+        <v>37756</v>
       </c>
       <c r="D17" s="1">
         <v>0.49799999594688416</v>
@@ -114780,24 +115860,24 @@
         <v>2.4030001163482666</v>
       </c>
       <c r="G17" t="s">
-        <v>37412</v>
+        <v>37772</v>
       </c>
       <c r="H17" t="s">
-        <v>37427</v>
+        <v>37787</v>
       </c>
       <c r="I17" t="s">
-        <v>37456</v>
+        <v>37816</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>37333</v>
+        <v>37693</v>
       </c>
       <c r="B18" t="s">
-        <v>37364</v>
+        <v>37724</v>
       </c>
       <c r="C18" t="s">
-        <v>37397</v>
+        <v>37757</v>
       </c>
       <c r="D18" s="1">
         <v>0.87000000476837158</v>
@@ -114809,24 +115889,24 @@
         <v>1.2899999618530273</v>
       </c>
       <c r="G18" t="s">
-        <v>37413</v>
+        <v>37773</v>
       </c>
       <c r="H18" t="s">
-        <v>37428</v>
+        <v>37788</v>
       </c>
       <c r="I18" t="s">
-        <v>37457</v>
+        <v>37817</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>37333</v>
+        <v>37693</v>
       </c>
       <c r="B19" t="s">
-        <v>37365</v>
+        <v>37725</v>
       </c>
       <c r="C19" t="s">
-        <v>37397</v>
+        <v>37757</v>
       </c>
       <c r="D19" s="1">
         <v>0.38999998569488525</v>
@@ -114838,24 +115918,24 @@
         <v>0.80000001192092896</v>
       </c>
       <c r="G19" t="s">
-        <v>37413</v>
+        <v>37773</v>
       </c>
       <c r="H19" t="s">
-        <v>37428</v>
+        <v>37788</v>
       </c>
       <c r="I19" t="s">
-        <v>37458</v>
+        <v>37818</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>37334</v>
+        <v>37694</v>
       </c>
       <c r="B20" t="s">
-        <v>37366</v>
+        <v>37726</v>
       </c>
       <c r="C20" t="s">
-        <v>37397</v>
+        <v>37757</v>
       </c>
       <c r="D20" s="1">
         <v>0.61000001430511475</v>
@@ -114867,24 +115947,24 @@
         <v>1.1699999570846558</v>
       </c>
       <c r="G20" t="s">
-        <v>37413</v>
+        <v>37773</v>
       </c>
       <c r="H20" t="s">
-        <v>37429</v>
+        <v>37789</v>
       </c>
       <c r="I20" t="s">
-        <v>37459</v>
+        <v>37819</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>37334</v>
+        <v>37694</v>
       </c>
       <c r="B21" t="s">
-        <v>37367</v>
+        <v>37727</v>
       </c>
       <c r="C21" t="s">
-        <v>37397</v>
+        <v>37757</v>
       </c>
       <c r="D21" s="1">
         <v>0.75</v>
@@ -114896,24 +115976,24 @@
         <v>1.3600000143051147</v>
       </c>
       <c r="G21" t="s">
-        <v>37413</v>
+        <v>37773</v>
       </c>
       <c r="H21" t="s">
-        <v>37429</v>
+        <v>37789</v>
       </c>
       <c r="I21" t="s">
-        <v>37460</v>
+        <v>37820</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>37334</v>
+        <v>37694</v>
       </c>
       <c r="B22" t="s">
-        <v>37368</v>
+        <v>37728</v>
       </c>
       <c r="C22" t="s">
-        <v>37398</v>
+        <v>37758</v>
       </c>
       <c r="D22" s="1">
         <v>5.9000000953674316</v>
@@ -114925,24 +116005,24 @@
         <v>46.099998474121094</v>
       </c>
       <c r="G22" t="s">
-        <v>37413</v>
+        <v>37773</v>
       </c>
       <c r="H22" t="s">
-        <v>37430</v>
+        <v>37790</v>
       </c>
       <c r="I22" t="s">
-        <v>37461</v>
+        <v>37821</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>37334</v>
+        <v>37694</v>
       </c>
       <c r="B23" t="s">
-        <v>37369</v>
+        <v>37729</v>
       </c>
       <c r="C23" t="s">
-        <v>37398</v>
+        <v>37758</v>
       </c>
       <c r="D23" s="1">
         <v>1.8200000524520874</v>
@@ -114954,24 +116034,24 @@
         <v>5.1399998664855957</v>
       </c>
       <c r="G23" t="s">
-        <v>37413</v>
+        <v>37773</v>
       </c>
       <c r="H23" t="s">
-        <v>37430</v>
+        <v>37790</v>
       </c>
       <c r="I23" t="s">
-        <v>37462</v>
+        <v>37822</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>37335</v>
+        <v>37695</v>
       </c>
       <c r="B24" t="s">
-        <v>37370</v>
+        <v>37730</v>
       </c>
       <c r="C24" t="s">
-        <v>37399</v>
+        <v>37759</v>
       </c>
       <c r="D24" s="1">
         <v>0.5899999737739563</v>
@@ -114983,24 +116063,24 @@
         <v>1.3999999761581421</v>
       </c>
       <c r="G24" t="s">
-        <v>37413</v>
+        <v>37773</v>
       </c>
       <c r="H24" t="s">
-        <v>37431</v>
+        <v>37791</v>
       </c>
       <c r="I24" t="s">
-        <v>37463</v>
+        <v>37823</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>37335</v>
+        <v>37695</v>
       </c>
       <c r="B25" t="s">
-        <v>37371</v>
+        <v>37731</v>
       </c>
       <c r="C25" t="s">
-        <v>37399</v>
+        <v>37759</v>
       </c>
       <c r="D25" s="1">
         <v>0.69999998807907104</v>
@@ -115012,24 +116092,24 @@
         <v>0.87000000476837158</v>
       </c>
       <c r="G25" t="s">
-        <v>37413</v>
+        <v>37773</v>
       </c>
       <c r="H25" t="s">
-        <v>37431</v>
+        <v>37791</v>
       </c>
       <c r="I25" t="s">
-        <v>37464</v>
+        <v>37824</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>37336</v>
+        <v>37696</v>
       </c>
       <c r="B26" t="s">
-        <v>37372</v>
+        <v>37732</v>
       </c>
       <c r="C26" t="s">
-        <v>37399</v>
+        <v>37759</v>
       </c>
       <c r="D26" s="1">
         <v>0.38999998569488525</v>
@@ -115041,24 +116121,24 @@
         <v>0.68999999761581421</v>
       </c>
       <c r="G26" t="s">
-        <v>37413</v>
+        <v>37773</v>
       </c>
       <c r="H26" t="s">
-        <v>37432</v>
+        <v>37792</v>
       </c>
       <c r="I26" t="s">
-        <v>37465</v>
+        <v>37825</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>37336</v>
+        <v>37696</v>
       </c>
       <c r="B27" t="s">
-        <v>37373</v>
+        <v>37733</v>
       </c>
       <c r="C27" t="s">
-        <v>37399</v>
+        <v>37759</v>
       </c>
       <c r="D27" s="1">
         <v>0.15999999642372131</v>
@@ -115070,24 +116150,24 @@
         <v>0.40000000596046448</v>
       </c>
       <c r="G27" t="s">
-        <v>37413</v>
+        <v>37773</v>
       </c>
       <c r="H27" t="s">
-        <v>37432</v>
+        <v>37792</v>
       </c>
       <c r="I27" t="s">
-        <v>37466</v>
+        <v>37826</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>37337</v>
+        <v>37697</v>
       </c>
       <c r="B28" t="s">
-        <v>37374</v>
+        <v>37734</v>
       </c>
       <c r="C28" t="s">
-        <v>37399</v>
+        <v>37759</v>
       </c>
       <c r="D28" s="1">
         <v>0.46000000834465027</v>
@@ -115099,24 +116179,24 @@
         <v>0.6600000262260437</v>
       </c>
       <c r="G28" t="s">
-        <v>37413</v>
+        <v>37773</v>
       </c>
       <c r="H28" t="s">
-        <v>37432</v>
+        <v>37792</v>
       </c>
       <c r="I28" t="s">
-        <v>37467</v>
+        <v>37827</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>37337</v>
+        <v>37697</v>
       </c>
       <c r="B29" t="s">
-        <v>37375</v>
+        <v>37735</v>
       </c>
       <c r="C29" t="s">
-        <v>37399</v>
+        <v>37759</v>
       </c>
       <c r="D29" s="1">
         <v>0.30000001192092896</v>
@@ -115128,24 +116208,24 @@
         <v>0.44999998807907104</v>
       </c>
       <c r="G29" t="s">
-        <v>37413</v>
+        <v>37773</v>
       </c>
       <c r="H29" t="s">
-        <v>37432</v>
+        <v>37792</v>
       </c>
       <c r="I29" t="s">
-        <v>37468</v>
+        <v>37828</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>37338</v>
+        <v>37698</v>
       </c>
       <c r="B30" t="s">
-        <v>37376</v>
+        <v>37736</v>
       </c>
       <c r="C30" t="s">
-        <v>37399</v>
+        <v>37759</v>
       </c>
       <c r="D30" s="1">
         <v>0.60000002384185791</v>
@@ -115157,24 +116237,24 @@
         <v>1.059999942779541</v>
       </c>
       <c r="G30" t="s">
-        <v>37413</v>
+        <v>37773</v>
       </c>
       <c r="H30" t="s">
-        <v>37433</v>
+        <v>37793</v>
       </c>
       <c r="I30" t="s">
-        <v>37469</v>
+        <v>37829</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>37338</v>
+        <v>37698</v>
       </c>
       <c r="B31" t="s">
-        <v>37377</v>
+        <v>37737</v>
       </c>
       <c r="C31" t="s">
-        <v>37399</v>
+        <v>37759</v>
       </c>
       <c r="D31" s="1">
         <v>0.47999998927116394</v>
@@ -115186,24 +116266,24 @@
         <v>0.81999999284744263</v>
       </c>
       <c r="G31" t="s">
-        <v>37413</v>
+        <v>37773</v>
       </c>
       <c r="H31" t="s">
-        <v>37433</v>
+        <v>37793</v>
       </c>
       <c r="I31" t="s">
-        <v>37470</v>
+        <v>37830</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>37339</v>
+        <v>37699</v>
       </c>
       <c r="B32" t="s">
-        <v>37378</v>
+        <v>37738</v>
       </c>
       <c r="C32" t="s">
-        <v>37399</v>
+        <v>37759</v>
       </c>
       <c r="D32" s="1">
         <v>1.6200000047683716</v>
@@ -115215,24 +116295,24 @@
         <v>2.4100000858306885</v>
       </c>
       <c r="G32" t="s">
-        <v>37413</v>
+        <v>37773</v>
       </c>
       <c r="H32" t="s">
-        <v>37433</v>
+        <v>37793</v>
       </c>
       <c r="I32" t="s">
-        <v>37471</v>
+        <v>37831</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>37339</v>
+        <v>37699</v>
       </c>
       <c r="B33" t="s">
-        <v>37379</v>
+        <v>37739</v>
       </c>
       <c r="C33" t="s">
-        <v>37399</v>
+        <v>37759</v>
       </c>
       <c r="D33" s="1">
         <v>2.0099999904632568</v>
@@ -115244,24 +116324,24 @@
         <v>2.8399999141693115</v>
       </c>
       <c r="G33" t="s">
-        <v>37413</v>
+        <v>37773</v>
       </c>
       <c r="H33" t="s">
-        <v>37433</v>
+        <v>37793</v>
       </c>
       <c r="I33" t="s">
-        <v>37472</v>
+        <v>37832</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>37340</v>
+        <v>37700</v>
       </c>
       <c r="B34" t="s">
-        <v>37380</v>
+        <v>37740</v>
       </c>
       <c r="C34" t="s">
-        <v>37400</v>
+        <v>37760</v>
       </c>
       <c r="D34" s="1">
         <v>0.95999997854232788</v>
@@ -115273,24 +116353,24 @@
         <v>1.2560000419616699</v>
       </c>
       <c r="G34" t="s">
-        <v>37414</v>
+        <v>37774</v>
       </c>
       <c r="H34" t="s">
-        <v>37434</v>
+        <v>37794</v>
       </c>
       <c r="I34" t="s">
-        <v>37473</v>
+        <v>37833</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>37340</v>
+        <v>37700</v>
       </c>
       <c r="B35" t="s">
-        <v>37381</v>
+        <v>37741</v>
       </c>
       <c r="C35" t="s">
-        <v>37400</v>
+        <v>37760</v>
       </c>
       <c r="D35" s="1">
         <v>1.0800000429153442</v>
@@ -115302,24 +116382,24 @@
         <v>1.3609999418258667</v>
       </c>
       <c r="G35" t="s">
-        <v>37414</v>
+        <v>37774</v>
       </c>
       <c r="H35" t="s">
-        <v>37434</v>
+        <v>37794</v>
       </c>
       <c r="I35" t="s">
-        <v>37474</v>
+        <v>37834</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>37341</v>
+        <v>37701</v>
       </c>
       <c r="B36" t="s">
-        <v>37382</v>
+        <v>37742</v>
       </c>
       <c r="C36" t="s">
-        <v>37400</v>
+        <v>37760</v>
       </c>
       <c r="D36" s="1">
         <v>0.87699997425079346</v>
@@ -115331,24 +116411,24 @@
         <v>1.156000018119812</v>
       </c>
       <c r="G36" t="s">
-        <v>37415</v>
+        <v>37775</v>
       </c>
       <c r="H36" t="s">
-        <v>37435</v>
+        <v>37795</v>
       </c>
       <c r="I36" t="s">
-        <v>37475</v>
+        <v>37835</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>37341</v>
+        <v>37701</v>
       </c>
       <c r="B37" t="s">
-        <v>37383</v>
+        <v>37743</v>
       </c>
       <c r="C37" t="s">
-        <v>37400</v>
+        <v>37760</v>
       </c>
       <c r="D37" s="1">
         <v>0.68400001525878906</v>
@@ -115360,24 +116440,24 @@
         <v>0.875</v>
       </c>
       <c r="G37" t="s">
-        <v>37415</v>
+        <v>37775</v>
       </c>
       <c r="H37" t="s">
-        <v>37435</v>
+        <v>37795</v>
       </c>
       <c r="I37" t="s">
-        <v>37476</v>
+        <v>37836</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>37341</v>
+        <v>37701</v>
       </c>
       <c r="B38" t="s">
-        <v>37384</v>
+        <v>37744</v>
       </c>
       <c r="C38" t="s">
-        <v>37400</v>
+        <v>37760</v>
       </c>
       <c r="D38" s="1">
         <v>0.85699999332427979</v>
@@ -115389,24 +116469,24 @@
         <v>1.1779999732971191</v>
       </c>
       <c r="G38" t="s">
-        <v>37415</v>
+        <v>37775</v>
       </c>
       <c r="H38" t="s">
-        <v>37435</v>
+        <v>37795</v>
       </c>
       <c r="I38" t="s">
-        <v>37477</v>
+        <v>37837</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>37342</v>
+        <v>37702</v>
       </c>
       <c r="B39" t="s">
-        <v>37384</v>
+        <v>37744</v>
       </c>
       <c r="C39" t="s">
-        <v>37401</v>
+        <v>37761</v>
       </c>
       <c r="D39" s="1">
         <v>0.64999997615814209</v>
@@ -115418,24 +116498,24 @@
         <v>0.8399999737739563</v>
       </c>
       <c r="G39" t="s">
-        <v>37416</v>
+        <v>37776</v>
       </c>
       <c r="H39" t="s">
-        <v>37435</v>
+        <v>37795</v>
       </c>
       <c r="I39" t="s">
-        <v>37478</v>
+        <v>37838</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>37342</v>
+        <v>37702</v>
       </c>
       <c r="B40" t="s">
-        <v>37385</v>
+        <v>37745</v>
       </c>
       <c r="C40" t="s">
-        <v>37401</v>
+        <v>37761</v>
       </c>
       <c r="D40" s="1">
         <v>0.47999998927116394</v>
@@ -115447,24 +116527,24 @@
         <v>0.75</v>
       </c>
       <c r="G40" t="s">
-        <v>37416</v>
+        <v>37776</v>
       </c>
       <c r="H40" t="s">
-        <v>37435</v>
+        <v>37795</v>
       </c>
       <c r="I40" t="s">
-        <v>37479</v>
+        <v>37839</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>37343</v>
+        <v>37703</v>
       </c>
       <c r="B41" t="s">
-        <v>37386</v>
+        <v>37746</v>
       </c>
       <c r="C41" t="s">
-        <v>37402</v>
+        <v>37762</v>
       </c>
       <c r="D41" s="1">
         <v>0.78100001811981201</v>
@@ -115476,24 +116556,24 @@
         <v>1.3220000267028809</v>
       </c>
       <c r="G41" t="s">
-        <v>37417</v>
+        <v>37777</v>
       </c>
       <c r="H41" t="s">
-        <v>37436</v>
+        <v>37796</v>
       </c>
       <c r="I41" t="s">
-        <v>37480</v>
+        <v>37840</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>37343</v>
+        <v>37703</v>
       </c>
       <c r="B42" t="s">
-        <v>37387</v>
+        <v>37747</v>
       </c>
       <c r="C42" t="s">
-        <v>37402</v>
+        <v>37762</v>
       </c>
       <c r="D42" s="1">
         <v>0.97500002384185791</v>
@@ -115505,82 +116585,82 @@
         <v>1.1829999685287476</v>
       </c>
       <c r="G42" t="s">
-        <v>37417</v>
+        <v>37777</v>
       </c>
       <c r="H42" t="s">
-        <v>37436</v>
+        <v>37796</v>
       </c>
       <c r="I42" t="s">
-        <v>37481</v>
+        <v>37841</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>37344</v>
+        <v>37704</v>
       </c>
       <c r="B43" t="s">
-        <v>37388</v>
+        <v>37748</v>
       </c>
       <c r="C43" t="s">
-        <v>37402</v>
+        <v>37762</v>
       </c>
       <c r="D43" s="1">
-        <v>0.93000000715255737</v>
+        <v>0.93999999761581421</v>
       </c>
       <c r="E43" s="1">
-        <v>0.6600000262260437</v>
+        <v>0.74000000953674316</v>
       </c>
       <c r="F43" s="1">
-        <v>1.309999942779541</v>
+        <v>1.190000057220459</v>
       </c>
       <c r="G43" t="s">
-        <v>37418</v>
+        <v>37778</v>
       </c>
       <c r="H43" t="s">
-        <v>37437</v>
+        <v>37797</v>
       </c>
       <c r="I43" t="s">
-        <v>37482</v>
+        <v>37842</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>37344</v>
+        <v>37704</v>
       </c>
       <c r="B44" t="s">
-        <v>37389</v>
+        <v>37749</v>
       </c>
       <c r="C44" t="s">
-        <v>37402</v>
+        <v>37762</v>
       </c>
       <c r="D44" s="1">
-        <v>0.93999999761581421</v>
+        <v>0.93000000715255737</v>
       </c>
       <c r="E44" s="1">
-        <v>0.74000000953674316</v>
+        <v>0.6600000262260437</v>
       </c>
       <c r="F44" s="1">
-        <v>1.190000057220459</v>
+        <v>1.309999942779541</v>
       </c>
       <c r="G44" t="s">
-        <v>37418</v>
+        <v>37778</v>
       </c>
       <c r="H44" t="s">
-        <v>37437</v>
+        <v>37797</v>
       </c>
       <c r="I44" t="s">
-        <v>37483</v>
+        <v>37843</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>37345</v>
+        <v>37705</v>
       </c>
       <c r="B45" t="s">
-        <v>37390</v>
+        <v>37750</v>
       </c>
       <c r="C45" t="s">
-        <v>37403</v>
+        <v>37763</v>
       </c>
       <c r="D45" s="1">
         <v>0.63999998569488525</v>
@@ -115592,24 +116672,24 @@
         <v>0.9100000262260437</v>
       </c>
       <c r="G45" t="s">
-        <v>37418</v>
+        <v>37778</v>
       </c>
       <c r="H45" t="s">
-        <v>37438</v>
+        <v>37798</v>
       </c>
       <c r="I45" t="s">
-        <v>37484</v>
+        <v>37844</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>37345</v>
+        <v>37705</v>
       </c>
       <c r="B46" t="s">
-        <v>37391</v>
+        <v>37751</v>
       </c>
       <c r="C46" t="s">
-        <v>37403</v>
+        <v>37763</v>
       </c>
       <c r="D46" s="1">
         <v>0.72000002861022949</v>
@@ -115621,24 +116701,24 @@
         <v>0.89999997615814209</v>
       </c>
       <c r="G46" t="s">
-        <v>37418</v>
+        <v>37778</v>
       </c>
       <c r="H46" t="s">
-        <v>37438</v>
+        <v>37798</v>
       </c>
       <c r="I46" t="s">
-        <v>37485</v>
+        <v>37845</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>37346</v>
+        <v>37706</v>
       </c>
       <c r="B47" t="s">
-        <v>37392</v>
+        <v>37752</v>
       </c>
       <c r="C47" t="s">
-        <v>37403</v>
+        <v>37763</v>
       </c>
       <c r="D47" s="1">
         <v>0.46000000834465027</v>
@@ -115650,24 +116730,24 @@
         <v>0.73000001907348633</v>
       </c>
       <c r="G47" t="s">
-        <v>37418</v>
+        <v>37778</v>
       </c>
       <c r="H47" t="s">
-        <v>37439</v>
+        <v>37799</v>
       </c>
       <c r="I47" t="s">
-        <v>37486</v>
+        <v>37846</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>37346</v>
+        <v>37706</v>
       </c>
       <c r="B48" t="s">
-        <v>37393</v>
+        <v>37753</v>
       </c>
       <c r="C48" t="s">
-        <v>37403</v>
+        <v>37763</v>
       </c>
       <c r="D48" s="1">
         <v>0.62999999523162842</v>
@@ -115679,13 +116759,13 @@
         <v>0.89999997615814209</v>
       </c>
       <c r="G48" t="s">
-        <v>37418</v>
+        <v>37778</v>
       </c>
       <c r="H48" t="s">
-        <v>37439</v>
+        <v>37799</v>
       </c>
       <c r="I48" t="s">
-        <v>37487</v>
+        <v>37847</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct data for Jakubowiak 2016 (NCT01478048)
</commit_message>
<xml_diff>
--- a/products/Exported Data.xlsx
+++ b/products/Exported Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64595" uniqueCount="37848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65215" uniqueCount="38208">
   <si>
     <t>Study</t>
   </si>
@@ -101537,6 +101537,1086 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Study: Treatment 1 vs Treatment 2</t>
+  </si>
+  <si>
+    <t>Attal 2019 (ICARIA-MM): IsPd vs Pd</t>
+  </si>
+  <si>
+    <t>Bahlis 2020 (POLLUX): DRd vs Rd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2013 (VANTAGE 088): VorV vs V</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2016 (ENDEAVOR): Kd vs Vd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2018 (ELOQUENT-3): EPd vs Pd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2018 (ELOQUENT-2): ELd vs Ld</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2020 (ELOQUENT-2): ELd vs Ld</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2021 (APOLLO): DPd vs Pd</t>
+  </si>
+  <si>
+    <t>Grosicki 2020 (BOSTON): SeVd vs Vd</t>
+  </si>
+  <si>
+    <t>Hou 2017 (China Cont.): IRd vs Rd</t>
+  </si>
+  <si>
+    <t>Jakubowiak 2016 (NCT01478048): EVd vs Vd</t>
+  </si>
+  <si>
+    <t>Kumar 2020 (BELLINI): VeVd vs Vd</t>
+  </si>
+  <si>
+    <t>Lu 2021 (LEPUS): DVd vs Vd</t>
+  </si>
+  <si>
+    <t>Mateos 2020 (CASTOR): DVd vs Vd</t>
+  </si>
+  <si>
+    <t>Moreau 2021 (IKEMA): IsKd vs Kd</t>
+  </si>
+  <si>
+    <t>Orlowski 2019 (ENDEAVOR): Kd vs Vd</t>
+  </si>
+  <si>
+    <t>Richardson 2019 (OPTIMISMM): PVd vs Vd</t>
+  </si>
+  <si>
+    <t>Richardson 2021 (TOURMALINE-MM1): IRd vs Rd</t>
+  </si>
+  <si>
+    <t>San-Miguel 2014 (PANORAMA-1): FVd vs Vd</t>
+  </si>
+  <si>
+    <t>San-Miguel 2016 (PANORAMA 1): FVd vs Vd</t>
+  </si>
+  <si>
+    <t>San-Miguel 2013 (MM-003): Pd vs GC</t>
+  </si>
+  <si>
+    <t>Siegel 2018 (ASPIRE): KRd vs Rd</t>
+  </si>
+  <si>
+    <t>Usamani 2022 (CANDOR): DKd vs Kd</t>
+  </si>
+  <si>
+    <t>lot</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>&gt;3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>&gt;3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>&gt;=4</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>&gt;=4</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>&gt;3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>&gt;3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>&gt;1</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>&gt;2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>&gt;=3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>&gt;2</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>&gt;2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>&gt;=2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>Outcome</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Lower 95% CI Bound on HR</t>
+  </si>
+  <si>
+    <t>Upper 95% CI Bound on HR</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t>Tab. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tab. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      p. 808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. S3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. S4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      AT 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      p. 730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t>Data Extraction Errors</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Study: Treatment 1 vs Treatment 2</t>
+  </si>
+  <si>
+    <t>Attal 2019 (ICARIA-MM): IsPd vs Pd</t>
+  </si>
+  <si>
+    <t>Bahlis 2020 (POLLUX): DRd vs Rd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2013 (VANTAGE 088): VorV vs V</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2016 (ENDEAVOR): Kd vs Vd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2018 (ELOQUENT-3): EPd vs Pd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2021 (APOLLO): DPd vs Pd</t>
+  </si>
+  <si>
+    <t>Hou 2017 (China Cont.): IRd vs Rd</t>
+  </si>
+  <si>
+    <t>Jakubowiak 2016 (NCT01478048): EVd vs Vd</t>
+  </si>
+  <si>
+    <t>Kumar 2020 (BELLINI): VeVd vs Vd</t>
+  </si>
+  <si>
+    <t>Lonial 2015 (ELOQUENT-2): ELd vs Ld</t>
+  </si>
+  <si>
+    <t>Lu 2021 (LEPUS): DVd vs Vd</t>
+  </si>
+  <si>
+    <t>Mateos 2020 (CASTOR): DVd vs Vd</t>
+  </si>
+  <si>
+    <t>Moreau 2021 (IKEMA): IsKd vs Kd</t>
+  </si>
+  <si>
+    <t>Orlowski 2007 (NCT00103506): V vs DoxV</t>
+  </si>
+  <si>
+    <t>Orlowski 2016 (NCT00103506): V vs DoxV</t>
+  </si>
+  <si>
+    <t>Orlowski 2019 (ENDEAVOR): Kd vs Vd</t>
+  </si>
+  <si>
+    <t>Richardson 2019 (OPTIMISMM): PVd vs Vd</t>
+  </si>
+  <si>
+    <t>Richardson 2021 (TOURMALINE-MM1): IRd vs Rd</t>
+  </si>
+  <si>
+    <t>San-Miguel 2016 (PANORAMA 1): FVd vs Vd</t>
+  </si>
+  <si>
+    <t>Stewart 2015 (ASPIRE): KRd vs Rd</t>
+  </si>
+  <si>
+    <t>Usmani 2022 (CANDOR): DKd vs Kd</t>
+  </si>
+  <si>
+    <t>refract</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Previous R use</t>
+  </si>
+  <si>
+    <t>No previous R use</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No IMiD use</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Ref. to R and a PI</t>
+  </si>
+  <si>
+    <t>Not ref. to R and a PI</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No IMiD use</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No IMiD use</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No IMiD use</t>
+  </si>
+  <si>
+    <t>Naive</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Naive</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Previous R use</t>
+  </si>
+  <si>
+    <t>No previous R use</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Not refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Not refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Previous R or T use</t>
+  </si>
+  <si>
+    <t>No previous R or T use</t>
+  </si>
+  <si>
+    <t>Previous R or T use</t>
+  </si>
+  <si>
+    <t>No previous R or T use</t>
+  </si>
+  <si>
+    <t>Previous R use</t>
+  </si>
+  <si>
+    <t>No previous R use</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Refractory to T</t>
+  </si>
+  <si>
+    <t>Not refractory to T</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No previous IMiD use</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Not refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Outcome</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Lower 95% CI Bound on HR</t>
+  </si>
+  <si>
+    <t>Upper 95% CI Bound on HR</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0230</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .       Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tab. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      p. 808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. S3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. S4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t>Data Extraction Errors</t>
   </si>
   <si>
     <t/>
@@ -113608,42 +114688,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>37488</v>
+        <v>37848</v>
       </c>
       <c r="B1" t="s">
-        <v>37512</v>
+        <v>37872</v>
       </c>
       <c r="C1" t="s">
-        <v>37576</v>
+        <v>37936</v>
       </c>
       <c r="D1" t="s">
-        <v>37592</v>
+        <v>37952</v>
       </c>
       <c r="E1" t="s">
-        <v>37593</v>
+        <v>37953</v>
       </c>
       <c r="F1" t="s">
-        <v>37594</v>
+        <v>37954</v>
       </c>
       <c r="G1" t="s">
-        <v>37595</v>
+        <v>37955</v>
       </c>
       <c r="H1" t="s">
-        <v>37596</v>
+        <v>37956</v>
       </c>
       <c r="I1" t="s">
-        <v>37620</v>
+        <v>37980</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>37489</v>
+        <v>37849</v>
       </c>
       <c r="B2" t="s">
-        <v>37513</v>
+        <v>37873</v>
       </c>
       <c r="C2" t="s">
-        <v>37577</v>
+        <v>37937</v>
       </c>
       <c r="D2" s="1">
         <v>0.5899999737739563</v>
@@ -113656,21 +114736,21 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" t="s">
-        <v>37597</v>
+        <v>37957</v>
       </c>
       <c r="I2" t="s">
-        <v>37621</v>
+        <v>37981</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>37489</v>
+        <v>37849</v>
       </c>
       <c r="B3" t="s">
-        <v>37514</v>
+        <v>37874</v>
       </c>
       <c r="C3" t="s">
-        <v>37577</v>
+        <v>37937</v>
       </c>
       <c r="D3" s="1">
         <v>0.5899999737739563</v>
@@ -113683,21 +114763,21 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" t="s">
-        <v>37597</v>
+        <v>37957</v>
       </c>
       <c r="I3" t="s">
-        <v>37622</v>
+        <v>37982</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>37490</v>
+        <v>37850</v>
       </c>
       <c r="B4" t="s">
-        <v>37515</v>
+        <v>37875</v>
       </c>
       <c r="C4" t="s">
-        <v>37577</v>
+        <v>37937</v>
       </c>
       <c r="D4" s="1">
         <v>0.41999998688697815</v>
@@ -113710,21 +114790,21 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" t="s">
-        <v>37598</v>
+        <v>37958</v>
       </c>
       <c r="I4" t="s">
-        <v>37623</v>
+        <v>37983</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>37490</v>
+        <v>37850</v>
       </c>
       <c r="B5" t="s">
-        <v>37516</v>
+        <v>37876</v>
       </c>
       <c r="C5" t="s">
-        <v>37577</v>
+        <v>37937</v>
       </c>
       <c r="D5" s="1">
         <v>0.38999998569488525</v>
@@ -113737,21 +114817,21 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" t="s">
-        <v>37598</v>
+        <v>37958</v>
       </c>
       <c r="I5" t="s">
-        <v>37624</v>
+        <v>37984</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>37490</v>
+        <v>37850</v>
       </c>
       <c r="B6" t="s">
-        <v>37517</v>
+        <v>37877</v>
       </c>
       <c r="C6" t="s">
-        <v>37577</v>
+        <v>37937</v>
       </c>
       <c r="D6" s="1">
         <v>0.47999998927116394</v>
@@ -113764,21 +114844,21 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" t="s">
-        <v>37598</v>
+        <v>37958</v>
       </c>
       <c r="I6" t="s">
-        <v>37625</v>
+        <v>37985</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>37490</v>
+        <v>37850</v>
       </c>
       <c r="B7" t="s">
-        <v>37518</v>
+        <v>37878</v>
       </c>
       <c r="C7" t="s">
-        <v>37577</v>
+        <v>37937</v>
       </c>
       <c r="D7" s="1">
         <v>0.74000000953674316</v>
@@ -113791,21 +114871,21 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" t="s">
-        <v>37598</v>
+        <v>37958</v>
       </c>
       <c r="I7" t="s">
-        <v>37626</v>
+        <v>37986</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>37491</v>
+        <v>37851</v>
       </c>
       <c r="B8" t="s">
-        <v>37519</v>
+        <v>37879</v>
       </c>
       <c r="C8" t="s">
-        <v>37577</v>
+        <v>37937</v>
       </c>
       <c r="D8" s="1">
         <v>0.68699997663497925</v>
@@ -113820,21 +114900,21 @@
         <v>0.015200000256299973</v>
       </c>
       <c r="H8" t="s">
-        <v>37599</v>
+        <v>37959</v>
       </c>
       <c r="I8" t="s">
-        <v>37627</v>
+        <v>37987</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>37491</v>
+        <v>37851</v>
       </c>
       <c r="B9" t="s">
-        <v>37520</v>
+        <v>37880</v>
       </c>
       <c r="C9" t="s">
-        <v>37577</v>
+        <v>37937</v>
       </c>
       <c r="D9" s="1">
         <v>0.91600000858306885</v>
@@ -113849,21 +114929,21 @@
         <v>0.48710000514984131</v>
       </c>
       <c r="H9" t="s">
-        <v>37600</v>
+        <v>37960</v>
       </c>
       <c r="I9" t="s">
-        <v>37628</v>
+        <v>37988</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>37492</v>
+        <v>37852</v>
       </c>
       <c r="B10" t="s">
-        <v>37521</v>
+        <v>37881</v>
       </c>
       <c r="C10" t="s">
-        <v>37577</v>
+        <v>37937</v>
       </c>
       <c r="D10" s="1">
         <v>0.44999998807907104</v>
@@ -113876,21 +114956,21 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" t="s">
-        <v>37601</v>
+        <v>37961</v>
       </c>
       <c r="I10" t="s">
-        <v>37629</v>
+        <v>37989</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>37492</v>
+        <v>37852</v>
       </c>
       <c r="B11" t="s">
-        <v>37522</v>
+        <v>37882</v>
       </c>
       <c r="C11" t="s">
-        <v>37577</v>
+        <v>37937</v>
       </c>
       <c r="D11" s="1">
         <v>0.60000002384185791</v>
@@ -113903,21 +114983,21 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" t="s">
-        <v>37601</v>
+        <v>37961</v>
       </c>
       <c r="I11" t="s">
-        <v>37630</v>
+        <v>37990</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>37493</v>
+        <v>37853</v>
       </c>
       <c r="B12" t="s">
-        <v>37522</v>
+        <v>37882</v>
       </c>
       <c r="C12" t="s">
-        <v>37577</v>
+        <v>37937</v>
       </c>
       <c r="D12" s="1">
         <v>0.55000001192092896</v>
@@ -113930,21 +115010,21 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" t="s">
-        <v>37602</v>
+        <v>37962</v>
       </c>
       <c r="I12" t="s">
-        <v>37631</v>
+        <v>37991</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>37493</v>
+        <v>37853</v>
       </c>
       <c r="B13" t="s">
-        <v>37523</v>
+        <v>37883</v>
       </c>
       <c r="C13" t="s">
-        <v>37577</v>
+        <v>37937</v>
       </c>
       <c r="D13" s="1">
         <v>0.50999999046325684</v>
@@ -113957,21 +115037,21 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" t="s">
-        <v>37602</v>
+        <v>37962</v>
       </c>
       <c r="I13" t="s">
-        <v>37632</v>
+        <v>37992</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>37494</v>
+        <v>37854</v>
       </c>
       <c r="B14" t="s">
-        <v>37524</v>
+        <v>37884</v>
       </c>
       <c r="C14" t="s">
-        <v>37577</v>
+        <v>37937</v>
       </c>
       <c r="D14" s="1">
         <v>0.76999998092651367</v>
@@ -113984,21 +115064,21 @@
       </c>
       <c r="G14" s="1"/>
       <c r="H14" t="s">
-        <v>37603</v>
+        <v>37963</v>
       </c>
       <c r="I14" t="s">
-        <v>37633</v>
+        <v>37993</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>37494</v>
+        <v>37854</v>
       </c>
       <c r="B15" t="s">
-        <v>37525</v>
+        <v>37885</v>
       </c>
       <c r="C15" t="s">
-        <v>37577</v>
+        <v>37937</v>
       </c>
       <c r="D15" s="1">
         <v>0.68000000715255737</v>
@@ -114011,21 +115091,21 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15" t="s">
-        <v>37603</v>
+        <v>37963</v>
       </c>
       <c r="I15" t="s">
-        <v>37634</v>
+        <v>37994</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>37495</v>
+        <v>37855</v>
       </c>
       <c r="B16" t="s">
-        <v>37526</v>
+        <v>37886</v>
       </c>
       <c r="C16" t="s">
-        <v>37578</v>
+        <v>37938</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
@@ -114038,21 +115118,21 @@
       </c>
       <c r="G16" s="1"/>
       <c r="H16" t="s">
-        <v>37603</v>
+        <v>37963</v>
       </c>
       <c r="I16" t="s">
-        <v>37635</v>
+        <v>37995</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>37495</v>
+        <v>37855</v>
       </c>
       <c r="B17" t="s">
-        <v>37527</v>
+        <v>37887</v>
       </c>
       <c r="C17" t="s">
-        <v>37578</v>
+        <v>37938</v>
       </c>
       <c r="D17" s="1">
         <v>0.70999997854232788</v>
@@ -114065,21 +115145,21 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" t="s">
-        <v>37603</v>
+        <v>37963</v>
       </c>
       <c r="I17" t="s">
-        <v>37636</v>
+        <v>37996</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>37496</v>
+        <v>37856</v>
       </c>
       <c r="B18" t="s">
-        <v>37528</v>
+        <v>37888</v>
       </c>
       <c r="C18" t="s">
-        <v>37579</v>
+        <v>37939</v>
       </c>
       <c r="D18" s="1">
         <v>0.69999998807907104</v>
@@ -114092,21 +115172,21 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" t="s">
-        <v>37604</v>
+        <v>37964</v>
       </c>
       <c r="I18" t="s">
-        <v>37637</v>
+        <v>37997</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>37496</v>
+        <v>37856</v>
       </c>
       <c r="B19" t="s">
-        <v>37529</v>
+        <v>37889</v>
       </c>
       <c r="C19" t="s">
-        <v>37579</v>
+        <v>37939</v>
       </c>
       <c r="D19" s="1">
         <v>0.6600000262260437</v>
@@ -114119,21 +115199,21 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19" t="s">
-        <v>37604</v>
+        <v>37964</v>
       </c>
       <c r="I19" t="s">
-        <v>37638</v>
+        <v>37998</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>37496</v>
+        <v>37856</v>
       </c>
       <c r="B20" t="s">
-        <v>37530</v>
+        <v>37890</v>
       </c>
       <c r="C20" t="s">
-        <v>37579</v>
+        <v>37939</v>
       </c>
       <c r="D20" s="1">
         <v>0.40000000596046448</v>
@@ -114146,21 +115226,21 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" t="s">
-        <v>37604</v>
+        <v>37964</v>
       </c>
       <c r="I20" t="s">
-        <v>37639</v>
+        <v>37999</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>37497</v>
+        <v>37857</v>
       </c>
       <c r="B21" t="s">
-        <v>37531</v>
+        <v>37891</v>
       </c>
       <c r="C21" t="s">
-        <v>37579</v>
+        <v>37939</v>
       </c>
       <c r="D21" s="1">
         <v>0.62999999523162842</v>
@@ -114173,21 +115253,21 @@
       </c>
       <c r="G21" s="1"/>
       <c r="H21" t="s">
-        <v>37605</v>
+        <v>37965</v>
       </c>
       <c r="I21" t="s">
-        <v>37640</v>
+        <v>38000</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>37497</v>
+        <v>37857</v>
       </c>
       <c r="B22" t="s">
-        <v>37532</v>
+        <v>37892</v>
       </c>
       <c r="C22" t="s">
-        <v>37579</v>
+        <v>37939</v>
       </c>
       <c r="D22" s="1">
         <v>0.64999997615814209</v>
@@ -114200,21 +115280,21 @@
       </c>
       <c r="G22" s="1"/>
       <c r="H22" t="s">
-        <v>37605</v>
+        <v>37965</v>
       </c>
       <c r="I22" t="s">
-        <v>37641</v>
+        <v>38001</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>37497</v>
+        <v>37857</v>
       </c>
       <c r="B23" t="s">
-        <v>37533</v>
+        <v>37893</v>
       </c>
       <c r="C23" t="s">
-        <v>37579</v>
+        <v>37939</v>
       </c>
       <c r="D23" s="1">
         <v>0.81999999284744263</v>
@@ -114227,21 +115307,21 @@
       </c>
       <c r="G23" s="1"/>
       <c r="H23" t="s">
-        <v>37605</v>
+        <v>37965</v>
       </c>
       <c r="I23" t="s">
-        <v>37642</v>
+        <v>38002</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>37498</v>
+        <v>37858</v>
       </c>
       <c r="B24" t="s">
-        <v>37534</v>
+        <v>37894</v>
       </c>
       <c r="C24" t="s">
-        <v>37579</v>
+        <v>37939</v>
       </c>
       <c r="D24" s="1">
         <v>0.84700000286102295</v>
@@ -114254,21 +115334,21 @@
       </c>
       <c r="G24" s="1"/>
       <c r="H24" t="s">
-        <v>37606</v>
+        <v>37966</v>
       </c>
       <c r="I24" t="s">
-        <v>37643</v>
+        <v>38003</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>37498</v>
+        <v>37858</v>
       </c>
       <c r="B25" t="s">
-        <v>37535</v>
+        <v>37895</v>
       </c>
       <c r="C25" t="s">
-        <v>37579</v>
+        <v>37939</v>
       </c>
       <c r="D25" s="1">
         <v>0.37000000476837158</v>
@@ -114281,21 +115361,21 @@
       </c>
       <c r="G25" s="1"/>
       <c r="H25" t="s">
-        <v>37606</v>
+        <v>37966</v>
       </c>
       <c r="I25" t="s">
-        <v>37644</v>
+        <v>38004</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>37498</v>
+        <v>37858</v>
       </c>
       <c r="B26" t="s">
-        <v>37536</v>
+        <v>37896</v>
       </c>
       <c r="C26" t="s">
-        <v>37579</v>
+        <v>37939</v>
       </c>
       <c r="D26" s="1">
         <v>0.70200002193450928</v>
@@ -114308,21 +115388,21 @@
       </c>
       <c r="G26" s="1"/>
       <c r="H26" t="s">
-        <v>37606</v>
+        <v>37966</v>
       </c>
       <c r="I26" t="s">
-        <v>37645</v>
+        <v>38005</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>37498</v>
+        <v>37858</v>
       </c>
       <c r="B27" t="s">
-        <v>37537</v>
+        <v>37897</v>
       </c>
       <c r="C27" t="s">
-        <v>37580</v>
+        <v>37940</v>
       </c>
       <c r="D27" s="1">
         <v>0.52100002765655518</v>
@@ -114335,21 +115415,21 @@
       </c>
       <c r="G27" s="1"/>
       <c r="H27" t="s">
-        <v>37607</v>
+        <v>37967</v>
       </c>
       <c r="I27" t="s">
-        <v>37646</v>
+        <v>38006</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>37498</v>
+        <v>37858</v>
       </c>
       <c r="B28" t="s">
-        <v>37538</v>
+        <v>37898</v>
       </c>
       <c r="C28" t="s">
-        <v>37580</v>
+        <v>37940</v>
       </c>
       <c r="D28" s="1">
         <v>0.38600000739097595</v>
@@ -114362,21 +115442,21 @@
       </c>
       <c r="G28" s="1"/>
       <c r="H28" t="s">
-        <v>37607</v>
+        <v>37967</v>
       </c>
       <c r="I28" t="s">
-        <v>37647</v>
+        <v>38007</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>37498</v>
+        <v>37858</v>
       </c>
       <c r="B29" t="s">
-        <v>37539</v>
+        <v>37899</v>
       </c>
       <c r="C29" t="s">
-        <v>37580</v>
+        <v>37940</v>
       </c>
       <c r="D29" s="1">
         <v>0.335999995470047</v>
@@ -114389,75 +115469,75 @@
       </c>
       <c r="G29" s="1"/>
       <c r="H29" t="s">
-        <v>37607</v>
+        <v>37967</v>
       </c>
       <c r="I29" t="s">
-        <v>37648</v>
+        <v>38008</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>37499</v>
+        <v>37859</v>
       </c>
       <c r="B30" t="s">
-        <v>37540</v>
+        <v>37900</v>
       </c>
       <c r="C30" t="s">
-        <v>37581</v>
+        <v>37941</v>
       </c>
       <c r="D30" s="1">
-        <v>0.74000000953674316</v>
+        <v>0.68000000715255737</v>
       </c>
       <c r="E30" s="1">
-        <v>0.47999998927116394</v>
+        <v>0.41999998688697815</v>
       </c>
       <c r="F30" s="1">
-        <v>1.1299999952316284</v>
+        <v>1.0900000333786011</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" t="s">
-        <v>37608</v>
+        <v>37968</v>
       </c>
       <c r="I30" t="s">
-        <v>37649</v>
+        <v>38009</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>37499</v>
+        <v>37859</v>
       </c>
       <c r="B31" t="s">
-        <v>37541</v>
+        <v>37901</v>
       </c>
       <c r="C31" t="s">
-        <v>37581</v>
+        <v>37941</v>
       </c>
       <c r="D31" s="1">
-        <v>0.75999999046325684</v>
+        <v>0.72000002861022949</v>
       </c>
       <c r="E31" s="1">
-        <v>0.43000000715255737</v>
+        <v>0.38999998569488525</v>
       </c>
       <c r="F31" s="1">
         <v>1.3500000238418579</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" t="s">
-        <v>37608</v>
+        <v>37968</v>
       </c>
       <c r="I31" t="s">
-        <v>37650</v>
+        <v>38010</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>37500</v>
+        <v>37860</v>
       </c>
       <c r="B32" t="s">
-        <v>37542</v>
+        <v>37902</v>
       </c>
       <c r="C32" t="s">
-        <v>37581</v>
+        <v>37941</v>
       </c>
       <c r="D32" s="1">
         <v>0.75</v>
@@ -114470,21 +115550,21 @@
       </c>
       <c r="G32" s="1"/>
       <c r="H32" t="s">
-        <v>37609</v>
+        <v>37969</v>
       </c>
       <c r="I32" t="s">
-        <v>37651</v>
+        <v>38011</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>37500</v>
+        <v>37860</v>
       </c>
       <c r="B33" t="s">
-        <v>37543</v>
+        <v>37903</v>
       </c>
       <c r="C33" t="s">
-        <v>37581</v>
+        <v>37941</v>
       </c>
       <c r="D33" s="1">
         <v>0.54000002145767212</v>
@@ -114497,21 +115577,21 @@
       </c>
       <c r="G33" s="1"/>
       <c r="H33" t="s">
-        <v>37609</v>
+        <v>37969</v>
       </c>
       <c r="I33" t="s">
-        <v>37652</v>
+        <v>38012</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>37500</v>
+        <v>37860</v>
       </c>
       <c r="B34" t="s">
-        <v>37544</v>
+        <v>37904</v>
       </c>
       <c r="C34" t="s">
-        <v>37582</v>
+        <v>37942</v>
       </c>
       <c r="D34" s="1">
         <v>1.6699999570846558</v>
@@ -114524,21 +115604,21 @@
       </c>
       <c r="G34" s="1"/>
       <c r="H34" t="s">
-        <v>37610</v>
+        <v>37970</v>
       </c>
       <c r="I34" t="s">
-        <v>37653</v>
+        <v>38013</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>37500</v>
+        <v>37860</v>
       </c>
       <c r="B35" t="s">
-        <v>37545</v>
+        <v>37905</v>
       </c>
       <c r="C35" t="s">
-        <v>37582</v>
+        <v>37942</v>
       </c>
       <c r="D35" s="1">
         <v>2.3299999237060547</v>
@@ -114551,21 +115631,21 @@
       </c>
       <c r="G35" s="1"/>
       <c r="H35" t="s">
-        <v>37610</v>
+        <v>37970</v>
       </c>
       <c r="I35" t="s">
-        <v>37654</v>
+        <v>38014</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>37501</v>
+        <v>37861</v>
       </c>
       <c r="B36" t="s">
-        <v>37546</v>
+        <v>37906</v>
       </c>
       <c r="C36" t="s">
-        <v>37583</v>
+        <v>37943</v>
       </c>
       <c r="D36" s="1">
         <v>0.15999999642372131</v>
@@ -114578,21 +115658,21 @@
       </c>
       <c r="G36" s="1"/>
       <c r="H36" t="s">
-        <v>37611</v>
+        <v>37971</v>
       </c>
       <c r="I36" t="s">
-        <v>37655</v>
+        <v>38015</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>37501</v>
+        <v>37861</v>
       </c>
       <c r="B37" t="s">
-        <v>37547</v>
+        <v>37907</v>
       </c>
       <c r="C37" t="s">
-        <v>37583</v>
+        <v>37943</v>
       </c>
       <c r="D37" s="1">
         <v>0.51999998092651367</v>
@@ -114605,21 +115685,21 @@
       </c>
       <c r="G37" s="1"/>
       <c r="H37" t="s">
-        <v>37611</v>
+        <v>37971</v>
       </c>
       <c r="I37" t="s">
-        <v>37656</v>
+        <v>38016</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>37501</v>
+        <v>37861</v>
       </c>
       <c r="B38" t="s">
-        <v>37548</v>
+        <v>37908</v>
       </c>
       <c r="C38" t="s">
-        <v>37583</v>
+        <v>37943</v>
       </c>
       <c r="D38" s="1">
         <v>0.62999999523162842</v>
@@ -114632,21 +115712,21 @@
       </c>
       <c r="G38" s="1"/>
       <c r="H38" t="s">
-        <v>37611</v>
+        <v>37971</v>
       </c>
       <c r="I38" t="s">
-        <v>37657</v>
+        <v>38017</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>37501</v>
+        <v>37861</v>
       </c>
       <c r="B39" t="s">
-        <v>37549</v>
+        <v>37909</v>
       </c>
       <c r="C39" t="s">
-        <v>37583</v>
+        <v>37943</v>
       </c>
       <c r="D39" s="1">
         <v>0.25999999046325684</v>
@@ -114659,21 +115739,21 @@
       </c>
       <c r="G39" s="1"/>
       <c r="H39" t="s">
-        <v>37611</v>
+        <v>37971</v>
       </c>
       <c r="I39" t="s">
-        <v>37658</v>
+        <v>38018</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>37502</v>
+        <v>37862</v>
       </c>
       <c r="B40" t="s">
-        <v>37550</v>
+        <v>37910</v>
       </c>
       <c r="C40" t="s">
-        <v>37583</v>
+        <v>37943</v>
       </c>
       <c r="D40" s="1">
         <v>0.2199999988079071</v>
@@ -114686,21 +115766,21 @@
       </c>
       <c r="G40" s="1"/>
       <c r="H40" t="s">
-        <v>37611</v>
+        <v>37971</v>
       </c>
       <c r="I40" t="s">
-        <v>37659</v>
+        <v>38019</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>37502</v>
+        <v>37862</v>
       </c>
       <c r="B41" t="s">
-        <v>37551</v>
+        <v>37911</v>
       </c>
       <c r="C41" t="s">
-        <v>37583</v>
+        <v>37943</v>
       </c>
       <c r="D41" s="1">
         <v>0.46000000834465027</v>
@@ -114713,21 +115793,21 @@
       </c>
       <c r="G41" s="1"/>
       <c r="H41" t="s">
-        <v>37611</v>
+        <v>37971</v>
       </c>
       <c r="I41" t="s">
-        <v>37660</v>
+        <v>38020</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>37502</v>
+        <v>37862</v>
       </c>
       <c r="B42" t="s">
-        <v>37552</v>
+        <v>37912</v>
       </c>
       <c r="C42" t="s">
-        <v>37583</v>
+        <v>37943</v>
       </c>
       <c r="D42" s="1">
         <v>0.60000002384185791</v>
@@ -114740,21 +115820,21 @@
       </c>
       <c r="G42" s="1"/>
       <c r="H42" t="s">
-        <v>37611</v>
+        <v>37971</v>
       </c>
       <c r="I42" t="s">
-        <v>37661</v>
+        <v>38021</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>37502</v>
+        <v>37862</v>
       </c>
       <c r="B43" t="s">
-        <v>37553</v>
+        <v>37913</v>
       </c>
       <c r="C43" t="s">
-        <v>37583</v>
+        <v>37943</v>
       </c>
       <c r="D43" s="1">
         <v>0.37000000476837158</v>
@@ -114767,21 +115847,21 @@
       </c>
       <c r="G43" s="1"/>
       <c r="H43" t="s">
-        <v>37611</v>
+        <v>37971</v>
       </c>
       <c r="I43" t="s">
-        <v>37662</v>
+        <v>38022</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>37503</v>
+        <v>37863</v>
       </c>
       <c r="B44" t="s">
-        <v>37554</v>
+        <v>37914</v>
       </c>
       <c r="C44" t="s">
-        <v>37583</v>
+        <v>37943</v>
       </c>
       <c r="D44" s="1">
         <v>0.5899999737739563</v>
@@ -114794,21 +115874,21 @@
       </c>
       <c r="G44" s="1"/>
       <c r="H44" t="s">
-        <v>37612</v>
+        <v>37972</v>
       </c>
       <c r="I44" t="s">
-        <v>37663</v>
+        <v>38023</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>37503</v>
+        <v>37863</v>
       </c>
       <c r="B45" t="s">
-        <v>37555</v>
+        <v>37915</v>
       </c>
       <c r="C45" t="s">
-        <v>37583</v>
+        <v>37943</v>
       </c>
       <c r="D45" s="1">
         <v>0.47999998927116394</v>
@@ -114821,21 +115901,21 @@
       </c>
       <c r="G45" s="1"/>
       <c r="H45" t="s">
-        <v>37612</v>
+        <v>37972</v>
       </c>
       <c r="I45" t="s">
-        <v>37664</v>
+        <v>38024</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>37504</v>
+        <v>37864</v>
       </c>
       <c r="B46" t="s">
-        <v>37556</v>
+        <v>37916</v>
       </c>
       <c r="C46" t="s">
-        <v>37584</v>
+        <v>37944</v>
       </c>
       <c r="D46" s="1">
         <v>0.77100002765655518</v>
@@ -114848,21 +115928,21 @@
       </c>
       <c r="G46" s="1"/>
       <c r="H46" t="s">
-        <v>37612</v>
+        <v>37972</v>
       </c>
       <c r="I46" t="s">
-        <v>37665</v>
+        <v>38025</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>37504</v>
+        <v>37864</v>
       </c>
       <c r="B47" t="s">
-        <v>37557</v>
+        <v>37917</v>
       </c>
       <c r="C47" t="s">
-        <v>37584</v>
+        <v>37944</v>
       </c>
       <c r="D47" s="1">
         <v>0.75199997425079346</v>
@@ -114875,21 +115955,21 @@
       </c>
       <c r="G47" s="1"/>
       <c r="H47" t="s">
-        <v>37612</v>
+        <v>37972</v>
       </c>
       <c r="I47" t="s">
-        <v>37666</v>
+        <v>38026</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>37505</v>
+        <v>37865</v>
       </c>
       <c r="B48" t="s">
-        <v>37558</v>
+        <v>37918</v>
       </c>
       <c r="C48" t="s">
-        <v>37585</v>
+        <v>37945</v>
       </c>
       <c r="D48" s="1">
         <v>0.54000002145767212</v>
@@ -114902,21 +115982,21 @@
       </c>
       <c r="G48" s="1"/>
       <c r="H48" t="s">
-        <v>37612</v>
+        <v>37972</v>
       </c>
       <c r="I48" t="s">
-        <v>37667</v>
+        <v>38027</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>37505</v>
+        <v>37865</v>
       </c>
       <c r="B49" t="s">
-        <v>37559</v>
+        <v>37919</v>
       </c>
       <c r="C49" t="s">
-        <v>37585</v>
+        <v>37945</v>
       </c>
       <c r="D49" s="1">
         <v>0.67000001668930054</v>
@@ -114929,21 +116009,21 @@
       </c>
       <c r="G49" s="1"/>
       <c r="H49" t="s">
-        <v>37612</v>
+        <v>37972</v>
       </c>
       <c r="I49" t="s">
-        <v>37668</v>
+        <v>38028</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>37505</v>
+        <v>37865</v>
       </c>
       <c r="B50" t="s">
-        <v>37560</v>
+        <v>37920</v>
       </c>
       <c r="C50" t="s">
-        <v>37585</v>
+        <v>37945</v>
       </c>
       <c r="D50" s="1">
         <v>0.60000002384185791</v>
@@ -114956,21 +116036,21 @@
       </c>
       <c r="G50" s="1"/>
       <c r="H50" t="s">
-        <v>37612</v>
+        <v>37972</v>
       </c>
       <c r="I50" t="s">
-        <v>37669</v>
+        <v>38029</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>37506</v>
+        <v>37866</v>
       </c>
       <c r="B51" t="s">
-        <v>37561</v>
+        <v>37921</v>
       </c>
       <c r="C51" t="s">
-        <v>37586</v>
+        <v>37946</v>
       </c>
       <c r="D51" s="1">
         <v>0.97600001096725464</v>
@@ -114983,21 +116063,21 @@
       </c>
       <c r="G51" s="1"/>
       <c r="H51" t="s">
-        <v>37613</v>
+        <v>37973</v>
       </c>
       <c r="I51" t="s">
-        <v>37670</v>
+        <v>38030</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>37506</v>
+        <v>37866</v>
       </c>
       <c r="B52" t="s">
-        <v>37562</v>
+        <v>37922</v>
       </c>
       <c r="C52" t="s">
-        <v>37586</v>
+        <v>37946</v>
       </c>
       <c r="D52" s="1">
         <v>0.92599999904632568</v>
@@ -115010,21 +116090,21 @@
       </c>
       <c r="G52" s="1"/>
       <c r="H52" t="s">
-        <v>37613</v>
+        <v>37973</v>
       </c>
       <c r="I52" t="s">
-        <v>37671</v>
+        <v>38031</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>37506</v>
+        <v>37866</v>
       </c>
       <c r="B53" t="s">
-        <v>37563</v>
+        <v>37923</v>
       </c>
       <c r="C53" t="s">
-        <v>37586</v>
+        <v>37946</v>
       </c>
       <c r="D53" s="1">
         <v>0.88300001621246338</v>
@@ -115037,21 +116117,21 @@
       </c>
       <c r="G53" s="1"/>
       <c r="H53" t="s">
-        <v>37613</v>
+        <v>37973</v>
       </c>
       <c r="I53" t="s">
-        <v>37672</v>
+        <v>38032</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>37507</v>
+        <v>37867</v>
       </c>
       <c r="B54" t="s">
-        <v>37564</v>
+        <v>37924</v>
       </c>
       <c r="C54" t="s">
-        <v>37587</v>
+        <v>37947</v>
       </c>
       <c r="D54" s="1">
         <v>0.6600000262260437</v>
@@ -115064,21 +116144,21 @@
       </c>
       <c r="G54" s="1"/>
       <c r="H54" t="s">
-        <v>37614</v>
+        <v>37974</v>
       </c>
       <c r="I54" t="s">
-        <v>37673</v>
+        <v>38033</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>37507</v>
+        <v>37867</v>
       </c>
       <c r="B55" t="s">
-        <v>37565</v>
+        <v>37925</v>
       </c>
       <c r="C55" t="s">
-        <v>37587</v>
+        <v>37947</v>
       </c>
       <c r="D55" s="1">
         <v>0.63999998569488525</v>
@@ -115091,21 +116171,21 @@
       </c>
       <c r="G55" s="1"/>
       <c r="H55" t="s">
-        <v>37614</v>
+        <v>37974</v>
       </c>
       <c r="I55" t="s">
-        <v>37674</v>
+        <v>38034</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>37508</v>
+        <v>37868</v>
       </c>
       <c r="B56" t="s">
-        <v>37566</v>
+        <v>37926</v>
       </c>
       <c r="C56" t="s">
-        <v>37588</v>
+        <v>37948</v>
       </c>
       <c r="D56" s="1">
         <v>0.89999997615814209</v>
@@ -115118,21 +116198,21 @@
       </c>
       <c r="G56" s="1"/>
       <c r="H56" t="s">
-        <v>37615</v>
+        <v>37975</v>
       </c>
       <c r="I56" t="s">
-        <v>37675</v>
+        <v>38035</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>37508</v>
+        <v>37868</v>
       </c>
       <c r="B57" t="s">
-        <v>37567</v>
+        <v>37927</v>
       </c>
       <c r="C57" t="s">
-        <v>37588</v>
+        <v>37948</v>
       </c>
       <c r="D57" s="1">
         <v>0.95999997854232788</v>
@@ -115145,21 +116225,21 @@
       </c>
       <c r="G57" s="1"/>
       <c r="H57" t="s">
-        <v>37615</v>
+        <v>37975</v>
       </c>
       <c r="I57" t="s">
-        <v>37676</v>
+        <v>38036</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>37509</v>
+        <v>37869</v>
       </c>
       <c r="B58" t="s">
-        <v>37568</v>
+        <v>37928</v>
       </c>
       <c r="C58" t="s">
-        <v>37589</v>
+        <v>37949</v>
       </c>
       <c r="D58" s="1">
         <v>0.4699999988079071</v>
@@ -115172,21 +116252,21 @@
       </c>
       <c r="G58" s="1"/>
       <c r="H58" t="s">
-        <v>37616</v>
+        <v>37976</v>
       </c>
       <c r="I58" t="s">
-        <v>37677</v>
+        <v>38037</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>37509</v>
+        <v>37869</v>
       </c>
       <c r="B59" t="s">
-        <v>37569</v>
+        <v>37929</v>
       </c>
       <c r="C59" t="s">
-        <v>37589</v>
+        <v>37949</v>
       </c>
       <c r="D59" s="1">
         <v>0.47999998927116394</v>
@@ -115199,21 +116279,21 @@
       </c>
       <c r="G59" s="1"/>
       <c r="H59" t="s">
-        <v>37616</v>
+        <v>37976</v>
       </c>
       <c r="I59" t="s">
-        <v>37678</v>
+        <v>38038</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>37509</v>
+        <v>37869</v>
       </c>
       <c r="B60" t="s">
-        <v>37570</v>
+        <v>37930</v>
       </c>
       <c r="C60" t="s">
-        <v>37590</v>
+        <v>37950</v>
       </c>
       <c r="D60" s="1">
         <v>0.43999999761581421</v>
@@ -115226,21 +116306,21 @@
       </c>
       <c r="G60" s="1"/>
       <c r="H60" t="s">
-        <v>37617</v>
+        <v>37977</v>
       </c>
       <c r="I60" t="s">
-        <v>37679</v>
+        <v>38039</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>37509</v>
+        <v>37869</v>
       </c>
       <c r="B61" t="s">
-        <v>37571</v>
+        <v>37931</v>
       </c>
       <c r="C61" t="s">
-        <v>37590</v>
+        <v>37950</v>
       </c>
       <c r="D61" s="1">
         <v>0.75999999046325684</v>
@@ -115253,21 +116333,21 @@
       </c>
       <c r="G61" s="1"/>
       <c r="H61" t="s">
-        <v>37617</v>
+        <v>37977</v>
       </c>
       <c r="I61" t="s">
-        <v>37680</v>
+        <v>38040</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>37510</v>
+        <v>37870</v>
       </c>
       <c r="B62" t="s">
-        <v>37572</v>
+        <v>37932</v>
       </c>
       <c r="C62" t="s">
-        <v>37590</v>
+        <v>37950</v>
       </c>
       <c r="D62" s="1">
         <v>0.81000000238418579</v>
@@ -115280,21 +116360,21 @@
       </c>
       <c r="G62" s="1"/>
       <c r="H62" t="s">
-        <v>37618</v>
+        <v>37978</v>
       </c>
       <c r="I62" t="s">
-        <v>37681</v>
+        <v>38041</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>37510</v>
+        <v>37870</v>
       </c>
       <c r="B63" t="s">
-        <v>37573</v>
+        <v>37933</v>
       </c>
       <c r="C63" t="s">
-        <v>37590</v>
+        <v>37950</v>
       </c>
       <c r="D63" s="1">
         <v>0.79000002145767212</v>
@@ -115307,21 +116387,21 @@
       </c>
       <c r="G63" s="1"/>
       <c r="H63" t="s">
-        <v>37618</v>
+        <v>37978</v>
       </c>
       <c r="I63" t="s">
-        <v>37682</v>
+        <v>38042</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>37511</v>
+        <v>37871</v>
       </c>
       <c r="B64" t="s">
-        <v>37574</v>
+        <v>37934</v>
       </c>
       <c r="C64" t="s">
-        <v>37591</v>
+        <v>37951</v>
       </c>
       <c r="D64" s="1">
         <v>0.6600000262260437</v>
@@ -115334,21 +116414,21 @@
       </c>
       <c r="G64" s="1"/>
       <c r="H64" t="s">
-        <v>37619</v>
+        <v>37979</v>
       </c>
       <c r="I64" t="s">
-        <v>37683</v>
+        <v>38043</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>37511</v>
+        <v>37871</v>
       </c>
       <c r="B65" t="s">
-        <v>37575</v>
+        <v>37935</v>
       </c>
       <c r="C65" t="s">
-        <v>37591</v>
+        <v>37951</v>
       </c>
       <c r="D65" s="1">
         <v>0.55000001192092896</v>
@@ -115361,10 +116441,10 @@
       </c>
       <c r="G65" s="1"/>
       <c r="H65" t="s">
-        <v>37619</v>
+        <v>37979</v>
       </c>
       <c r="I65" t="s">
-        <v>37684</v>
+        <v>38044</v>
       </c>
     </row>
   </sheetData>
@@ -115378,42 +116458,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>37685</v>
+        <v>38045</v>
       </c>
       <c r="B1" t="s">
-        <v>37707</v>
+        <v>38067</v>
       </c>
       <c r="C1" t="s">
-        <v>37754</v>
+        <v>38114</v>
       </c>
       <c r="D1" t="s">
-        <v>37764</v>
+        <v>38124</v>
       </c>
       <c r="E1" t="s">
-        <v>37765</v>
+        <v>38125</v>
       </c>
       <c r="F1" t="s">
-        <v>37766</v>
+        <v>38126</v>
       </c>
       <c r="G1" t="s">
-        <v>37767</v>
+        <v>38127</v>
       </c>
       <c r="H1" t="s">
-        <v>37779</v>
+        <v>38139</v>
       </c>
       <c r="I1" t="s">
-        <v>37800</v>
+        <v>38160</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>37686</v>
+        <v>38046</v>
       </c>
       <c r="B2" t="s">
-        <v>37708</v>
+        <v>38068</v>
       </c>
       <c r="C2" t="s">
-        <v>37755</v>
+        <v>38115</v>
       </c>
       <c r="D2" s="1">
         <v>0.5899999737739563</v>
@@ -115425,24 +116505,24 @@
         <v>0.81999999284744263</v>
       </c>
       <c r="G2" t="s">
-        <v>37768</v>
+        <v>38128</v>
       </c>
       <c r="H2" t="s">
-        <v>37780</v>
+        <v>38140</v>
       </c>
       <c r="I2" t="s">
-        <v>37801</v>
+        <v>38161</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>37686</v>
+        <v>38046</v>
       </c>
       <c r="B3" t="s">
-        <v>37709</v>
+        <v>38069</v>
       </c>
       <c r="C3" t="s">
-        <v>37755</v>
+        <v>38115</v>
       </c>
       <c r="D3" s="1">
         <v>0.18000000715255737</v>
@@ -115454,24 +116534,24 @@
         <v>1.4900000095367432</v>
       </c>
       <c r="G3" t="s">
-        <v>37768</v>
+        <v>38128</v>
       </c>
       <c r="H3" t="s">
-        <v>37780</v>
+        <v>38140</v>
       </c>
       <c r="I3" t="s">
-        <v>37802</v>
+        <v>38162</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>37687</v>
+        <v>38047</v>
       </c>
       <c r="B4" t="s">
-        <v>37710</v>
+        <v>38070</v>
       </c>
       <c r="C4" t="s">
-        <v>37755</v>
+        <v>38115</v>
       </c>
       <c r="D4" s="1">
         <v>0.37999999523162842</v>
@@ -115483,24 +116563,24 @@
         <v>0.6600000262260437</v>
       </c>
       <c r="G4" t="s">
-        <v>37768</v>
+        <v>38128</v>
       </c>
       <c r="H4" t="s">
-        <v>37781</v>
+        <v>38141</v>
       </c>
       <c r="I4" t="s">
-        <v>37803</v>
+        <v>38163</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>37687</v>
+        <v>38047</v>
       </c>
       <c r="B5" t="s">
-        <v>37711</v>
+        <v>38071</v>
       </c>
       <c r="C5" t="s">
-        <v>37755</v>
+        <v>38115</v>
       </c>
       <c r="D5" s="1">
         <v>0.44999998807907104</v>
@@ -115512,24 +116592,24 @@
         <v>0.57999998331069946</v>
       </c>
       <c r="G5" t="s">
-        <v>37768</v>
+        <v>38128</v>
       </c>
       <c r="H5" t="s">
-        <v>37781</v>
+        <v>38141</v>
       </c>
       <c r="I5" t="s">
-        <v>37804</v>
+        <v>38164</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>37688</v>
+        <v>38048</v>
       </c>
       <c r="B6" t="s">
-        <v>37712</v>
+        <v>38072</v>
       </c>
       <c r="C6" t="s">
-        <v>37755</v>
+        <v>38115</v>
       </c>
       <c r="D6" s="1">
         <v>0.75700002908706665</v>
@@ -115541,24 +116621,24 @@
         <v>0.96299999952316284</v>
       </c>
       <c r="G6" t="s">
-        <v>37769</v>
+        <v>38129</v>
       </c>
       <c r="H6" t="s">
-        <v>37782</v>
+        <v>38142</v>
       </c>
       <c r="I6" t="s">
-        <v>37805</v>
+        <v>38165</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>37688</v>
+        <v>38048</v>
       </c>
       <c r="B7" t="s">
-        <v>37713</v>
+        <v>38073</v>
       </c>
       <c r="C7" t="s">
-        <v>37755</v>
+        <v>38115</v>
       </c>
       <c r="D7" s="1">
         <v>0.92599999904632568</v>
@@ -115570,24 +116650,24 @@
         <v>1.2790000438690186</v>
       </c>
       <c r="G7" t="s">
-        <v>37770</v>
+        <v>38130</v>
       </c>
       <c r="H7" t="s">
-        <v>37782</v>
+        <v>38142</v>
       </c>
       <c r="I7" t="s">
-        <v>37806</v>
+        <v>38166</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>37689</v>
+        <v>38049</v>
       </c>
       <c r="B8" t="s">
-        <v>37714</v>
+        <v>38074</v>
       </c>
       <c r="C8" t="s">
-        <v>37755</v>
+        <v>38115</v>
       </c>
       <c r="D8" s="1">
         <v>0.43999999761581421</v>
@@ -115599,24 +116679,24 @@
         <v>0.56000000238418579</v>
       </c>
       <c r="G8" t="s">
-        <v>37771</v>
+        <v>38131</v>
       </c>
       <c r="H8" t="s">
-        <v>37783</v>
+        <v>38143</v>
       </c>
       <c r="I8" t="s">
-        <v>37807</v>
+        <v>38167</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>37689</v>
+        <v>38049</v>
       </c>
       <c r="B9" t="s">
-        <v>37715</v>
+        <v>38075</v>
       </c>
       <c r="C9" t="s">
-        <v>37755</v>
+        <v>38115</v>
       </c>
       <c r="D9" s="1">
         <v>0.80000001192092896</v>
@@ -115628,24 +116708,24 @@
         <v>1.1100000143051147</v>
       </c>
       <c r="G9" t="s">
-        <v>37771</v>
+        <v>38131</v>
       </c>
       <c r="H9" t="s">
-        <v>37783</v>
+        <v>38143</v>
       </c>
       <c r="I9" t="s">
-        <v>37808</v>
+        <v>38168</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>37690</v>
+        <v>38050</v>
       </c>
       <c r="B10" t="s">
-        <v>37716</v>
+        <v>38076</v>
       </c>
       <c r="C10" t="s">
-        <v>37755</v>
+        <v>38115</v>
       </c>
       <c r="D10" s="1">
         <v>0.56000000238418579</v>
@@ -115657,24 +116737,24 @@
         <v>0.97000002861022949</v>
       </c>
       <c r="G10" t="s">
-        <v>37771</v>
+        <v>38131</v>
       </c>
       <c r="H10" t="s">
-        <v>37784</v>
+        <v>38144</v>
       </c>
       <c r="I10" t="s">
-        <v>37809</v>
+        <v>38169</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>37690</v>
+        <v>38050</v>
       </c>
       <c r="B11" t="s">
-        <v>37717</v>
+        <v>38077</v>
       </c>
       <c r="C11" t="s">
-        <v>37755</v>
+        <v>38115</v>
       </c>
       <c r="D11" s="1">
         <v>0.50999999046325684</v>
@@ -115686,24 +116766,24 @@
         <v>1.190000057220459</v>
       </c>
       <c r="G11" t="s">
-        <v>37771</v>
+        <v>38131</v>
       </c>
       <c r="H11" t="s">
-        <v>37784</v>
+        <v>38144</v>
       </c>
       <c r="I11" t="s">
-        <v>37810</v>
+        <v>38170</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>37691</v>
+        <v>38051</v>
       </c>
       <c r="B12" t="s">
-        <v>37718</v>
+        <v>38078</v>
       </c>
       <c r="C12" t="s">
-        <v>37755</v>
+        <v>38115</v>
       </c>
       <c r="D12" s="1">
         <v>0.6600000262260437</v>
@@ -115715,24 +116795,24 @@
         <v>0.89999997615814209</v>
       </c>
       <c r="G12" t="s">
-        <v>37771</v>
+        <v>38131</v>
       </c>
       <c r="H12" t="s">
-        <v>37785</v>
+        <v>38145</v>
       </c>
       <c r="I12" t="s">
-        <v>37811</v>
+        <v>38171</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>37691</v>
+        <v>38051</v>
       </c>
       <c r="B13" t="s">
-        <v>37719</v>
+        <v>38079</v>
       </c>
       <c r="C13" t="s">
-        <v>37755</v>
+        <v>38115</v>
       </c>
       <c r="D13" s="1">
         <v>0.36000001430511475</v>
@@ -115744,24 +116824,24 @@
         <v>0.82999998331069946</v>
       </c>
       <c r="G13" t="s">
-        <v>37771</v>
+        <v>38131</v>
       </c>
       <c r="H13" t="s">
-        <v>37785</v>
+        <v>38145</v>
       </c>
       <c r="I13" t="s">
-        <v>37812</v>
+        <v>38172</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>37692</v>
+        <v>38052</v>
       </c>
       <c r="B14" t="s">
-        <v>37720</v>
+        <v>38080</v>
       </c>
       <c r="C14" t="s">
-        <v>37755</v>
+        <v>38115</v>
       </c>
       <c r="D14" s="1">
         <v>0.55299997329711914</v>
@@ -115773,24 +116853,24 @@
         <v>0.9309999942779541</v>
       </c>
       <c r="G14" t="s">
-        <v>37772</v>
+        <v>38132</v>
       </c>
       <c r="H14" t="s">
-        <v>37786</v>
+        <v>38146</v>
       </c>
       <c r="I14" t="s">
-        <v>37813</v>
+        <v>38173</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>37692</v>
+        <v>38052</v>
       </c>
       <c r="B15" t="s">
-        <v>37721</v>
+        <v>38081</v>
       </c>
       <c r="C15" t="s">
-        <v>37755</v>
+        <v>38115</v>
       </c>
       <c r="D15" s="1">
         <v>0.76599997282028198</v>
@@ -115802,24 +116882,24 @@
         <v>3.9639999866485596</v>
       </c>
       <c r="G15" t="s">
-        <v>37772</v>
+        <v>38132</v>
       </c>
       <c r="H15" t="s">
-        <v>37786</v>
+        <v>38146</v>
       </c>
       <c r="I15" t="s">
-        <v>37814</v>
+        <v>38174</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>37692</v>
+        <v>38052</v>
       </c>
       <c r="B16" t="s">
-        <v>37722</v>
+        <v>38082</v>
       </c>
       <c r="C16" t="s">
-        <v>37756</v>
+        <v>38116</v>
       </c>
       <c r="D16" s="1">
         <v>0.39800000190734863</v>
@@ -115831,24 +116911,24 @@
         <v>0.71899998188018799</v>
       </c>
       <c r="G16" t="s">
-        <v>37772</v>
+        <v>38132</v>
       </c>
       <c r="H16" t="s">
-        <v>37787</v>
+        <v>38147</v>
       </c>
       <c r="I16" t="s">
-        <v>37815</v>
+        <v>38175</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>37692</v>
+        <v>38052</v>
       </c>
       <c r="B17" t="s">
-        <v>37723</v>
+        <v>38083</v>
       </c>
       <c r="C17" t="s">
-        <v>37756</v>
+        <v>38116</v>
       </c>
       <c r="D17" s="1">
         <v>0.49799999594688416</v>
@@ -115860,24 +116940,24 @@
         <v>2.4030001163482666</v>
       </c>
       <c r="G17" t="s">
-        <v>37772</v>
+        <v>38132</v>
       </c>
       <c r="H17" t="s">
-        <v>37787</v>
+        <v>38147</v>
       </c>
       <c r="I17" t="s">
-        <v>37816</v>
+        <v>38176</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>37693</v>
+        <v>38053</v>
       </c>
       <c r="B18" t="s">
-        <v>37724</v>
+        <v>38084</v>
       </c>
       <c r="C18" t="s">
-        <v>37757</v>
+        <v>38117</v>
       </c>
       <c r="D18" s="1">
         <v>0.87000000476837158</v>
@@ -115889,24 +116969,24 @@
         <v>1.2899999618530273</v>
       </c>
       <c r="G18" t="s">
-        <v>37773</v>
+        <v>38133</v>
       </c>
       <c r="H18" t="s">
-        <v>37788</v>
+        <v>38148</v>
       </c>
       <c r="I18" t="s">
-        <v>37817</v>
+        <v>38177</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>37693</v>
+        <v>38053</v>
       </c>
       <c r="B19" t="s">
-        <v>37725</v>
+        <v>38085</v>
       </c>
       <c r="C19" t="s">
-        <v>37757</v>
+        <v>38117</v>
       </c>
       <c r="D19" s="1">
         <v>0.38999998569488525</v>
@@ -115918,24 +116998,24 @@
         <v>0.80000001192092896</v>
       </c>
       <c r="G19" t="s">
-        <v>37773</v>
+        <v>38133</v>
       </c>
       <c r="H19" t="s">
-        <v>37788</v>
+        <v>38148</v>
       </c>
       <c r="I19" t="s">
-        <v>37818</v>
+        <v>38178</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>37694</v>
+        <v>38054</v>
       </c>
       <c r="B20" t="s">
-        <v>37726</v>
+        <v>38086</v>
       </c>
       <c r="C20" t="s">
-        <v>37757</v>
+        <v>38117</v>
       </c>
       <c r="D20" s="1">
         <v>0.61000001430511475</v>
@@ -115947,24 +117027,24 @@
         <v>1.1699999570846558</v>
       </c>
       <c r="G20" t="s">
-        <v>37773</v>
+        <v>38133</v>
       </c>
       <c r="H20" t="s">
-        <v>37789</v>
+        <v>38149</v>
       </c>
       <c r="I20" t="s">
-        <v>37819</v>
+        <v>38179</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>37694</v>
+        <v>38054</v>
       </c>
       <c r="B21" t="s">
-        <v>37727</v>
+        <v>38087</v>
       </c>
       <c r="C21" t="s">
-        <v>37757</v>
+        <v>38117</v>
       </c>
       <c r="D21" s="1">
         <v>0.75</v>
@@ -115976,24 +117056,24 @@
         <v>1.3600000143051147</v>
       </c>
       <c r="G21" t="s">
-        <v>37773</v>
+        <v>38133</v>
       </c>
       <c r="H21" t="s">
-        <v>37789</v>
+        <v>38149</v>
       </c>
       <c r="I21" t="s">
-        <v>37820</v>
+        <v>38180</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>37694</v>
+        <v>38054</v>
       </c>
       <c r="B22" t="s">
-        <v>37728</v>
+        <v>38088</v>
       </c>
       <c r="C22" t="s">
-        <v>37758</v>
+        <v>38118</v>
       </c>
       <c r="D22" s="1">
         <v>5.9000000953674316</v>
@@ -116005,24 +117085,24 @@
         <v>46.099998474121094</v>
       </c>
       <c r="G22" t="s">
-        <v>37773</v>
+        <v>38133</v>
       </c>
       <c r="H22" t="s">
-        <v>37790</v>
+        <v>38150</v>
       </c>
       <c r="I22" t="s">
-        <v>37821</v>
+        <v>38181</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>37694</v>
+        <v>38054</v>
       </c>
       <c r="B23" t="s">
-        <v>37729</v>
+        <v>38089</v>
       </c>
       <c r="C23" t="s">
-        <v>37758</v>
+        <v>38118</v>
       </c>
       <c r="D23" s="1">
         <v>1.8200000524520874</v>
@@ -116034,24 +117114,24 @@
         <v>5.1399998664855957</v>
       </c>
       <c r="G23" t="s">
-        <v>37773</v>
+        <v>38133</v>
       </c>
       <c r="H23" t="s">
-        <v>37790</v>
+        <v>38150</v>
       </c>
       <c r="I23" t="s">
-        <v>37822</v>
+        <v>38182</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>37695</v>
+        <v>38055</v>
       </c>
       <c r="B24" t="s">
-        <v>37730</v>
+        <v>38090</v>
       </c>
       <c r="C24" t="s">
-        <v>37759</v>
+        <v>38119</v>
       </c>
       <c r="D24" s="1">
         <v>0.5899999737739563</v>
@@ -116063,24 +117143,24 @@
         <v>1.3999999761581421</v>
       </c>
       <c r="G24" t="s">
-        <v>37773</v>
+        <v>38133</v>
       </c>
       <c r="H24" t="s">
-        <v>37791</v>
+        <v>38151</v>
       </c>
       <c r="I24" t="s">
-        <v>37823</v>
+        <v>38183</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>37695</v>
+        <v>38055</v>
       </c>
       <c r="B25" t="s">
-        <v>37731</v>
+        <v>38091</v>
       </c>
       <c r="C25" t="s">
-        <v>37759</v>
+        <v>38119</v>
       </c>
       <c r="D25" s="1">
         <v>0.69999998807907104</v>
@@ -116092,24 +117172,24 @@
         <v>0.87000000476837158</v>
       </c>
       <c r="G25" t="s">
-        <v>37773</v>
+        <v>38133</v>
       </c>
       <c r="H25" t="s">
-        <v>37791</v>
+        <v>38151</v>
       </c>
       <c r="I25" t="s">
-        <v>37824</v>
+        <v>38184</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>37696</v>
+        <v>38056</v>
       </c>
       <c r="B26" t="s">
-        <v>37732</v>
+        <v>38092</v>
       </c>
       <c r="C26" t="s">
-        <v>37759</v>
+        <v>38119</v>
       </c>
       <c r="D26" s="1">
         <v>0.38999998569488525</v>
@@ -116121,24 +117201,24 @@
         <v>0.68999999761581421</v>
       </c>
       <c r="G26" t="s">
-        <v>37773</v>
+        <v>38133</v>
       </c>
       <c r="H26" t="s">
-        <v>37792</v>
+        <v>38152</v>
       </c>
       <c r="I26" t="s">
-        <v>37825</v>
+        <v>38185</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>37696</v>
+        <v>38056</v>
       </c>
       <c r="B27" t="s">
-        <v>37733</v>
+        <v>38093</v>
       </c>
       <c r="C27" t="s">
-        <v>37759</v>
+        <v>38119</v>
       </c>
       <c r="D27" s="1">
         <v>0.15999999642372131</v>
@@ -116150,24 +117230,24 @@
         <v>0.40000000596046448</v>
       </c>
       <c r="G27" t="s">
-        <v>37773</v>
+        <v>38133</v>
       </c>
       <c r="H27" t="s">
-        <v>37792</v>
+        <v>38152</v>
       </c>
       <c r="I27" t="s">
-        <v>37826</v>
+        <v>38186</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>37697</v>
+        <v>38057</v>
       </c>
       <c r="B28" t="s">
-        <v>37734</v>
+        <v>38094</v>
       </c>
       <c r="C28" t="s">
-        <v>37759</v>
+        <v>38119</v>
       </c>
       <c r="D28" s="1">
         <v>0.46000000834465027</v>
@@ -116179,24 +117259,24 @@
         <v>0.6600000262260437</v>
       </c>
       <c r="G28" t="s">
-        <v>37773</v>
+        <v>38133</v>
       </c>
       <c r="H28" t="s">
-        <v>37792</v>
+        <v>38152</v>
       </c>
       <c r="I28" t="s">
-        <v>37827</v>
+        <v>38187</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>37697</v>
+        <v>38057</v>
       </c>
       <c r="B29" t="s">
-        <v>37735</v>
+        <v>38095</v>
       </c>
       <c r="C29" t="s">
-        <v>37759</v>
+        <v>38119</v>
       </c>
       <c r="D29" s="1">
         <v>0.30000001192092896</v>
@@ -116208,24 +117288,24 @@
         <v>0.44999998807907104</v>
       </c>
       <c r="G29" t="s">
-        <v>37773</v>
+        <v>38133</v>
       </c>
       <c r="H29" t="s">
-        <v>37792</v>
+        <v>38152</v>
       </c>
       <c r="I29" t="s">
-        <v>37828</v>
+        <v>38188</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>37698</v>
+        <v>38058</v>
       </c>
       <c r="B30" t="s">
-        <v>37736</v>
+        <v>38096</v>
       </c>
       <c r="C30" t="s">
-        <v>37759</v>
+        <v>38119</v>
       </c>
       <c r="D30" s="1">
         <v>0.60000002384185791</v>
@@ -116237,24 +117317,24 @@
         <v>1.059999942779541</v>
       </c>
       <c r="G30" t="s">
-        <v>37773</v>
+        <v>38133</v>
       </c>
       <c r="H30" t="s">
-        <v>37793</v>
+        <v>38153</v>
       </c>
       <c r="I30" t="s">
-        <v>37829</v>
+        <v>38189</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>37698</v>
+        <v>38058</v>
       </c>
       <c r="B31" t="s">
-        <v>37737</v>
+        <v>38097</v>
       </c>
       <c r="C31" t="s">
-        <v>37759</v>
+        <v>38119</v>
       </c>
       <c r="D31" s="1">
         <v>0.47999998927116394</v>
@@ -116266,24 +117346,24 @@
         <v>0.81999999284744263</v>
       </c>
       <c r="G31" t="s">
-        <v>37773</v>
+        <v>38133</v>
       </c>
       <c r="H31" t="s">
-        <v>37793</v>
+        <v>38153</v>
       </c>
       <c r="I31" t="s">
-        <v>37830</v>
+        <v>38190</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>37699</v>
+        <v>38059</v>
       </c>
       <c r="B32" t="s">
-        <v>37738</v>
+        <v>38098</v>
       </c>
       <c r="C32" t="s">
-        <v>37759</v>
+        <v>38119</v>
       </c>
       <c r="D32" s="1">
         <v>1.6200000047683716</v>
@@ -116295,24 +117375,24 @@
         <v>2.4100000858306885</v>
       </c>
       <c r="G32" t="s">
-        <v>37773</v>
+        <v>38133</v>
       </c>
       <c r="H32" t="s">
-        <v>37793</v>
+        <v>38153</v>
       </c>
       <c r="I32" t="s">
-        <v>37831</v>
+        <v>38191</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>37699</v>
+        <v>38059</v>
       </c>
       <c r="B33" t="s">
-        <v>37739</v>
+        <v>38099</v>
       </c>
       <c r="C33" t="s">
-        <v>37759</v>
+        <v>38119</v>
       </c>
       <c r="D33" s="1">
         <v>2.0099999904632568</v>
@@ -116324,24 +117404,24 @@
         <v>2.8399999141693115</v>
       </c>
       <c r="G33" t="s">
-        <v>37773</v>
+        <v>38133</v>
       </c>
       <c r="H33" t="s">
-        <v>37793</v>
+        <v>38153</v>
       </c>
       <c r="I33" t="s">
-        <v>37832</v>
+        <v>38192</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>37700</v>
+        <v>38060</v>
       </c>
       <c r="B34" t="s">
-        <v>37740</v>
+        <v>38100</v>
       </c>
       <c r="C34" t="s">
-        <v>37760</v>
+        <v>38120</v>
       </c>
       <c r="D34" s="1">
         <v>0.95999997854232788</v>
@@ -116353,24 +117433,24 @@
         <v>1.2560000419616699</v>
       </c>
       <c r="G34" t="s">
-        <v>37774</v>
+        <v>38134</v>
       </c>
       <c r="H34" t="s">
-        <v>37794</v>
+        <v>38154</v>
       </c>
       <c r="I34" t="s">
-        <v>37833</v>
+        <v>38193</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>37700</v>
+        <v>38060</v>
       </c>
       <c r="B35" t="s">
-        <v>37741</v>
+        <v>38101</v>
       </c>
       <c r="C35" t="s">
-        <v>37760</v>
+        <v>38120</v>
       </c>
       <c r="D35" s="1">
         <v>1.0800000429153442</v>
@@ -116382,24 +117462,24 @@
         <v>1.3609999418258667</v>
       </c>
       <c r="G35" t="s">
-        <v>37774</v>
+        <v>38134</v>
       </c>
       <c r="H35" t="s">
-        <v>37794</v>
+        <v>38154</v>
       </c>
       <c r="I35" t="s">
-        <v>37834</v>
+        <v>38194</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>37701</v>
+        <v>38061</v>
       </c>
       <c r="B36" t="s">
-        <v>37742</v>
+        <v>38102</v>
       </c>
       <c r="C36" t="s">
-        <v>37760</v>
+        <v>38120</v>
       </c>
       <c r="D36" s="1">
         <v>0.87699997425079346</v>
@@ -116411,24 +117491,24 @@
         <v>1.156000018119812</v>
       </c>
       <c r="G36" t="s">
-        <v>37775</v>
+        <v>38135</v>
       </c>
       <c r="H36" t="s">
-        <v>37795</v>
+        <v>38155</v>
       </c>
       <c r="I36" t="s">
-        <v>37835</v>
+        <v>38195</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>37701</v>
+        <v>38061</v>
       </c>
       <c r="B37" t="s">
-        <v>37743</v>
+        <v>38103</v>
       </c>
       <c r="C37" t="s">
-        <v>37760</v>
+        <v>38120</v>
       </c>
       <c r="D37" s="1">
         <v>0.68400001525878906</v>
@@ -116440,24 +117520,24 @@
         <v>0.875</v>
       </c>
       <c r="G37" t="s">
-        <v>37775</v>
+        <v>38135</v>
       </c>
       <c r="H37" t="s">
-        <v>37795</v>
+        <v>38155</v>
       </c>
       <c r="I37" t="s">
-        <v>37836</v>
+        <v>38196</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>37701</v>
+        <v>38061</v>
       </c>
       <c r="B38" t="s">
-        <v>37744</v>
+        <v>38104</v>
       </c>
       <c r="C38" t="s">
-        <v>37760</v>
+        <v>38120</v>
       </c>
       <c r="D38" s="1">
         <v>0.85699999332427979</v>
@@ -116469,24 +117549,24 @@
         <v>1.1779999732971191</v>
       </c>
       <c r="G38" t="s">
-        <v>37775</v>
+        <v>38135</v>
       </c>
       <c r="H38" t="s">
-        <v>37795</v>
+        <v>38155</v>
       </c>
       <c r="I38" t="s">
-        <v>37837</v>
+        <v>38197</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>37702</v>
+        <v>38062</v>
       </c>
       <c r="B39" t="s">
-        <v>37744</v>
+        <v>38104</v>
       </c>
       <c r="C39" t="s">
-        <v>37761</v>
+        <v>38121</v>
       </c>
       <c r="D39" s="1">
         <v>0.64999997615814209</v>
@@ -116498,24 +117578,24 @@
         <v>0.8399999737739563</v>
       </c>
       <c r="G39" t="s">
-        <v>37776</v>
+        <v>38136</v>
       </c>
       <c r="H39" t="s">
-        <v>37795</v>
+        <v>38155</v>
       </c>
       <c r="I39" t="s">
-        <v>37838</v>
+        <v>38198</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>37702</v>
+        <v>38062</v>
       </c>
       <c r="B40" t="s">
-        <v>37745</v>
+        <v>38105</v>
       </c>
       <c r="C40" t="s">
-        <v>37761</v>
+        <v>38121</v>
       </c>
       <c r="D40" s="1">
         <v>0.47999998927116394</v>
@@ -116527,24 +117607,24 @@
         <v>0.75</v>
       </c>
       <c r="G40" t="s">
-        <v>37776</v>
+        <v>38136</v>
       </c>
       <c r="H40" t="s">
-        <v>37795</v>
+        <v>38155</v>
       </c>
       <c r="I40" t="s">
-        <v>37839</v>
+        <v>38199</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>37703</v>
+        <v>38063</v>
       </c>
       <c r="B41" t="s">
-        <v>37746</v>
+        <v>38106</v>
       </c>
       <c r="C41" t="s">
-        <v>37762</v>
+        <v>38122</v>
       </c>
       <c r="D41" s="1">
         <v>0.78100001811981201</v>
@@ -116556,24 +117636,24 @@
         <v>1.3220000267028809</v>
       </c>
       <c r="G41" t="s">
-        <v>37777</v>
+        <v>38137</v>
       </c>
       <c r="H41" t="s">
-        <v>37796</v>
+        <v>38156</v>
       </c>
       <c r="I41" t="s">
-        <v>37840</v>
+        <v>38200</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>37703</v>
+        <v>38063</v>
       </c>
       <c r="B42" t="s">
-        <v>37747</v>
+        <v>38107</v>
       </c>
       <c r="C42" t="s">
-        <v>37762</v>
+        <v>38122</v>
       </c>
       <c r="D42" s="1">
         <v>0.97500002384185791</v>
@@ -116585,24 +117665,24 @@
         <v>1.1829999685287476</v>
       </c>
       <c r="G42" t="s">
-        <v>37777</v>
+        <v>38137</v>
       </c>
       <c r="H42" t="s">
-        <v>37796</v>
+        <v>38156</v>
       </c>
       <c r="I42" t="s">
-        <v>37841</v>
+        <v>38201</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>37704</v>
+        <v>38064</v>
       </c>
       <c r="B43" t="s">
-        <v>37748</v>
+        <v>38108</v>
       </c>
       <c r="C43" t="s">
-        <v>37762</v>
+        <v>38122</v>
       </c>
       <c r="D43" s="1">
         <v>0.93999999761581421</v>
@@ -116614,24 +117694,24 @@
         <v>1.190000057220459</v>
       </c>
       <c r="G43" t="s">
-        <v>37778</v>
+        <v>38138</v>
       </c>
       <c r="H43" t="s">
-        <v>37797</v>
+        <v>38157</v>
       </c>
       <c r="I43" t="s">
-        <v>37842</v>
+        <v>38202</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>37704</v>
+        <v>38064</v>
       </c>
       <c r="B44" t="s">
-        <v>37749</v>
+        <v>38109</v>
       </c>
       <c r="C44" t="s">
-        <v>37762</v>
+        <v>38122</v>
       </c>
       <c r="D44" s="1">
         <v>0.93000000715255737</v>
@@ -116643,24 +117723,24 @@
         <v>1.309999942779541</v>
       </c>
       <c r="G44" t="s">
-        <v>37778</v>
+        <v>38138</v>
       </c>
       <c r="H44" t="s">
-        <v>37797</v>
+        <v>38157</v>
       </c>
       <c r="I44" t="s">
-        <v>37843</v>
+        <v>38203</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>37705</v>
+        <v>38065</v>
       </c>
       <c r="B45" t="s">
-        <v>37750</v>
+        <v>38110</v>
       </c>
       <c r="C45" t="s">
-        <v>37763</v>
+        <v>38123</v>
       </c>
       <c r="D45" s="1">
         <v>0.63999998569488525</v>
@@ -116672,24 +117752,24 @@
         <v>0.9100000262260437</v>
       </c>
       <c r="G45" t="s">
-        <v>37778</v>
+        <v>38138</v>
       </c>
       <c r="H45" t="s">
-        <v>37798</v>
+        <v>38158</v>
       </c>
       <c r="I45" t="s">
-        <v>37844</v>
+        <v>38204</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>37705</v>
+        <v>38065</v>
       </c>
       <c r="B46" t="s">
-        <v>37751</v>
+        <v>38111</v>
       </c>
       <c r="C46" t="s">
-        <v>37763</v>
+        <v>38123</v>
       </c>
       <c r="D46" s="1">
         <v>0.72000002861022949</v>
@@ -116701,24 +117781,24 @@
         <v>0.89999997615814209</v>
       </c>
       <c r="G46" t="s">
-        <v>37778</v>
+        <v>38138</v>
       </c>
       <c r="H46" t="s">
-        <v>37798</v>
+        <v>38158</v>
       </c>
       <c r="I46" t="s">
-        <v>37845</v>
+        <v>38205</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>37706</v>
+        <v>38066</v>
       </c>
       <c r="B47" t="s">
-        <v>37752</v>
+        <v>38112</v>
       </c>
       <c r="C47" t="s">
-        <v>37763</v>
+        <v>38123</v>
       </c>
       <c r="D47" s="1">
         <v>0.46000000834465027</v>
@@ -116730,24 +117810,24 @@
         <v>0.73000001907348633</v>
       </c>
       <c r="G47" t="s">
-        <v>37778</v>
+        <v>38138</v>
       </c>
       <c r="H47" t="s">
-        <v>37799</v>
+        <v>38159</v>
       </c>
       <c r="I47" t="s">
-        <v>37846</v>
+        <v>38206</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>37706</v>
+        <v>38066</v>
       </c>
       <c r="B48" t="s">
-        <v>37753</v>
+        <v>38113</v>
       </c>
       <c r="C48" t="s">
-        <v>37763</v>
+        <v>38123</v>
       </c>
       <c r="D48" s="1">
         <v>0.62999999523162842</v>
@@ -116759,13 +117839,13 @@
         <v>0.89999997615814209</v>
       </c>
       <c r="G48" t="s">
-        <v>37778</v>
+        <v>38138</v>
       </c>
       <c r="H48" t="s">
-        <v>37799</v>
+        <v>38159</v>
       </c>
       <c r="I48" t="s">
-        <v>37847</v>
+        <v>38207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make forest plots to illustrate inversion of RHRs (#11)
* Add do file to make forest plots showing need for inversion

* Make an all.do file to run all Stata do files.

* Add simulated data

* Export inversion forest plots

* Update generated files
</commit_message>
<xml_diff>
--- a/products/Exported Data.xlsx
+++ b/products/Exported Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65215" uniqueCount="38208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65835" uniqueCount="38568">
   <si>
     <t>Study</t>
   </si>
@@ -101537,6 +101537,1086 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Study: Treatment 1 vs Treatment 2</t>
+  </si>
+  <si>
+    <t>Attal 2019 (ICARIA-MM): IsPd vs Pd</t>
+  </si>
+  <si>
+    <t>Bahlis 2020 (POLLUX): DRd vs Rd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2013 (VANTAGE 088): VorV vs V</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2016 (ENDEAVOR): Kd vs Vd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2018 (ELOQUENT-3): EPd vs Pd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2018 (ELOQUENT-2): ELd vs Ld</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2020 (ELOQUENT-2): ELd vs Ld</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2021 (APOLLO): DPd vs Pd</t>
+  </si>
+  <si>
+    <t>Grosicki 2020 (BOSTON): SeVd vs Vd</t>
+  </si>
+  <si>
+    <t>Hou 2017 (China Cont.): IRd vs Rd</t>
+  </si>
+  <si>
+    <t>Jakubowiak 2016 (NCT01478048): EVd vs Vd</t>
+  </si>
+  <si>
+    <t>Kumar 2020 (BELLINI): VeVd vs Vd</t>
+  </si>
+  <si>
+    <t>Lu 2021 (LEPUS): DVd vs Vd</t>
+  </si>
+  <si>
+    <t>Mateos 2020 (CASTOR): DVd vs Vd</t>
+  </si>
+  <si>
+    <t>Moreau 2021 (IKEMA): IsKd vs Kd</t>
+  </si>
+  <si>
+    <t>Orlowski 2019 (ENDEAVOR): Kd vs Vd</t>
+  </si>
+  <si>
+    <t>Richardson 2019 (OPTIMISMM): PVd vs Vd</t>
+  </si>
+  <si>
+    <t>Richardson 2021 (TOURMALINE-MM1): IRd vs Rd</t>
+  </si>
+  <si>
+    <t>San-Miguel 2014 (PANORAMA-1): FVd vs Vd</t>
+  </si>
+  <si>
+    <t>San-Miguel 2016 (PANORAMA 1): FVd vs Vd</t>
+  </si>
+  <si>
+    <t>San-Miguel 2013 (MM-003): Pd vs GC</t>
+  </si>
+  <si>
+    <t>Siegel 2018 (ASPIRE): KRd vs Rd</t>
+  </si>
+  <si>
+    <t>Usamani 2022 (CANDOR): DKd vs Kd</t>
+  </si>
+  <si>
+    <t>lot</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>&gt;3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>&gt;3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>&gt;=4</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>&gt;=4</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>&gt;3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>&gt;3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>&gt;1</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>&gt;2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>&gt;=3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>&gt;2</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>&gt;2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>&gt;=2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>Outcome</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Lower 95% CI Bound on HR</t>
+  </si>
+  <si>
+    <t>Upper 95% CI Bound on HR</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t>Tab. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tab. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      p. 808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. S3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. S4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      AT 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      p. 730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t>Data Extraction Errors</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Study: Treatment 1 vs Treatment 2</t>
+  </si>
+  <si>
+    <t>Attal 2019 (ICARIA-MM): IsPd vs Pd</t>
+  </si>
+  <si>
+    <t>Bahlis 2020 (POLLUX): DRd vs Rd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2013 (VANTAGE 088): VorV vs V</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2016 (ENDEAVOR): Kd vs Vd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2018 (ELOQUENT-3): EPd vs Pd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2021 (APOLLO): DPd vs Pd</t>
+  </si>
+  <si>
+    <t>Hou 2017 (China Cont.): IRd vs Rd</t>
+  </si>
+  <si>
+    <t>Jakubowiak 2016 (NCT01478048): EVd vs Vd</t>
+  </si>
+  <si>
+    <t>Kumar 2020 (BELLINI): VeVd vs Vd</t>
+  </si>
+  <si>
+    <t>Lonial 2015 (ELOQUENT-2): ELd vs Ld</t>
+  </si>
+  <si>
+    <t>Lu 2021 (LEPUS): DVd vs Vd</t>
+  </si>
+  <si>
+    <t>Mateos 2020 (CASTOR): DVd vs Vd</t>
+  </si>
+  <si>
+    <t>Moreau 2021 (IKEMA): IsKd vs Kd</t>
+  </si>
+  <si>
+    <t>Orlowski 2007 (NCT00103506): V vs DoxV</t>
+  </si>
+  <si>
+    <t>Orlowski 2016 (NCT00103506): V vs DoxV</t>
+  </si>
+  <si>
+    <t>Orlowski 2019 (ENDEAVOR): Kd vs Vd</t>
+  </si>
+  <si>
+    <t>Richardson 2019 (OPTIMISMM): PVd vs Vd</t>
+  </si>
+  <si>
+    <t>Richardson 2021 (TOURMALINE-MM1): IRd vs Rd</t>
+  </si>
+  <si>
+    <t>San-Miguel 2016 (PANORAMA 1): FVd vs Vd</t>
+  </si>
+  <si>
+    <t>Stewart 2015 (ASPIRE): KRd vs Rd</t>
+  </si>
+  <si>
+    <t>Usmani 2022 (CANDOR): DKd vs Kd</t>
+  </si>
+  <si>
+    <t>refract</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Previous R use</t>
+  </si>
+  <si>
+    <t>No previous R use</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No IMiD use</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Ref. to R and a PI</t>
+  </si>
+  <si>
+    <t>Not ref. to R and a PI</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No IMiD use</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No IMiD use</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No IMiD use</t>
+  </si>
+  <si>
+    <t>Naive</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Naive</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Previous R use</t>
+  </si>
+  <si>
+    <t>No previous R use</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Not refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Not refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Previous R or T use</t>
+  </si>
+  <si>
+    <t>No previous R or T use</t>
+  </si>
+  <si>
+    <t>Previous R or T use</t>
+  </si>
+  <si>
+    <t>No previous R or T use</t>
+  </si>
+  <si>
+    <t>Previous R use</t>
+  </si>
+  <si>
+    <t>No previous R use</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Refractory to T</t>
+  </si>
+  <si>
+    <t>Not refractory to T</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No previous IMiD use</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Not refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Outcome</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Lower 95% CI Bound on HR</t>
+  </si>
+  <si>
+    <t>Upper 95% CI Bound on HR</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0230</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .       Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tab. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      p. 808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. S3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. S4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t>Data Extraction Errors</t>
   </si>
   <si>
     <t/>
@@ -114688,42 +115768,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>37848</v>
+        <v>38208</v>
       </c>
       <c r="B1" t="s">
-        <v>37872</v>
+        <v>38232</v>
       </c>
       <c r="C1" t="s">
-        <v>37936</v>
+        <v>38296</v>
       </c>
       <c r="D1" t="s">
-        <v>37952</v>
+        <v>38312</v>
       </c>
       <c r="E1" t="s">
-        <v>37953</v>
+        <v>38313</v>
       </c>
       <c r="F1" t="s">
-        <v>37954</v>
+        <v>38314</v>
       </c>
       <c r="G1" t="s">
-        <v>37955</v>
+        <v>38315</v>
       </c>
       <c r="H1" t="s">
-        <v>37956</v>
+        <v>38316</v>
       </c>
       <c r="I1" t="s">
-        <v>37980</v>
+        <v>38340</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>37849</v>
+        <v>38209</v>
       </c>
       <c r="B2" t="s">
-        <v>37873</v>
+        <v>38233</v>
       </c>
       <c r="C2" t="s">
-        <v>37937</v>
+        <v>38297</v>
       </c>
       <c r="D2" s="1">
         <v>0.5899999737739563</v>
@@ -114736,21 +115816,21 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" t="s">
-        <v>37957</v>
+        <v>38317</v>
       </c>
       <c r="I2" t="s">
-        <v>37981</v>
+        <v>38341</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>37849</v>
+        <v>38209</v>
       </c>
       <c r="B3" t="s">
-        <v>37874</v>
+        <v>38234</v>
       </c>
       <c r="C3" t="s">
-        <v>37937</v>
+        <v>38297</v>
       </c>
       <c r="D3" s="1">
         <v>0.5899999737739563</v>
@@ -114763,21 +115843,21 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" t="s">
-        <v>37957</v>
+        <v>38317</v>
       </c>
       <c r="I3" t="s">
-        <v>37982</v>
+        <v>38342</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>37850</v>
+        <v>38210</v>
       </c>
       <c r="B4" t="s">
-        <v>37875</v>
+        <v>38235</v>
       </c>
       <c r="C4" t="s">
-        <v>37937</v>
+        <v>38297</v>
       </c>
       <c r="D4" s="1">
         <v>0.41999998688697815</v>
@@ -114790,21 +115870,21 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" t="s">
-        <v>37958</v>
+        <v>38318</v>
       </c>
       <c r="I4" t="s">
-        <v>37983</v>
+        <v>38343</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>37850</v>
+        <v>38210</v>
       </c>
       <c r="B5" t="s">
-        <v>37876</v>
+        <v>38236</v>
       </c>
       <c r="C5" t="s">
-        <v>37937</v>
+        <v>38297</v>
       </c>
       <c r="D5" s="1">
         <v>0.38999998569488525</v>
@@ -114817,21 +115897,21 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" t="s">
-        <v>37958</v>
+        <v>38318</v>
       </c>
       <c r="I5" t="s">
-        <v>37984</v>
+        <v>38344</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>37850</v>
+        <v>38210</v>
       </c>
       <c r="B6" t="s">
-        <v>37877</v>
+        <v>38237</v>
       </c>
       <c r="C6" t="s">
-        <v>37937</v>
+        <v>38297</v>
       </c>
       <c r="D6" s="1">
         <v>0.47999998927116394</v>
@@ -114844,21 +115924,21 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" t="s">
-        <v>37958</v>
+        <v>38318</v>
       </c>
       <c r="I6" t="s">
-        <v>37985</v>
+        <v>38345</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>37850</v>
+        <v>38210</v>
       </c>
       <c r="B7" t="s">
-        <v>37878</v>
+        <v>38238</v>
       </c>
       <c r="C7" t="s">
-        <v>37937</v>
+        <v>38297</v>
       </c>
       <c r="D7" s="1">
         <v>0.74000000953674316</v>
@@ -114871,21 +115951,21 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" t="s">
-        <v>37958</v>
+        <v>38318</v>
       </c>
       <c r="I7" t="s">
-        <v>37986</v>
+        <v>38346</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>37851</v>
+        <v>38211</v>
       </c>
       <c r="B8" t="s">
-        <v>37879</v>
+        <v>38239</v>
       </c>
       <c r="C8" t="s">
-        <v>37937</v>
+        <v>38297</v>
       </c>
       <c r="D8" s="1">
         <v>0.68699997663497925</v>
@@ -114900,21 +115980,21 @@
         <v>0.015200000256299973</v>
       </c>
       <c r="H8" t="s">
-        <v>37959</v>
+        <v>38319</v>
       </c>
       <c r="I8" t="s">
-        <v>37987</v>
+        <v>38347</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>37851</v>
+        <v>38211</v>
       </c>
       <c r="B9" t="s">
-        <v>37880</v>
+        <v>38240</v>
       </c>
       <c r="C9" t="s">
-        <v>37937</v>
+        <v>38297</v>
       </c>
       <c r="D9" s="1">
         <v>0.91600000858306885</v>
@@ -114929,21 +116009,21 @@
         <v>0.48710000514984131</v>
       </c>
       <c r="H9" t="s">
-        <v>37960</v>
+        <v>38320</v>
       </c>
       <c r="I9" t="s">
-        <v>37988</v>
+        <v>38348</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>37852</v>
+        <v>38212</v>
       </c>
       <c r="B10" t="s">
-        <v>37881</v>
+        <v>38241</v>
       </c>
       <c r="C10" t="s">
-        <v>37937</v>
+        <v>38297</v>
       </c>
       <c r="D10" s="1">
         <v>0.44999998807907104</v>
@@ -114956,21 +116036,21 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" t="s">
-        <v>37961</v>
+        <v>38321</v>
       </c>
       <c r="I10" t="s">
-        <v>37989</v>
+        <v>38349</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>37852</v>
+        <v>38212</v>
       </c>
       <c r="B11" t="s">
-        <v>37882</v>
+        <v>38242</v>
       </c>
       <c r="C11" t="s">
-        <v>37937</v>
+        <v>38297</v>
       </c>
       <c r="D11" s="1">
         <v>0.60000002384185791</v>
@@ -114983,21 +116063,21 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" t="s">
-        <v>37961</v>
+        <v>38321</v>
       </c>
       <c r="I11" t="s">
-        <v>37990</v>
+        <v>38350</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>37853</v>
+        <v>38213</v>
       </c>
       <c r="B12" t="s">
-        <v>37882</v>
+        <v>38242</v>
       </c>
       <c r="C12" t="s">
-        <v>37937</v>
+        <v>38297</v>
       </c>
       <c r="D12" s="1">
         <v>0.55000001192092896</v>
@@ -115010,21 +116090,21 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" t="s">
-        <v>37962</v>
+        <v>38322</v>
       </c>
       <c r="I12" t="s">
-        <v>37991</v>
+        <v>38351</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>37853</v>
+        <v>38213</v>
       </c>
       <c r="B13" t="s">
-        <v>37883</v>
+        <v>38243</v>
       </c>
       <c r="C13" t="s">
-        <v>37937</v>
+        <v>38297</v>
       </c>
       <c r="D13" s="1">
         <v>0.50999999046325684</v>
@@ -115037,21 +116117,21 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" t="s">
-        <v>37962</v>
+        <v>38322</v>
       </c>
       <c r="I13" t="s">
-        <v>37992</v>
+        <v>38352</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>37854</v>
+        <v>38214</v>
       </c>
       <c r="B14" t="s">
-        <v>37884</v>
+        <v>38244</v>
       </c>
       <c r="C14" t="s">
-        <v>37937</v>
+        <v>38297</v>
       </c>
       <c r="D14" s="1">
         <v>0.76999998092651367</v>
@@ -115064,21 +116144,21 @@
       </c>
       <c r="G14" s="1"/>
       <c r="H14" t="s">
-        <v>37963</v>
+        <v>38323</v>
       </c>
       <c r="I14" t="s">
-        <v>37993</v>
+        <v>38353</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>37854</v>
+        <v>38214</v>
       </c>
       <c r="B15" t="s">
-        <v>37885</v>
+        <v>38245</v>
       </c>
       <c r="C15" t="s">
-        <v>37937</v>
+        <v>38297</v>
       </c>
       <c r="D15" s="1">
         <v>0.68000000715255737</v>
@@ -115091,21 +116171,21 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15" t="s">
-        <v>37963</v>
+        <v>38323</v>
       </c>
       <c r="I15" t="s">
-        <v>37994</v>
+        <v>38354</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>37855</v>
+        <v>38215</v>
       </c>
       <c r="B16" t="s">
-        <v>37886</v>
+        <v>38246</v>
       </c>
       <c r="C16" t="s">
-        <v>37938</v>
+        <v>38298</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
@@ -115118,21 +116198,21 @@
       </c>
       <c r="G16" s="1"/>
       <c r="H16" t="s">
-        <v>37963</v>
+        <v>38323</v>
       </c>
       <c r="I16" t="s">
-        <v>37995</v>
+        <v>38355</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>37855</v>
+        <v>38215</v>
       </c>
       <c r="B17" t="s">
-        <v>37887</v>
+        <v>38247</v>
       </c>
       <c r="C17" t="s">
-        <v>37938</v>
+        <v>38298</v>
       </c>
       <c r="D17" s="1">
         <v>0.70999997854232788</v>
@@ -115145,21 +116225,21 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" t="s">
-        <v>37963</v>
+        <v>38323</v>
       </c>
       <c r="I17" t="s">
-        <v>37996</v>
+        <v>38356</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>37856</v>
+        <v>38216</v>
       </c>
       <c r="B18" t="s">
-        <v>37888</v>
+        <v>38248</v>
       </c>
       <c r="C18" t="s">
-        <v>37939</v>
+        <v>38299</v>
       </c>
       <c r="D18" s="1">
         <v>0.69999998807907104</v>
@@ -115172,21 +116252,21 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" t="s">
-        <v>37964</v>
+        <v>38324</v>
       </c>
       <c r="I18" t="s">
-        <v>37997</v>
+        <v>38357</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>37856</v>
+        <v>38216</v>
       </c>
       <c r="B19" t="s">
-        <v>37889</v>
+        <v>38249</v>
       </c>
       <c r="C19" t="s">
-        <v>37939</v>
+        <v>38299</v>
       </c>
       <c r="D19" s="1">
         <v>0.6600000262260437</v>
@@ -115199,21 +116279,21 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19" t="s">
-        <v>37964</v>
+        <v>38324</v>
       </c>
       <c r="I19" t="s">
-        <v>37998</v>
+        <v>38358</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>37856</v>
+        <v>38216</v>
       </c>
       <c r="B20" t="s">
-        <v>37890</v>
+        <v>38250</v>
       </c>
       <c r="C20" t="s">
-        <v>37939</v>
+        <v>38299</v>
       </c>
       <c r="D20" s="1">
         <v>0.40000000596046448</v>
@@ -115226,21 +116306,21 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" t="s">
-        <v>37964</v>
+        <v>38324</v>
       </c>
       <c r="I20" t="s">
-        <v>37999</v>
+        <v>38359</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>37857</v>
+        <v>38217</v>
       </c>
       <c r="B21" t="s">
-        <v>37891</v>
+        <v>38251</v>
       </c>
       <c r="C21" t="s">
-        <v>37939</v>
+        <v>38299</v>
       </c>
       <c r="D21" s="1">
         <v>0.62999999523162842</v>
@@ -115253,21 +116333,21 @@
       </c>
       <c r="G21" s="1"/>
       <c r="H21" t="s">
-        <v>37965</v>
+        <v>38325</v>
       </c>
       <c r="I21" t="s">
-        <v>38000</v>
+        <v>38360</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>37857</v>
+        <v>38217</v>
       </c>
       <c r="B22" t="s">
-        <v>37892</v>
+        <v>38252</v>
       </c>
       <c r="C22" t="s">
-        <v>37939</v>
+        <v>38299</v>
       </c>
       <c r="D22" s="1">
         <v>0.64999997615814209</v>
@@ -115280,21 +116360,21 @@
       </c>
       <c r="G22" s="1"/>
       <c r="H22" t="s">
-        <v>37965</v>
+        <v>38325</v>
       </c>
       <c r="I22" t="s">
-        <v>38001</v>
+        <v>38361</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>37857</v>
+        <v>38217</v>
       </c>
       <c r="B23" t="s">
-        <v>37893</v>
+        <v>38253</v>
       </c>
       <c r="C23" t="s">
-        <v>37939</v>
+        <v>38299</v>
       </c>
       <c r="D23" s="1">
         <v>0.81999999284744263</v>
@@ -115307,21 +116387,21 @@
       </c>
       <c r="G23" s="1"/>
       <c r="H23" t="s">
-        <v>37965</v>
+        <v>38325</v>
       </c>
       <c r="I23" t="s">
-        <v>38002</v>
+        <v>38362</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>37858</v>
+        <v>38218</v>
       </c>
       <c r="B24" t="s">
-        <v>37894</v>
+        <v>38254</v>
       </c>
       <c r="C24" t="s">
-        <v>37939</v>
+        <v>38299</v>
       </c>
       <c r="D24" s="1">
         <v>0.84700000286102295</v>
@@ -115334,21 +116414,21 @@
       </c>
       <c r="G24" s="1"/>
       <c r="H24" t="s">
-        <v>37966</v>
+        <v>38326</v>
       </c>
       <c r="I24" t="s">
-        <v>38003</v>
+        <v>38363</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>37858</v>
+        <v>38218</v>
       </c>
       <c r="B25" t="s">
-        <v>37895</v>
+        <v>38255</v>
       </c>
       <c r="C25" t="s">
-        <v>37939</v>
+        <v>38299</v>
       </c>
       <c r="D25" s="1">
         <v>0.37000000476837158</v>
@@ -115361,21 +116441,21 @@
       </c>
       <c r="G25" s="1"/>
       <c r="H25" t="s">
-        <v>37966</v>
+        <v>38326</v>
       </c>
       <c r="I25" t="s">
-        <v>38004</v>
+        <v>38364</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>37858</v>
+        <v>38218</v>
       </c>
       <c r="B26" t="s">
-        <v>37896</v>
+        <v>38256</v>
       </c>
       <c r="C26" t="s">
-        <v>37939</v>
+        <v>38299</v>
       </c>
       <c r="D26" s="1">
         <v>0.70200002193450928</v>
@@ -115388,21 +116468,21 @@
       </c>
       <c r="G26" s="1"/>
       <c r="H26" t="s">
-        <v>37966</v>
+        <v>38326</v>
       </c>
       <c r="I26" t="s">
-        <v>38005</v>
+        <v>38365</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>37858</v>
+        <v>38218</v>
       </c>
       <c r="B27" t="s">
-        <v>37897</v>
+        <v>38257</v>
       </c>
       <c r="C27" t="s">
-        <v>37940</v>
+        <v>38300</v>
       </c>
       <c r="D27" s="1">
         <v>0.52100002765655518</v>
@@ -115415,21 +116495,21 @@
       </c>
       <c r="G27" s="1"/>
       <c r="H27" t="s">
-        <v>37967</v>
+        <v>38327</v>
       </c>
       <c r="I27" t="s">
-        <v>38006</v>
+        <v>38366</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>37858</v>
+        <v>38218</v>
       </c>
       <c r="B28" t="s">
-        <v>37898</v>
+        <v>38258</v>
       </c>
       <c r="C28" t="s">
-        <v>37940</v>
+        <v>38300</v>
       </c>
       <c r="D28" s="1">
         <v>0.38600000739097595</v>
@@ -115442,21 +116522,21 @@
       </c>
       <c r="G28" s="1"/>
       <c r="H28" t="s">
-        <v>37967</v>
+        <v>38327</v>
       </c>
       <c r="I28" t="s">
-        <v>38007</v>
+        <v>38367</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>37858</v>
+        <v>38218</v>
       </c>
       <c r="B29" t="s">
-        <v>37899</v>
+        <v>38259</v>
       </c>
       <c r="C29" t="s">
-        <v>37940</v>
+        <v>38300</v>
       </c>
       <c r="D29" s="1">
         <v>0.335999995470047</v>
@@ -115469,21 +116549,21 @@
       </c>
       <c r="G29" s="1"/>
       <c r="H29" t="s">
-        <v>37967</v>
+        <v>38327</v>
       </c>
       <c r="I29" t="s">
-        <v>38008</v>
+        <v>38368</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>37859</v>
+        <v>38219</v>
       </c>
       <c r="B30" t="s">
-        <v>37900</v>
+        <v>38260</v>
       </c>
       <c r="C30" t="s">
-        <v>37941</v>
+        <v>38301</v>
       </c>
       <c r="D30" s="1">
         <v>0.68000000715255737</v>
@@ -115496,21 +116576,21 @@
       </c>
       <c r="G30" s="1"/>
       <c r="H30" t="s">
-        <v>37968</v>
+        <v>38328</v>
       </c>
       <c r="I30" t="s">
-        <v>38009</v>
+        <v>38369</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>37859</v>
+        <v>38219</v>
       </c>
       <c r="B31" t="s">
-        <v>37901</v>
+        <v>38261</v>
       </c>
       <c r="C31" t="s">
-        <v>37941</v>
+        <v>38301</v>
       </c>
       <c r="D31" s="1">
         <v>0.72000002861022949</v>
@@ -115523,21 +116603,21 @@
       </c>
       <c r="G31" s="1"/>
       <c r="H31" t="s">
-        <v>37968</v>
+        <v>38328</v>
       </c>
       <c r="I31" t="s">
-        <v>38010</v>
+        <v>38370</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>37860</v>
+        <v>38220</v>
       </c>
       <c r="B32" t="s">
-        <v>37902</v>
+        <v>38262</v>
       </c>
       <c r="C32" t="s">
-        <v>37941</v>
+        <v>38301</v>
       </c>
       <c r="D32" s="1">
         <v>0.75</v>
@@ -115550,21 +116630,21 @@
       </c>
       <c r="G32" s="1"/>
       <c r="H32" t="s">
-        <v>37969</v>
+        <v>38329</v>
       </c>
       <c r="I32" t="s">
-        <v>38011</v>
+        <v>38371</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>37860</v>
+        <v>38220</v>
       </c>
       <c r="B33" t="s">
-        <v>37903</v>
+        <v>38263</v>
       </c>
       <c r="C33" t="s">
-        <v>37941</v>
+        <v>38301</v>
       </c>
       <c r="D33" s="1">
         <v>0.54000002145767212</v>
@@ -115577,21 +116657,21 @@
       </c>
       <c r="G33" s="1"/>
       <c r="H33" t="s">
-        <v>37969</v>
+        <v>38329</v>
       </c>
       <c r="I33" t="s">
-        <v>38012</v>
+        <v>38372</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>37860</v>
+        <v>38220</v>
       </c>
       <c r="B34" t="s">
-        <v>37904</v>
+        <v>38264</v>
       </c>
       <c r="C34" t="s">
-        <v>37942</v>
+        <v>38302</v>
       </c>
       <c r="D34" s="1">
         <v>1.6699999570846558</v>
@@ -115604,21 +116684,21 @@
       </c>
       <c r="G34" s="1"/>
       <c r="H34" t="s">
-        <v>37970</v>
+        <v>38330</v>
       </c>
       <c r="I34" t="s">
-        <v>38013</v>
+        <v>38373</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>37860</v>
+        <v>38220</v>
       </c>
       <c r="B35" t="s">
-        <v>37905</v>
+        <v>38265</v>
       </c>
       <c r="C35" t="s">
-        <v>37942</v>
+        <v>38302</v>
       </c>
       <c r="D35" s="1">
         <v>2.3299999237060547</v>
@@ -115631,21 +116711,21 @@
       </c>
       <c r="G35" s="1"/>
       <c r="H35" t="s">
-        <v>37970</v>
+        <v>38330</v>
       </c>
       <c r="I35" t="s">
-        <v>38014</v>
+        <v>38374</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>37861</v>
+        <v>38221</v>
       </c>
       <c r="B36" t="s">
-        <v>37906</v>
+        <v>38266</v>
       </c>
       <c r="C36" t="s">
-        <v>37943</v>
+        <v>38303</v>
       </c>
       <c r="D36" s="1">
         <v>0.15999999642372131</v>
@@ -115658,21 +116738,21 @@
       </c>
       <c r="G36" s="1"/>
       <c r="H36" t="s">
-        <v>37971</v>
+        <v>38331</v>
       </c>
       <c r="I36" t="s">
-        <v>38015</v>
+        <v>38375</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>37861</v>
+        <v>38221</v>
       </c>
       <c r="B37" t="s">
-        <v>37907</v>
+        <v>38267</v>
       </c>
       <c r="C37" t="s">
-        <v>37943</v>
+        <v>38303</v>
       </c>
       <c r="D37" s="1">
         <v>0.51999998092651367</v>
@@ -115685,21 +116765,21 @@
       </c>
       <c r="G37" s="1"/>
       <c r="H37" t="s">
-        <v>37971</v>
+        <v>38331</v>
       </c>
       <c r="I37" t="s">
-        <v>38016</v>
+        <v>38376</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>37861</v>
+        <v>38221</v>
       </c>
       <c r="B38" t="s">
-        <v>37908</v>
+        <v>38268</v>
       </c>
       <c r="C38" t="s">
-        <v>37943</v>
+        <v>38303</v>
       </c>
       <c r="D38" s="1">
         <v>0.62999999523162842</v>
@@ -115712,21 +116792,21 @@
       </c>
       <c r="G38" s="1"/>
       <c r="H38" t="s">
-        <v>37971</v>
+        <v>38331</v>
       </c>
       <c r="I38" t="s">
-        <v>38017</v>
+        <v>38377</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>37861</v>
+        <v>38221</v>
       </c>
       <c r="B39" t="s">
-        <v>37909</v>
+        <v>38269</v>
       </c>
       <c r="C39" t="s">
-        <v>37943</v>
+        <v>38303</v>
       </c>
       <c r="D39" s="1">
         <v>0.25999999046325684</v>
@@ -115739,21 +116819,21 @@
       </c>
       <c r="G39" s="1"/>
       <c r="H39" t="s">
-        <v>37971</v>
+        <v>38331</v>
       </c>
       <c r="I39" t="s">
-        <v>38018</v>
+        <v>38378</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>37862</v>
+        <v>38222</v>
       </c>
       <c r="B40" t="s">
-        <v>37910</v>
+        <v>38270</v>
       </c>
       <c r="C40" t="s">
-        <v>37943</v>
+        <v>38303</v>
       </c>
       <c r="D40" s="1">
         <v>0.2199999988079071</v>
@@ -115766,21 +116846,21 @@
       </c>
       <c r="G40" s="1"/>
       <c r="H40" t="s">
-        <v>37971</v>
+        <v>38331</v>
       </c>
       <c r="I40" t="s">
-        <v>38019</v>
+        <v>38379</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>37862</v>
+        <v>38222</v>
       </c>
       <c r="B41" t="s">
-        <v>37911</v>
+        <v>38271</v>
       </c>
       <c r="C41" t="s">
-        <v>37943</v>
+        <v>38303</v>
       </c>
       <c r="D41" s="1">
         <v>0.46000000834465027</v>
@@ -115793,21 +116873,21 @@
       </c>
       <c r="G41" s="1"/>
       <c r="H41" t="s">
-        <v>37971</v>
+        <v>38331</v>
       </c>
       <c r="I41" t="s">
-        <v>38020</v>
+        <v>38380</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>37862</v>
+        <v>38222</v>
       </c>
       <c r="B42" t="s">
-        <v>37912</v>
+        <v>38272</v>
       </c>
       <c r="C42" t="s">
-        <v>37943</v>
+        <v>38303</v>
       </c>
       <c r="D42" s="1">
         <v>0.60000002384185791</v>
@@ -115820,21 +116900,21 @@
       </c>
       <c r="G42" s="1"/>
       <c r="H42" t="s">
-        <v>37971</v>
+        <v>38331</v>
       </c>
       <c r="I42" t="s">
-        <v>38021</v>
+        <v>38381</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>37862</v>
+        <v>38222</v>
       </c>
       <c r="B43" t="s">
-        <v>37913</v>
+        <v>38273</v>
       </c>
       <c r="C43" t="s">
-        <v>37943</v>
+        <v>38303</v>
       </c>
       <c r="D43" s="1">
         <v>0.37000000476837158</v>
@@ -115847,21 +116927,21 @@
       </c>
       <c r="G43" s="1"/>
       <c r="H43" t="s">
-        <v>37971</v>
+        <v>38331</v>
       </c>
       <c r="I43" t="s">
-        <v>38022</v>
+        <v>38382</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>37863</v>
+        <v>38223</v>
       </c>
       <c r="B44" t="s">
-        <v>37914</v>
+        <v>38274</v>
       </c>
       <c r="C44" t="s">
-        <v>37943</v>
+        <v>38303</v>
       </c>
       <c r="D44" s="1">
         <v>0.5899999737739563</v>
@@ -115874,21 +116954,21 @@
       </c>
       <c r="G44" s="1"/>
       <c r="H44" t="s">
-        <v>37972</v>
+        <v>38332</v>
       </c>
       <c r="I44" t="s">
-        <v>38023</v>
+        <v>38383</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>37863</v>
+        <v>38223</v>
       </c>
       <c r="B45" t="s">
-        <v>37915</v>
+        <v>38275</v>
       </c>
       <c r="C45" t="s">
-        <v>37943</v>
+        <v>38303</v>
       </c>
       <c r="D45" s="1">
         <v>0.47999998927116394</v>
@@ -115901,21 +116981,21 @@
       </c>
       <c r="G45" s="1"/>
       <c r="H45" t="s">
-        <v>37972</v>
+        <v>38332</v>
       </c>
       <c r="I45" t="s">
-        <v>38024</v>
+        <v>38384</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>37864</v>
+        <v>38224</v>
       </c>
       <c r="B46" t="s">
-        <v>37916</v>
+        <v>38276</v>
       </c>
       <c r="C46" t="s">
-        <v>37944</v>
+        <v>38304</v>
       </c>
       <c r="D46" s="1">
         <v>0.77100002765655518</v>
@@ -115928,21 +117008,21 @@
       </c>
       <c r="G46" s="1"/>
       <c r="H46" t="s">
-        <v>37972</v>
+        <v>38332</v>
       </c>
       <c r="I46" t="s">
-        <v>38025</v>
+        <v>38385</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>37864</v>
+        <v>38224</v>
       </c>
       <c r="B47" t="s">
-        <v>37917</v>
+        <v>38277</v>
       </c>
       <c r="C47" t="s">
-        <v>37944</v>
+        <v>38304</v>
       </c>
       <c r="D47" s="1">
         <v>0.75199997425079346</v>
@@ -115955,21 +117035,21 @@
       </c>
       <c r="G47" s="1"/>
       <c r="H47" t="s">
-        <v>37972</v>
+        <v>38332</v>
       </c>
       <c r="I47" t="s">
-        <v>38026</v>
+        <v>38386</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>37865</v>
+        <v>38225</v>
       </c>
       <c r="B48" t="s">
-        <v>37918</v>
+        <v>38278</v>
       </c>
       <c r="C48" t="s">
-        <v>37945</v>
+        <v>38305</v>
       </c>
       <c r="D48" s="1">
         <v>0.54000002145767212</v>
@@ -115982,21 +117062,21 @@
       </c>
       <c r="G48" s="1"/>
       <c r="H48" t="s">
-        <v>37972</v>
+        <v>38332</v>
       </c>
       <c r="I48" t="s">
-        <v>38027</v>
+        <v>38387</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>37865</v>
+        <v>38225</v>
       </c>
       <c r="B49" t="s">
-        <v>37919</v>
+        <v>38279</v>
       </c>
       <c r="C49" t="s">
-        <v>37945</v>
+        <v>38305</v>
       </c>
       <c r="D49" s="1">
         <v>0.67000001668930054</v>
@@ -116009,21 +117089,21 @@
       </c>
       <c r="G49" s="1"/>
       <c r="H49" t="s">
-        <v>37972</v>
+        <v>38332</v>
       </c>
       <c r="I49" t="s">
-        <v>38028</v>
+        <v>38388</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>37865</v>
+        <v>38225</v>
       </c>
       <c r="B50" t="s">
-        <v>37920</v>
+        <v>38280</v>
       </c>
       <c r="C50" t="s">
-        <v>37945</v>
+        <v>38305</v>
       </c>
       <c r="D50" s="1">
         <v>0.60000002384185791</v>
@@ -116036,21 +117116,21 @@
       </c>
       <c r="G50" s="1"/>
       <c r="H50" t="s">
-        <v>37972</v>
+        <v>38332</v>
       </c>
       <c r="I50" t="s">
-        <v>38029</v>
+        <v>38389</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>37866</v>
+        <v>38226</v>
       </c>
       <c r="B51" t="s">
-        <v>37921</v>
+        <v>38281</v>
       </c>
       <c r="C51" t="s">
-        <v>37946</v>
+        <v>38306</v>
       </c>
       <c r="D51" s="1">
         <v>0.97600001096725464</v>
@@ -116063,21 +117143,21 @@
       </c>
       <c r="G51" s="1"/>
       <c r="H51" t="s">
-        <v>37973</v>
+        <v>38333</v>
       </c>
       <c r="I51" t="s">
-        <v>38030</v>
+        <v>38390</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>37866</v>
+        <v>38226</v>
       </c>
       <c r="B52" t="s">
-        <v>37922</v>
+        <v>38282</v>
       </c>
       <c r="C52" t="s">
-        <v>37946</v>
+        <v>38306</v>
       </c>
       <c r="D52" s="1">
         <v>0.92599999904632568</v>
@@ -116090,21 +117170,21 @@
       </c>
       <c r="G52" s="1"/>
       <c r="H52" t="s">
-        <v>37973</v>
+        <v>38333</v>
       </c>
       <c r="I52" t="s">
-        <v>38031</v>
+        <v>38391</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>37866</v>
+        <v>38226</v>
       </c>
       <c r="B53" t="s">
-        <v>37923</v>
+        <v>38283</v>
       </c>
       <c r="C53" t="s">
-        <v>37946</v>
+        <v>38306</v>
       </c>
       <c r="D53" s="1">
         <v>0.88300001621246338</v>
@@ -116117,21 +117197,21 @@
       </c>
       <c r="G53" s="1"/>
       <c r="H53" t="s">
-        <v>37973</v>
+        <v>38333</v>
       </c>
       <c r="I53" t="s">
-        <v>38032</v>
+        <v>38392</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>37867</v>
+        <v>38227</v>
       </c>
       <c r="B54" t="s">
-        <v>37924</v>
+        <v>38284</v>
       </c>
       <c r="C54" t="s">
-        <v>37947</v>
+        <v>38307</v>
       </c>
       <c r="D54" s="1">
         <v>0.6600000262260437</v>
@@ -116144,21 +117224,21 @@
       </c>
       <c r="G54" s="1"/>
       <c r="H54" t="s">
-        <v>37974</v>
+        <v>38334</v>
       </c>
       <c r="I54" t="s">
-        <v>38033</v>
+        <v>38393</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>37867</v>
+        <v>38227</v>
       </c>
       <c r="B55" t="s">
-        <v>37925</v>
+        <v>38285</v>
       </c>
       <c r="C55" t="s">
-        <v>37947</v>
+        <v>38307</v>
       </c>
       <c r="D55" s="1">
         <v>0.63999998569488525</v>
@@ -116171,21 +117251,21 @@
       </c>
       <c r="G55" s="1"/>
       <c r="H55" t="s">
-        <v>37974</v>
+        <v>38334</v>
       </c>
       <c r="I55" t="s">
-        <v>38034</v>
+        <v>38394</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>37868</v>
+        <v>38228</v>
       </c>
       <c r="B56" t="s">
-        <v>37926</v>
+        <v>38286</v>
       </c>
       <c r="C56" t="s">
-        <v>37948</v>
+        <v>38308</v>
       </c>
       <c r="D56" s="1">
         <v>0.89999997615814209</v>
@@ -116198,21 +117278,21 @@
       </c>
       <c r="G56" s="1"/>
       <c r="H56" t="s">
-        <v>37975</v>
+        <v>38335</v>
       </c>
       <c r="I56" t="s">
-        <v>38035</v>
+        <v>38395</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>37868</v>
+        <v>38228</v>
       </c>
       <c r="B57" t="s">
-        <v>37927</v>
+        <v>38287</v>
       </c>
       <c r="C57" t="s">
-        <v>37948</v>
+        <v>38308</v>
       </c>
       <c r="D57" s="1">
         <v>0.95999997854232788</v>
@@ -116225,21 +117305,21 @@
       </c>
       <c r="G57" s="1"/>
       <c r="H57" t="s">
-        <v>37975</v>
+        <v>38335</v>
       </c>
       <c r="I57" t="s">
-        <v>38036</v>
+        <v>38396</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>37869</v>
+        <v>38229</v>
       </c>
       <c r="B58" t="s">
-        <v>37928</v>
+        <v>38288</v>
       </c>
       <c r="C58" t="s">
-        <v>37949</v>
+        <v>38309</v>
       </c>
       <c r="D58" s="1">
         <v>0.4699999988079071</v>
@@ -116252,21 +117332,21 @@
       </c>
       <c r="G58" s="1"/>
       <c r="H58" t="s">
-        <v>37976</v>
+        <v>38336</v>
       </c>
       <c r="I58" t="s">
-        <v>38037</v>
+        <v>38397</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>37869</v>
+        <v>38229</v>
       </c>
       <c r="B59" t="s">
-        <v>37929</v>
+        <v>38289</v>
       </c>
       <c r="C59" t="s">
-        <v>37949</v>
+        <v>38309</v>
       </c>
       <c r="D59" s="1">
         <v>0.47999998927116394</v>
@@ -116279,21 +117359,21 @@
       </c>
       <c r="G59" s="1"/>
       <c r="H59" t="s">
-        <v>37976</v>
+        <v>38336</v>
       </c>
       <c r="I59" t="s">
-        <v>38038</v>
+        <v>38398</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>37869</v>
+        <v>38229</v>
       </c>
       <c r="B60" t="s">
-        <v>37930</v>
+        <v>38290</v>
       </c>
       <c r="C60" t="s">
-        <v>37950</v>
+        <v>38310</v>
       </c>
       <c r="D60" s="1">
         <v>0.43999999761581421</v>
@@ -116306,21 +117386,21 @@
       </c>
       <c r="G60" s="1"/>
       <c r="H60" t="s">
-        <v>37977</v>
+        <v>38337</v>
       </c>
       <c r="I60" t="s">
-        <v>38039</v>
+        <v>38399</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>37869</v>
+        <v>38229</v>
       </c>
       <c r="B61" t="s">
-        <v>37931</v>
+        <v>38291</v>
       </c>
       <c r="C61" t="s">
-        <v>37950</v>
+        <v>38310</v>
       </c>
       <c r="D61" s="1">
         <v>0.75999999046325684</v>
@@ -116333,21 +117413,21 @@
       </c>
       <c r="G61" s="1"/>
       <c r="H61" t="s">
-        <v>37977</v>
+        <v>38337</v>
       </c>
       <c r="I61" t="s">
-        <v>38040</v>
+        <v>38400</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>37870</v>
+        <v>38230</v>
       </c>
       <c r="B62" t="s">
-        <v>37932</v>
+        <v>38292</v>
       </c>
       <c r="C62" t="s">
-        <v>37950</v>
+        <v>38310</v>
       </c>
       <c r="D62" s="1">
         <v>0.81000000238418579</v>
@@ -116360,21 +117440,21 @@
       </c>
       <c r="G62" s="1"/>
       <c r="H62" t="s">
-        <v>37978</v>
+        <v>38338</v>
       </c>
       <c r="I62" t="s">
-        <v>38041</v>
+        <v>38401</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>37870</v>
+        <v>38230</v>
       </c>
       <c r="B63" t="s">
-        <v>37933</v>
+        <v>38293</v>
       </c>
       <c r="C63" t="s">
-        <v>37950</v>
+        <v>38310</v>
       </c>
       <c r="D63" s="1">
         <v>0.79000002145767212</v>
@@ -116387,21 +117467,21 @@
       </c>
       <c r="G63" s="1"/>
       <c r="H63" t="s">
-        <v>37978</v>
+        <v>38338</v>
       </c>
       <c r="I63" t="s">
-        <v>38042</v>
+        <v>38402</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>37871</v>
+        <v>38231</v>
       </c>
       <c r="B64" t="s">
-        <v>37934</v>
+        <v>38294</v>
       </c>
       <c r="C64" t="s">
-        <v>37951</v>
+        <v>38311</v>
       </c>
       <c r="D64" s="1">
         <v>0.6600000262260437</v>
@@ -116414,21 +117494,21 @@
       </c>
       <c r="G64" s="1"/>
       <c r="H64" t="s">
-        <v>37979</v>
+        <v>38339</v>
       </c>
       <c r="I64" t="s">
-        <v>38043</v>
+        <v>38403</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>37871</v>
+        <v>38231</v>
       </c>
       <c r="B65" t="s">
-        <v>37935</v>
+        <v>38295</v>
       </c>
       <c r="C65" t="s">
-        <v>37951</v>
+        <v>38311</v>
       </c>
       <c r="D65" s="1">
         <v>0.55000001192092896</v>
@@ -116441,10 +117521,10 @@
       </c>
       <c r="G65" s="1"/>
       <c r="H65" t="s">
-        <v>37979</v>
+        <v>38339</v>
       </c>
       <c r="I65" t="s">
-        <v>38044</v>
+        <v>38404</v>
       </c>
     </row>
   </sheetData>
@@ -116458,42 +117538,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>38045</v>
+        <v>38405</v>
       </c>
       <c r="B1" t="s">
-        <v>38067</v>
+        <v>38427</v>
       </c>
       <c r="C1" t="s">
-        <v>38114</v>
+        <v>38474</v>
       </c>
       <c r="D1" t="s">
-        <v>38124</v>
+        <v>38484</v>
       </c>
       <c r="E1" t="s">
-        <v>38125</v>
+        <v>38485</v>
       </c>
       <c r="F1" t="s">
-        <v>38126</v>
+        <v>38486</v>
       </c>
       <c r="G1" t="s">
-        <v>38127</v>
+        <v>38487</v>
       </c>
       <c r="H1" t="s">
-        <v>38139</v>
+        <v>38499</v>
       </c>
       <c r="I1" t="s">
-        <v>38160</v>
+        <v>38520</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>38046</v>
+        <v>38406</v>
       </c>
       <c r="B2" t="s">
-        <v>38068</v>
+        <v>38428</v>
       </c>
       <c r="C2" t="s">
-        <v>38115</v>
+        <v>38475</v>
       </c>
       <c r="D2" s="1">
         <v>0.5899999737739563</v>
@@ -116505,24 +117585,24 @@
         <v>0.81999999284744263</v>
       </c>
       <c r="G2" t="s">
-        <v>38128</v>
+        <v>38488</v>
       </c>
       <c r="H2" t="s">
-        <v>38140</v>
+        <v>38500</v>
       </c>
       <c r="I2" t="s">
-        <v>38161</v>
+        <v>38521</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>38046</v>
+        <v>38406</v>
       </c>
       <c r="B3" t="s">
-        <v>38069</v>
+        <v>38429</v>
       </c>
       <c r="C3" t="s">
-        <v>38115</v>
+        <v>38475</v>
       </c>
       <c r="D3" s="1">
         <v>0.18000000715255737</v>
@@ -116534,24 +117614,24 @@
         <v>1.4900000095367432</v>
       </c>
       <c r="G3" t="s">
-        <v>38128</v>
+        <v>38488</v>
       </c>
       <c r="H3" t="s">
-        <v>38140</v>
+        <v>38500</v>
       </c>
       <c r="I3" t="s">
-        <v>38162</v>
+        <v>38522</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>38047</v>
+        <v>38407</v>
       </c>
       <c r="B4" t="s">
-        <v>38070</v>
+        <v>38430</v>
       </c>
       <c r="C4" t="s">
-        <v>38115</v>
+        <v>38475</v>
       </c>
       <c r="D4" s="1">
         <v>0.37999999523162842</v>
@@ -116563,24 +117643,24 @@
         <v>0.6600000262260437</v>
       </c>
       <c r="G4" t="s">
-        <v>38128</v>
+        <v>38488</v>
       </c>
       <c r="H4" t="s">
-        <v>38141</v>
+        <v>38501</v>
       </c>
       <c r="I4" t="s">
-        <v>38163</v>
+        <v>38523</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>38047</v>
+        <v>38407</v>
       </c>
       <c r="B5" t="s">
-        <v>38071</v>
+        <v>38431</v>
       </c>
       <c r="C5" t="s">
-        <v>38115</v>
+        <v>38475</v>
       </c>
       <c r="D5" s="1">
         <v>0.44999998807907104</v>
@@ -116592,24 +117672,24 @@
         <v>0.57999998331069946</v>
       </c>
       <c r="G5" t="s">
-        <v>38128</v>
+        <v>38488</v>
       </c>
       <c r="H5" t="s">
-        <v>38141</v>
+        <v>38501</v>
       </c>
       <c r="I5" t="s">
-        <v>38164</v>
+        <v>38524</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>38048</v>
+        <v>38408</v>
       </c>
       <c r="B6" t="s">
-        <v>38072</v>
+        <v>38432</v>
       </c>
       <c r="C6" t="s">
-        <v>38115</v>
+        <v>38475</v>
       </c>
       <c r="D6" s="1">
         <v>0.75700002908706665</v>
@@ -116621,24 +117701,24 @@
         <v>0.96299999952316284</v>
       </c>
       <c r="G6" t="s">
-        <v>38129</v>
+        <v>38489</v>
       </c>
       <c r="H6" t="s">
-        <v>38142</v>
+        <v>38502</v>
       </c>
       <c r="I6" t="s">
-        <v>38165</v>
+        <v>38525</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>38048</v>
+        <v>38408</v>
       </c>
       <c r="B7" t="s">
-        <v>38073</v>
+        <v>38433</v>
       </c>
       <c r="C7" t="s">
-        <v>38115</v>
+        <v>38475</v>
       </c>
       <c r="D7" s="1">
         <v>0.92599999904632568</v>
@@ -116650,24 +117730,24 @@
         <v>1.2790000438690186</v>
       </c>
       <c r="G7" t="s">
-        <v>38130</v>
+        <v>38490</v>
       </c>
       <c r="H7" t="s">
-        <v>38142</v>
+        <v>38502</v>
       </c>
       <c r="I7" t="s">
-        <v>38166</v>
+        <v>38526</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>38049</v>
+        <v>38409</v>
       </c>
       <c r="B8" t="s">
-        <v>38074</v>
+        <v>38434</v>
       </c>
       <c r="C8" t="s">
-        <v>38115</v>
+        <v>38475</v>
       </c>
       <c r="D8" s="1">
         <v>0.43999999761581421</v>
@@ -116679,24 +117759,24 @@
         <v>0.56000000238418579</v>
       </c>
       <c r="G8" t="s">
-        <v>38131</v>
+        <v>38491</v>
       </c>
       <c r="H8" t="s">
-        <v>38143</v>
+        <v>38503</v>
       </c>
       <c r="I8" t="s">
-        <v>38167</v>
+        <v>38527</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>38049</v>
+        <v>38409</v>
       </c>
       <c r="B9" t="s">
-        <v>38075</v>
+        <v>38435</v>
       </c>
       <c r="C9" t="s">
-        <v>38115</v>
+        <v>38475</v>
       </c>
       <c r="D9" s="1">
         <v>0.80000001192092896</v>
@@ -116708,24 +117788,24 @@
         <v>1.1100000143051147</v>
       </c>
       <c r="G9" t="s">
-        <v>38131</v>
+        <v>38491</v>
       </c>
       <c r="H9" t="s">
-        <v>38143</v>
+        <v>38503</v>
       </c>
       <c r="I9" t="s">
-        <v>38168</v>
+        <v>38528</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>38050</v>
+        <v>38410</v>
       </c>
       <c r="B10" t="s">
-        <v>38076</v>
+        <v>38436</v>
       </c>
       <c r="C10" t="s">
-        <v>38115</v>
+        <v>38475</v>
       </c>
       <c r="D10" s="1">
         <v>0.56000000238418579</v>
@@ -116737,24 +117817,24 @@
         <v>0.97000002861022949</v>
       </c>
       <c r="G10" t="s">
-        <v>38131</v>
+        <v>38491</v>
       </c>
       <c r="H10" t="s">
-        <v>38144</v>
+        <v>38504</v>
       </c>
       <c r="I10" t="s">
-        <v>38169</v>
+        <v>38529</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>38050</v>
+        <v>38410</v>
       </c>
       <c r="B11" t="s">
-        <v>38077</v>
+        <v>38437</v>
       </c>
       <c r="C11" t="s">
-        <v>38115</v>
+        <v>38475</v>
       </c>
       <c r="D11" s="1">
         <v>0.50999999046325684</v>
@@ -116766,24 +117846,24 @@
         <v>1.190000057220459</v>
       </c>
       <c r="G11" t="s">
-        <v>38131</v>
+        <v>38491</v>
       </c>
       <c r="H11" t="s">
-        <v>38144</v>
+        <v>38504</v>
       </c>
       <c r="I11" t="s">
-        <v>38170</v>
+        <v>38530</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>38051</v>
+        <v>38411</v>
       </c>
       <c r="B12" t="s">
-        <v>38078</v>
+        <v>38438</v>
       </c>
       <c r="C12" t="s">
-        <v>38115</v>
+        <v>38475</v>
       </c>
       <c r="D12" s="1">
         <v>0.6600000262260437</v>
@@ -116795,24 +117875,24 @@
         <v>0.89999997615814209</v>
       </c>
       <c r="G12" t="s">
-        <v>38131</v>
+        <v>38491</v>
       </c>
       <c r="H12" t="s">
-        <v>38145</v>
+        <v>38505</v>
       </c>
       <c r="I12" t="s">
-        <v>38171</v>
+        <v>38531</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>38051</v>
+        <v>38411</v>
       </c>
       <c r="B13" t="s">
-        <v>38079</v>
+        <v>38439</v>
       </c>
       <c r="C13" t="s">
-        <v>38115</v>
+        <v>38475</v>
       </c>
       <c r="D13" s="1">
         <v>0.36000001430511475</v>
@@ -116824,24 +117904,24 @@
         <v>0.82999998331069946</v>
       </c>
       <c r="G13" t="s">
-        <v>38131</v>
+        <v>38491</v>
       </c>
       <c r="H13" t="s">
-        <v>38145</v>
+        <v>38505</v>
       </c>
       <c r="I13" t="s">
-        <v>38172</v>
+        <v>38532</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>38052</v>
+        <v>38412</v>
       </c>
       <c r="B14" t="s">
-        <v>38080</v>
+        <v>38440</v>
       </c>
       <c r="C14" t="s">
-        <v>38115</v>
+        <v>38475</v>
       </c>
       <c r="D14" s="1">
         <v>0.55299997329711914</v>
@@ -116853,24 +117933,24 @@
         <v>0.9309999942779541</v>
       </c>
       <c r="G14" t="s">
-        <v>38132</v>
+        <v>38492</v>
       </c>
       <c r="H14" t="s">
-        <v>38146</v>
+        <v>38506</v>
       </c>
       <c r="I14" t="s">
-        <v>38173</v>
+        <v>38533</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>38052</v>
+        <v>38412</v>
       </c>
       <c r="B15" t="s">
-        <v>38081</v>
+        <v>38441</v>
       </c>
       <c r="C15" t="s">
-        <v>38115</v>
+        <v>38475</v>
       </c>
       <c r="D15" s="1">
         <v>0.76599997282028198</v>
@@ -116882,24 +117962,24 @@
         <v>3.9639999866485596</v>
       </c>
       <c r="G15" t="s">
-        <v>38132</v>
+        <v>38492</v>
       </c>
       <c r="H15" t="s">
-        <v>38146</v>
+        <v>38506</v>
       </c>
       <c r="I15" t="s">
-        <v>38174</v>
+        <v>38534</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>38052</v>
+        <v>38412</v>
       </c>
       <c r="B16" t="s">
-        <v>38082</v>
+        <v>38442</v>
       </c>
       <c r="C16" t="s">
-        <v>38116</v>
+        <v>38476</v>
       </c>
       <c r="D16" s="1">
         <v>0.39800000190734863</v>
@@ -116911,24 +117991,24 @@
         <v>0.71899998188018799</v>
       </c>
       <c r="G16" t="s">
-        <v>38132</v>
+        <v>38492</v>
       </c>
       <c r="H16" t="s">
-        <v>38147</v>
+        <v>38507</v>
       </c>
       <c r="I16" t="s">
-        <v>38175</v>
+        <v>38535</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>38052</v>
+        <v>38412</v>
       </c>
       <c r="B17" t="s">
-        <v>38083</v>
+        <v>38443</v>
       </c>
       <c r="C17" t="s">
-        <v>38116</v>
+        <v>38476</v>
       </c>
       <c r="D17" s="1">
         <v>0.49799999594688416</v>
@@ -116940,24 +118020,24 @@
         <v>2.4030001163482666</v>
       </c>
       <c r="G17" t="s">
-        <v>38132</v>
+        <v>38492</v>
       </c>
       <c r="H17" t="s">
-        <v>38147</v>
+        <v>38507</v>
       </c>
       <c r="I17" t="s">
-        <v>38176</v>
+        <v>38536</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>38053</v>
+        <v>38413</v>
       </c>
       <c r="B18" t="s">
-        <v>38084</v>
+        <v>38444</v>
       </c>
       <c r="C18" t="s">
-        <v>38117</v>
+        <v>38477</v>
       </c>
       <c r="D18" s="1">
         <v>0.87000000476837158</v>
@@ -116969,24 +118049,24 @@
         <v>1.2899999618530273</v>
       </c>
       <c r="G18" t="s">
-        <v>38133</v>
+        <v>38493</v>
       </c>
       <c r="H18" t="s">
-        <v>38148</v>
+        <v>38508</v>
       </c>
       <c r="I18" t="s">
-        <v>38177</v>
+        <v>38537</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>38053</v>
+        <v>38413</v>
       </c>
       <c r="B19" t="s">
-        <v>38085</v>
+        <v>38445</v>
       </c>
       <c r="C19" t="s">
-        <v>38117</v>
+        <v>38477</v>
       </c>
       <c r="D19" s="1">
         <v>0.38999998569488525</v>
@@ -116998,24 +118078,24 @@
         <v>0.80000001192092896</v>
       </c>
       <c r="G19" t="s">
-        <v>38133</v>
+        <v>38493</v>
       </c>
       <c r="H19" t="s">
-        <v>38148</v>
+        <v>38508</v>
       </c>
       <c r="I19" t="s">
-        <v>38178</v>
+        <v>38538</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>38054</v>
+        <v>38414</v>
       </c>
       <c r="B20" t="s">
-        <v>38086</v>
+        <v>38446</v>
       </c>
       <c r="C20" t="s">
-        <v>38117</v>
+        <v>38477</v>
       </c>
       <c r="D20" s="1">
         <v>0.61000001430511475</v>
@@ -117027,24 +118107,24 @@
         <v>1.1699999570846558</v>
       </c>
       <c r="G20" t="s">
-        <v>38133</v>
+        <v>38493</v>
       </c>
       <c r="H20" t="s">
-        <v>38149</v>
+        <v>38509</v>
       </c>
       <c r="I20" t="s">
-        <v>38179</v>
+        <v>38539</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>38054</v>
+        <v>38414</v>
       </c>
       <c r="B21" t="s">
-        <v>38087</v>
+        <v>38447</v>
       </c>
       <c r="C21" t="s">
-        <v>38117</v>
+        <v>38477</v>
       </c>
       <c r="D21" s="1">
         <v>0.75</v>
@@ -117056,24 +118136,24 @@
         <v>1.3600000143051147</v>
       </c>
       <c r="G21" t="s">
-        <v>38133</v>
+        <v>38493</v>
       </c>
       <c r="H21" t="s">
-        <v>38149</v>
+        <v>38509</v>
       </c>
       <c r="I21" t="s">
-        <v>38180</v>
+        <v>38540</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>38054</v>
+        <v>38414</v>
       </c>
       <c r="B22" t="s">
-        <v>38088</v>
+        <v>38448</v>
       </c>
       <c r="C22" t="s">
-        <v>38118</v>
+        <v>38478</v>
       </c>
       <c r="D22" s="1">
         <v>5.9000000953674316</v>
@@ -117085,24 +118165,24 @@
         <v>46.099998474121094</v>
       </c>
       <c r="G22" t="s">
-        <v>38133</v>
+        <v>38493</v>
       </c>
       <c r="H22" t="s">
-        <v>38150</v>
+        <v>38510</v>
       </c>
       <c r="I22" t="s">
-        <v>38181</v>
+        <v>38541</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>38054</v>
+        <v>38414</v>
       </c>
       <c r="B23" t="s">
-        <v>38089</v>
+        <v>38449</v>
       </c>
       <c r="C23" t="s">
-        <v>38118</v>
+        <v>38478</v>
       </c>
       <c r="D23" s="1">
         <v>1.8200000524520874</v>
@@ -117114,24 +118194,24 @@
         <v>5.1399998664855957</v>
       </c>
       <c r="G23" t="s">
-        <v>38133</v>
+        <v>38493</v>
       </c>
       <c r="H23" t="s">
-        <v>38150</v>
+        <v>38510</v>
       </c>
       <c r="I23" t="s">
-        <v>38182</v>
+        <v>38542</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>38055</v>
+        <v>38415</v>
       </c>
       <c r="B24" t="s">
-        <v>38090</v>
+        <v>38450</v>
       </c>
       <c r="C24" t="s">
-        <v>38119</v>
+        <v>38479</v>
       </c>
       <c r="D24" s="1">
         <v>0.5899999737739563</v>
@@ -117143,24 +118223,24 @@
         <v>1.3999999761581421</v>
       </c>
       <c r="G24" t="s">
-        <v>38133</v>
+        <v>38493</v>
       </c>
       <c r="H24" t="s">
-        <v>38151</v>
+        <v>38511</v>
       </c>
       <c r="I24" t="s">
-        <v>38183</v>
+        <v>38543</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>38055</v>
+        <v>38415</v>
       </c>
       <c r="B25" t="s">
-        <v>38091</v>
+        <v>38451</v>
       </c>
       <c r="C25" t="s">
-        <v>38119</v>
+        <v>38479</v>
       </c>
       <c r="D25" s="1">
         <v>0.69999998807907104</v>
@@ -117172,24 +118252,24 @@
         <v>0.87000000476837158</v>
       </c>
       <c r="G25" t="s">
-        <v>38133</v>
+        <v>38493</v>
       </c>
       <c r="H25" t="s">
-        <v>38151</v>
+        <v>38511</v>
       </c>
       <c r="I25" t="s">
-        <v>38184</v>
+        <v>38544</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>38056</v>
+        <v>38416</v>
       </c>
       <c r="B26" t="s">
-        <v>38092</v>
+        <v>38452</v>
       </c>
       <c r="C26" t="s">
-        <v>38119</v>
+        <v>38479</v>
       </c>
       <c r="D26" s="1">
         <v>0.38999998569488525</v>
@@ -117201,24 +118281,24 @@
         <v>0.68999999761581421</v>
       </c>
       <c r="G26" t="s">
-        <v>38133</v>
+        <v>38493</v>
       </c>
       <c r="H26" t="s">
-        <v>38152</v>
+        <v>38512</v>
       </c>
       <c r="I26" t="s">
-        <v>38185</v>
+        <v>38545</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>38056</v>
+        <v>38416</v>
       </c>
       <c r="B27" t="s">
-        <v>38093</v>
+        <v>38453</v>
       </c>
       <c r="C27" t="s">
-        <v>38119</v>
+        <v>38479</v>
       </c>
       <c r="D27" s="1">
         <v>0.15999999642372131</v>
@@ -117230,24 +118310,24 @@
         <v>0.40000000596046448</v>
       </c>
       <c r="G27" t="s">
-        <v>38133</v>
+        <v>38493</v>
       </c>
       <c r="H27" t="s">
-        <v>38152</v>
+        <v>38512</v>
       </c>
       <c r="I27" t="s">
-        <v>38186</v>
+        <v>38546</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>38057</v>
+        <v>38417</v>
       </c>
       <c r="B28" t="s">
-        <v>38094</v>
+        <v>38454</v>
       </c>
       <c r="C28" t="s">
-        <v>38119</v>
+        <v>38479</v>
       </c>
       <c r="D28" s="1">
         <v>0.46000000834465027</v>
@@ -117259,24 +118339,24 @@
         <v>0.6600000262260437</v>
       </c>
       <c r="G28" t="s">
-        <v>38133</v>
+        <v>38493</v>
       </c>
       <c r="H28" t="s">
-        <v>38152</v>
+        <v>38512</v>
       </c>
       <c r="I28" t="s">
-        <v>38187</v>
+        <v>38547</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>38057</v>
+        <v>38417</v>
       </c>
       <c r="B29" t="s">
-        <v>38095</v>
+        <v>38455</v>
       </c>
       <c r="C29" t="s">
-        <v>38119</v>
+        <v>38479</v>
       </c>
       <c r="D29" s="1">
         <v>0.30000001192092896</v>
@@ -117288,24 +118368,24 @@
         <v>0.44999998807907104</v>
       </c>
       <c r="G29" t="s">
-        <v>38133</v>
+        <v>38493</v>
       </c>
       <c r="H29" t="s">
-        <v>38152</v>
+        <v>38512</v>
       </c>
       <c r="I29" t="s">
-        <v>38188</v>
+        <v>38548</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>38058</v>
+        <v>38418</v>
       </c>
       <c r="B30" t="s">
-        <v>38096</v>
+        <v>38456</v>
       </c>
       <c r="C30" t="s">
-        <v>38119</v>
+        <v>38479</v>
       </c>
       <c r="D30" s="1">
         <v>0.60000002384185791</v>
@@ -117317,24 +118397,24 @@
         <v>1.059999942779541</v>
       </c>
       <c r="G30" t="s">
-        <v>38133</v>
+        <v>38493</v>
       </c>
       <c r="H30" t="s">
-        <v>38153</v>
+        <v>38513</v>
       </c>
       <c r="I30" t="s">
-        <v>38189</v>
+        <v>38549</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>38058</v>
+        <v>38418</v>
       </c>
       <c r="B31" t="s">
-        <v>38097</v>
+        <v>38457</v>
       </c>
       <c r="C31" t="s">
-        <v>38119</v>
+        <v>38479</v>
       </c>
       <c r="D31" s="1">
         <v>0.47999998927116394</v>
@@ -117346,24 +118426,24 @@
         <v>0.81999999284744263</v>
       </c>
       <c r="G31" t="s">
-        <v>38133</v>
+        <v>38493</v>
       </c>
       <c r="H31" t="s">
-        <v>38153</v>
+        <v>38513</v>
       </c>
       <c r="I31" t="s">
-        <v>38190</v>
+        <v>38550</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>38059</v>
+        <v>38419</v>
       </c>
       <c r="B32" t="s">
-        <v>38098</v>
+        <v>38458</v>
       </c>
       <c r="C32" t="s">
-        <v>38119</v>
+        <v>38479</v>
       </c>
       <c r="D32" s="1">
         <v>1.6200000047683716</v>
@@ -117375,24 +118455,24 @@
         <v>2.4100000858306885</v>
       </c>
       <c r="G32" t="s">
-        <v>38133</v>
+        <v>38493</v>
       </c>
       <c r="H32" t="s">
-        <v>38153</v>
+        <v>38513</v>
       </c>
       <c r="I32" t="s">
-        <v>38191</v>
+        <v>38551</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>38059</v>
+        <v>38419</v>
       </c>
       <c r="B33" t="s">
-        <v>38099</v>
+        <v>38459</v>
       </c>
       <c r="C33" t="s">
-        <v>38119</v>
+        <v>38479</v>
       </c>
       <c r="D33" s="1">
         <v>2.0099999904632568</v>
@@ -117404,24 +118484,24 @@
         <v>2.8399999141693115</v>
       </c>
       <c r="G33" t="s">
-        <v>38133</v>
+        <v>38493</v>
       </c>
       <c r="H33" t="s">
-        <v>38153</v>
+        <v>38513</v>
       </c>
       <c r="I33" t="s">
-        <v>38192</v>
+        <v>38552</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>38060</v>
+        <v>38420</v>
       </c>
       <c r="B34" t="s">
-        <v>38100</v>
+        <v>38460</v>
       </c>
       <c r="C34" t="s">
-        <v>38120</v>
+        <v>38480</v>
       </c>
       <c r="D34" s="1">
         <v>0.95999997854232788</v>
@@ -117433,24 +118513,24 @@
         <v>1.2560000419616699</v>
       </c>
       <c r="G34" t="s">
-        <v>38134</v>
+        <v>38494</v>
       </c>
       <c r="H34" t="s">
-        <v>38154</v>
+        <v>38514</v>
       </c>
       <c r="I34" t="s">
-        <v>38193</v>
+        <v>38553</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>38060</v>
+        <v>38420</v>
       </c>
       <c r="B35" t="s">
-        <v>38101</v>
+        <v>38461</v>
       </c>
       <c r="C35" t="s">
-        <v>38120</v>
+        <v>38480</v>
       </c>
       <c r="D35" s="1">
         <v>1.0800000429153442</v>
@@ -117462,24 +118542,24 @@
         <v>1.3609999418258667</v>
       </c>
       <c r="G35" t="s">
-        <v>38134</v>
+        <v>38494</v>
       </c>
       <c r="H35" t="s">
-        <v>38154</v>
+        <v>38514</v>
       </c>
       <c r="I35" t="s">
-        <v>38194</v>
+        <v>38554</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>38061</v>
+        <v>38421</v>
       </c>
       <c r="B36" t="s">
-        <v>38102</v>
+        <v>38462</v>
       </c>
       <c r="C36" t="s">
-        <v>38120</v>
+        <v>38480</v>
       </c>
       <c r="D36" s="1">
         <v>0.87699997425079346</v>
@@ -117491,24 +118571,24 @@
         <v>1.156000018119812</v>
       </c>
       <c r="G36" t="s">
-        <v>38135</v>
+        <v>38495</v>
       </c>
       <c r="H36" t="s">
-        <v>38155</v>
+        <v>38515</v>
       </c>
       <c r="I36" t="s">
-        <v>38195</v>
+        <v>38555</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>38061</v>
+        <v>38421</v>
       </c>
       <c r="B37" t="s">
-        <v>38103</v>
+        <v>38463</v>
       </c>
       <c r="C37" t="s">
-        <v>38120</v>
+        <v>38480</v>
       </c>
       <c r="D37" s="1">
         <v>0.68400001525878906</v>
@@ -117520,24 +118600,24 @@
         <v>0.875</v>
       </c>
       <c r="G37" t="s">
-        <v>38135</v>
+        <v>38495</v>
       </c>
       <c r="H37" t="s">
-        <v>38155</v>
+        <v>38515</v>
       </c>
       <c r="I37" t="s">
-        <v>38196</v>
+        <v>38556</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>38061</v>
+        <v>38421</v>
       </c>
       <c r="B38" t="s">
-        <v>38104</v>
+        <v>38464</v>
       </c>
       <c r="C38" t="s">
-        <v>38120</v>
+        <v>38480</v>
       </c>
       <c r="D38" s="1">
         <v>0.85699999332427979</v>
@@ -117549,24 +118629,24 @@
         <v>1.1779999732971191</v>
       </c>
       <c r="G38" t="s">
-        <v>38135</v>
+        <v>38495</v>
       </c>
       <c r="H38" t="s">
-        <v>38155</v>
+        <v>38515</v>
       </c>
       <c r="I38" t="s">
-        <v>38197</v>
+        <v>38557</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>38062</v>
+        <v>38422</v>
       </c>
       <c r="B39" t="s">
-        <v>38104</v>
+        <v>38464</v>
       </c>
       <c r="C39" t="s">
-        <v>38121</v>
+        <v>38481</v>
       </c>
       <c r="D39" s="1">
         <v>0.64999997615814209</v>
@@ -117578,24 +118658,24 @@
         <v>0.8399999737739563</v>
       </c>
       <c r="G39" t="s">
-        <v>38136</v>
+        <v>38496</v>
       </c>
       <c r="H39" t="s">
-        <v>38155</v>
+        <v>38515</v>
       </c>
       <c r="I39" t="s">
-        <v>38198</v>
+        <v>38558</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>38062</v>
+        <v>38422</v>
       </c>
       <c r="B40" t="s">
-        <v>38105</v>
+        <v>38465</v>
       </c>
       <c r="C40" t="s">
-        <v>38121</v>
+        <v>38481</v>
       </c>
       <c r="D40" s="1">
         <v>0.47999998927116394</v>
@@ -117607,24 +118687,24 @@
         <v>0.75</v>
       </c>
       <c r="G40" t="s">
-        <v>38136</v>
+        <v>38496</v>
       </c>
       <c r="H40" t="s">
-        <v>38155</v>
+        <v>38515</v>
       </c>
       <c r="I40" t="s">
-        <v>38199</v>
+        <v>38559</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>38063</v>
+        <v>38423</v>
       </c>
       <c r="B41" t="s">
-        <v>38106</v>
+        <v>38466</v>
       </c>
       <c r="C41" t="s">
-        <v>38122</v>
+        <v>38482</v>
       </c>
       <c r="D41" s="1">
         <v>0.78100001811981201</v>
@@ -117636,24 +118716,24 @@
         <v>1.3220000267028809</v>
       </c>
       <c r="G41" t="s">
-        <v>38137</v>
+        <v>38497</v>
       </c>
       <c r="H41" t="s">
-        <v>38156</v>
+        <v>38516</v>
       </c>
       <c r="I41" t="s">
-        <v>38200</v>
+        <v>38560</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>38063</v>
+        <v>38423</v>
       </c>
       <c r="B42" t="s">
-        <v>38107</v>
+        <v>38467</v>
       </c>
       <c r="C42" t="s">
-        <v>38122</v>
+        <v>38482</v>
       </c>
       <c r="D42" s="1">
         <v>0.97500002384185791</v>
@@ -117665,24 +118745,24 @@
         <v>1.1829999685287476</v>
       </c>
       <c r="G42" t="s">
-        <v>38137</v>
+        <v>38497</v>
       </c>
       <c r="H42" t="s">
-        <v>38156</v>
+        <v>38516</v>
       </c>
       <c r="I42" t="s">
-        <v>38201</v>
+        <v>38561</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>38064</v>
+        <v>38424</v>
       </c>
       <c r="B43" t="s">
-        <v>38108</v>
+        <v>38468</v>
       </c>
       <c r="C43" t="s">
-        <v>38122</v>
+        <v>38482</v>
       </c>
       <c r="D43" s="1">
         <v>0.93999999761581421</v>
@@ -117694,24 +118774,24 @@
         <v>1.190000057220459</v>
       </c>
       <c r="G43" t="s">
-        <v>38138</v>
+        <v>38498</v>
       </c>
       <c r="H43" t="s">
-        <v>38157</v>
+        <v>38517</v>
       </c>
       <c r="I43" t="s">
-        <v>38202</v>
+        <v>38562</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>38064</v>
+        <v>38424</v>
       </c>
       <c r="B44" t="s">
-        <v>38109</v>
+        <v>38469</v>
       </c>
       <c r="C44" t="s">
-        <v>38122</v>
+        <v>38482</v>
       </c>
       <c r="D44" s="1">
         <v>0.93000000715255737</v>
@@ -117723,24 +118803,24 @@
         <v>1.309999942779541</v>
       </c>
       <c r="G44" t="s">
-        <v>38138</v>
+        <v>38498</v>
       </c>
       <c r="H44" t="s">
-        <v>38157</v>
+        <v>38517</v>
       </c>
       <c r="I44" t="s">
-        <v>38203</v>
+        <v>38563</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>38065</v>
+        <v>38425</v>
       </c>
       <c r="B45" t="s">
-        <v>38110</v>
+        <v>38470</v>
       </c>
       <c r="C45" t="s">
-        <v>38123</v>
+        <v>38483</v>
       </c>
       <c r="D45" s="1">
         <v>0.63999998569488525</v>
@@ -117752,24 +118832,24 @@
         <v>0.9100000262260437</v>
       </c>
       <c r="G45" t="s">
-        <v>38138</v>
+        <v>38498</v>
       </c>
       <c r="H45" t="s">
-        <v>38158</v>
+        <v>38518</v>
       </c>
       <c r="I45" t="s">
-        <v>38204</v>
+        <v>38564</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>38065</v>
+        <v>38425</v>
       </c>
       <c r="B46" t="s">
-        <v>38111</v>
+        <v>38471</v>
       </c>
       <c r="C46" t="s">
-        <v>38123</v>
+        <v>38483</v>
       </c>
       <c r="D46" s="1">
         <v>0.72000002861022949</v>
@@ -117781,24 +118861,24 @@
         <v>0.89999997615814209</v>
       </c>
       <c r="G46" t="s">
-        <v>38138</v>
+        <v>38498</v>
       </c>
       <c r="H46" t="s">
-        <v>38158</v>
+        <v>38518</v>
       </c>
       <c r="I46" t="s">
-        <v>38205</v>
+        <v>38565</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>38066</v>
+        <v>38426</v>
       </c>
       <c r="B47" t="s">
-        <v>38112</v>
+        <v>38472</v>
       </c>
       <c r="C47" t="s">
-        <v>38123</v>
+        <v>38483</v>
       </c>
       <c r="D47" s="1">
         <v>0.46000000834465027</v>
@@ -117810,24 +118890,24 @@
         <v>0.73000001907348633</v>
       </c>
       <c r="G47" t="s">
-        <v>38138</v>
+        <v>38498</v>
       </c>
       <c r="H47" t="s">
-        <v>38159</v>
+        <v>38519</v>
       </c>
       <c r="I47" t="s">
-        <v>38206</v>
+        <v>38566</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>38066</v>
+        <v>38426</v>
       </c>
       <c r="B48" t="s">
-        <v>38113</v>
+        <v>38473</v>
       </c>
       <c r="C48" t="s">
-        <v>38123</v>
+        <v>38483</v>
       </c>
       <c r="D48" s="1">
         <v>0.62999999523162842</v>
@@ -117839,13 +118919,13 @@
         <v>0.89999997615814209</v>
       </c>
       <c r="G48" t="s">
-        <v>38138</v>
+        <v>38498</v>
       </c>
       <c r="H48" t="s">
-        <v>38159</v>
+        <v>38519</v>
       </c>
       <c r="I48" t="s">
-        <v>38207</v>
+        <v>38567</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data with whether a trial could report a stratified estimate
</commit_message>
<xml_diff>
--- a/products/Exported Data.xlsx
+++ b/products/Exported Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67075" uniqueCount="39288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67695" uniqueCount="39648">
   <si>
     <t>Study</t>
   </si>
@@ -101537,6 +101537,1086 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Study: Treatment 1 vs Treatment 2</t>
+  </si>
+  <si>
+    <t>Attal 2019 (ICARIA-MM): IsPd vs Pd</t>
+  </si>
+  <si>
+    <t>Bahlis 2020 (POLLUX): DRd vs Rd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2013 (VANTAGE 088): VorV vs V</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2016 (ENDEAVOR): Kd vs Vd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2018 (ELOQUENT-3): EPd vs Pd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2018 (ELOQUENT-2): ELd vs Ld</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2020 (ELOQUENT-2): ELd vs Ld</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2021 (APOLLO): DPd vs Pd</t>
+  </si>
+  <si>
+    <t>Grosicki 2020 (BOSTON): SeVd vs Vd</t>
+  </si>
+  <si>
+    <t>Hou 2017 (China Cont.): IRd vs Rd</t>
+  </si>
+  <si>
+    <t>Jakubowiak 2016 (NCT01478048): EVd vs Vd</t>
+  </si>
+  <si>
+    <t>Kumar 2020 (BELLINI): VeVd vs Vd</t>
+  </si>
+  <si>
+    <t>Lu 2021 (LEPUS): DVd vs Vd</t>
+  </si>
+  <si>
+    <t>Mateos 2020 (CASTOR): DVd vs Vd</t>
+  </si>
+  <si>
+    <t>Moreau 2021 (IKEMA): IsKd vs Kd</t>
+  </si>
+  <si>
+    <t>Orlowski 2019 (ENDEAVOR): Kd vs Vd</t>
+  </si>
+  <si>
+    <t>Richardson 2019 (OPTIMISMM): PVd vs Vd</t>
+  </si>
+  <si>
+    <t>Richardson 2021 (TOURMALINE-MM1): IRd vs Rd</t>
+  </si>
+  <si>
+    <t>San-Miguel 2014 (PANORAMA-1): FVd vs Vd</t>
+  </si>
+  <si>
+    <t>San-Miguel 2016 (PANORAMA 1): FVd vs Vd</t>
+  </si>
+  <si>
+    <t>San-Miguel 2013 (MM-003): Pd vs GC</t>
+  </si>
+  <si>
+    <t>Siegel 2018 (ASPIRE): KRd vs Rd</t>
+  </si>
+  <si>
+    <t>Usamani 2022 (CANDOR): DKd vs Kd</t>
+  </si>
+  <si>
+    <t>lot</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>&gt;3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>&gt;3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>&gt;=4</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>&gt;=4</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>&gt;3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>&gt;3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>&gt;1</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>&gt;2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>&gt;=3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>&gt;2</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>&gt;2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>&gt;=2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>Outcome</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Lower 95% CI Bound on HR</t>
+  </si>
+  <si>
+    <t>Upper 95% CI Bound on HR</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t>Tab. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tab. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      p. 808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. S3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. S4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      AT 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      p. 730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t>Data Extraction Errors</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Study: Treatment 1 vs Treatment 2</t>
+  </si>
+  <si>
+    <t>Attal 2019 (ICARIA-MM): IsPd vs Pd</t>
+  </si>
+  <si>
+    <t>Bahlis 2020 (POLLUX): DRd vs Rd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2013 (VANTAGE 088): VorV vs V</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2016 (ENDEAVOR): Kd vs Vd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2018 (ELOQUENT-3): EPd vs Pd</t>
+  </si>
+  <si>
+    <t>Dimopoulos 2021 (APOLLO): DPd vs Pd</t>
+  </si>
+  <si>
+    <t>Hou 2017 (China Cont.): IRd vs Rd</t>
+  </si>
+  <si>
+    <t>Jakubowiak 2016 (NCT01478048): EVd vs Vd</t>
+  </si>
+  <si>
+    <t>Kumar 2020 (BELLINI): VeVd vs Vd</t>
+  </si>
+  <si>
+    <t>Lonial 2015 (ELOQUENT-2): ELd vs Ld</t>
+  </si>
+  <si>
+    <t>Lu 2021 (LEPUS): DVd vs Vd</t>
+  </si>
+  <si>
+    <t>Mateos 2020 (CASTOR): DVd vs Vd</t>
+  </si>
+  <si>
+    <t>Moreau 2021 (IKEMA): IsKd vs Kd</t>
+  </si>
+  <si>
+    <t>Orlowski 2007 (NCT00103506): V vs DoxV</t>
+  </si>
+  <si>
+    <t>Orlowski 2016 (NCT00103506): V vs DoxV</t>
+  </si>
+  <si>
+    <t>Orlowski 2019 (ENDEAVOR): Kd vs Vd</t>
+  </si>
+  <si>
+    <t>Richardson 2019 (OPTIMISMM): PVd vs Vd</t>
+  </si>
+  <si>
+    <t>Richardson 2021 (TOURMALINE-MM1): IRd vs Rd</t>
+  </si>
+  <si>
+    <t>San-Miguel 2016 (PANORAMA 1): FVd vs Vd</t>
+  </si>
+  <si>
+    <t>Stewart 2015 (ASPIRE): KRd vs Rd</t>
+  </si>
+  <si>
+    <t>Usmani 2022 (CANDOR): DKd vs Kd</t>
+  </si>
+  <si>
+    <t>refract</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Previous R use</t>
+  </si>
+  <si>
+    <t>No previous R use</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No IMiD use</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Ref. to R and a PI</t>
+  </si>
+  <si>
+    <t>Not ref. to R and a PI</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No IMiD use</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No IMiD use</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No IMiD use</t>
+  </si>
+  <si>
+    <t>Naive</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Naive</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Previous R use</t>
+  </si>
+  <si>
+    <t>No previous R use</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Not refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Not refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Previous R or T use</t>
+  </si>
+  <si>
+    <t>No previous R or T use</t>
+  </si>
+  <si>
+    <t>Previous R or T use</t>
+  </si>
+  <si>
+    <t>No previous R or T use</t>
+  </si>
+  <si>
+    <t>Previous R use</t>
+  </si>
+  <si>
+    <t>No previous R use</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Refractory to T</t>
+  </si>
+  <si>
+    <t>Not refractory to T</t>
+  </si>
+  <si>
+    <t>Previous IMiD use</t>
+  </si>
+  <si>
+    <t>No previous IMiD use</t>
+  </si>
+  <si>
+    <t>Refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Not refractory to IMiD</t>
+  </si>
+  <si>
+    <t>Refractory to R</t>
+  </si>
+  <si>
+    <t>Not refractory to R</t>
+  </si>
+  <si>
+    <t>Outcome</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>PFS</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Lower 95% CI Bound on HR</t>
+  </si>
+  <si>
+    <t>Upper 95% CI Bound on HR</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0230</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .       Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  .</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tab. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      p. 808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. S3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. S4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fig. 3</t>
+  </si>
+  <si>
+    <t>Data Extraction Errors</t>
   </si>
   <si>
     <t/>
@@ -117928,42 +119008,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>38928</v>
+        <v>39288</v>
       </c>
       <c r="B1" t="s">
-        <v>38952</v>
+        <v>39312</v>
       </c>
       <c r="C1" t="s">
-        <v>39016</v>
+        <v>39376</v>
       </c>
       <c r="D1" t="s">
-        <v>39032</v>
+        <v>39392</v>
       </c>
       <c r="E1" t="s">
-        <v>39033</v>
+        <v>39393</v>
       </c>
       <c r="F1" t="s">
-        <v>39034</v>
+        <v>39394</v>
       </c>
       <c r="G1" t="s">
-        <v>39035</v>
+        <v>39395</v>
       </c>
       <c r="H1" t="s">
-        <v>39036</v>
+        <v>39396</v>
       </c>
       <c r="I1" t="s">
-        <v>39060</v>
+        <v>39420</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>38929</v>
+        <v>39289</v>
       </c>
       <c r="B2" t="s">
-        <v>38953</v>
+        <v>39313</v>
       </c>
       <c r="C2" t="s">
-        <v>39017</v>
+        <v>39377</v>
       </c>
       <c r="D2" s="1">
         <v>0.5899999737739563</v>
@@ -117976,21 +119056,21 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" t="s">
-        <v>39037</v>
+        <v>39397</v>
       </c>
       <c r="I2" t="s">
-        <v>39061</v>
+        <v>39421</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>38929</v>
+        <v>39289</v>
       </c>
       <c r="B3" t="s">
-        <v>38954</v>
+        <v>39314</v>
       </c>
       <c r="C3" t="s">
-        <v>39017</v>
+        <v>39377</v>
       </c>
       <c r="D3" s="1">
         <v>0.5899999737739563</v>
@@ -118003,21 +119083,21 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" t="s">
-        <v>39037</v>
+        <v>39397</v>
       </c>
       <c r="I3" t="s">
-        <v>39062</v>
+        <v>39422</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>38930</v>
+        <v>39290</v>
       </c>
       <c r="B4" t="s">
-        <v>38955</v>
+        <v>39315</v>
       </c>
       <c r="C4" t="s">
-        <v>39017</v>
+        <v>39377</v>
       </c>
       <c r="D4" s="1">
         <v>0.41999998688697815</v>
@@ -118030,21 +119110,21 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" t="s">
-        <v>39038</v>
+        <v>39398</v>
       </c>
       <c r="I4" t="s">
-        <v>39063</v>
+        <v>39423</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>38930</v>
+        <v>39290</v>
       </c>
       <c r="B5" t="s">
-        <v>38956</v>
+        <v>39316</v>
       </c>
       <c r="C5" t="s">
-        <v>39017</v>
+        <v>39377</v>
       </c>
       <c r="D5" s="1">
         <v>0.38999998569488525</v>
@@ -118057,21 +119137,21 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" t="s">
-        <v>39038</v>
+        <v>39398</v>
       </c>
       <c r="I5" t="s">
-        <v>39064</v>
+        <v>39424</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>38930</v>
+        <v>39290</v>
       </c>
       <c r="B6" t="s">
-        <v>38957</v>
+        <v>39317</v>
       </c>
       <c r="C6" t="s">
-        <v>39017</v>
+        <v>39377</v>
       </c>
       <c r="D6" s="1">
         <v>0.47999998927116394</v>
@@ -118084,21 +119164,21 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" t="s">
-        <v>39038</v>
+        <v>39398</v>
       </c>
       <c r="I6" t="s">
-        <v>39065</v>
+        <v>39425</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>38930</v>
+        <v>39290</v>
       </c>
       <c r="B7" t="s">
-        <v>38958</v>
+        <v>39318</v>
       </c>
       <c r="C7" t="s">
-        <v>39017</v>
+        <v>39377</v>
       </c>
       <c r="D7" s="1">
         <v>0.74000000953674316</v>
@@ -118111,21 +119191,21 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" t="s">
-        <v>39038</v>
+        <v>39398</v>
       </c>
       <c r="I7" t="s">
-        <v>39066</v>
+        <v>39426</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>38931</v>
+        <v>39291</v>
       </c>
       <c r="B8" t="s">
-        <v>38959</v>
+        <v>39319</v>
       </c>
       <c r="C8" t="s">
-        <v>39017</v>
+        <v>39377</v>
       </c>
       <c r="D8" s="1">
         <v>0.68699997663497925</v>
@@ -118140,21 +119220,21 @@
         <v>0.015200000256299973</v>
       </c>
       <c r="H8" t="s">
-        <v>39039</v>
+        <v>39399</v>
       </c>
       <c r="I8" t="s">
-        <v>39067</v>
+        <v>39427</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>38931</v>
+        <v>39291</v>
       </c>
       <c r="B9" t="s">
-        <v>38960</v>
+        <v>39320</v>
       </c>
       <c r="C9" t="s">
-        <v>39017</v>
+        <v>39377</v>
       </c>
       <c r="D9" s="1">
         <v>0.91600000858306885</v>
@@ -118169,21 +119249,21 @@
         <v>0.48710000514984131</v>
       </c>
       <c r="H9" t="s">
-        <v>39040</v>
+        <v>39400</v>
       </c>
       <c r="I9" t="s">
-        <v>39068</v>
+        <v>39428</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>38932</v>
+        <v>39292</v>
       </c>
       <c r="B10" t="s">
-        <v>38961</v>
+        <v>39321</v>
       </c>
       <c r="C10" t="s">
-        <v>39017</v>
+        <v>39377</v>
       </c>
       <c r="D10" s="1">
         <v>0.44999998807907104</v>
@@ -118196,21 +119276,21 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" t="s">
-        <v>39041</v>
+        <v>39401</v>
       </c>
       <c r="I10" t="s">
-        <v>39069</v>
+        <v>39429</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>38932</v>
+        <v>39292</v>
       </c>
       <c r="B11" t="s">
-        <v>38962</v>
+        <v>39322</v>
       </c>
       <c r="C11" t="s">
-        <v>39017</v>
+        <v>39377</v>
       </c>
       <c r="D11" s="1">
         <v>0.60000002384185791</v>
@@ -118223,21 +119303,21 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" t="s">
-        <v>39041</v>
+        <v>39401</v>
       </c>
       <c r="I11" t="s">
-        <v>39070</v>
+        <v>39430</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>38933</v>
+        <v>39293</v>
       </c>
       <c r="B12" t="s">
-        <v>38962</v>
+        <v>39322</v>
       </c>
       <c r="C12" t="s">
-        <v>39017</v>
+        <v>39377</v>
       </c>
       <c r="D12" s="1">
         <v>0.55000001192092896</v>
@@ -118250,21 +119330,21 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" t="s">
-        <v>39042</v>
+        <v>39402</v>
       </c>
       <c r="I12" t="s">
-        <v>39071</v>
+        <v>39431</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>38933</v>
+        <v>39293</v>
       </c>
       <c r="B13" t="s">
-        <v>38963</v>
+        <v>39323</v>
       </c>
       <c r="C13" t="s">
-        <v>39017</v>
+        <v>39377</v>
       </c>
       <c r="D13" s="1">
         <v>0.50999999046325684</v>
@@ -118277,21 +119357,21 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" t="s">
-        <v>39042</v>
+        <v>39402</v>
       </c>
       <c r="I13" t="s">
-        <v>39072</v>
+        <v>39432</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>38934</v>
+        <v>39294</v>
       </c>
       <c r="B14" t="s">
-        <v>38964</v>
+        <v>39324</v>
       </c>
       <c r="C14" t="s">
-        <v>39017</v>
+        <v>39377</v>
       </c>
       <c r="D14" s="1">
         <v>0.76999998092651367</v>
@@ -118304,21 +119384,21 @@
       </c>
       <c r="G14" s="1"/>
       <c r="H14" t="s">
-        <v>39043</v>
+        <v>39403</v>
       </c>
       <c r="I14" t="s">
-        <v>39073</v>
+        <v>39433</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>38934</v>
+        <v>39294</v>
       </c>
       <c r="B15" t="s">
-        <v>38965</v>
+        <v>39325</v>
       </c>
       <c r="C15" t="s">
-        <v>39017</v>
+        <v>39377</v>
       </c>
       <c r="D15" s="1">
         <v>0.68000000715255737</v>
@@ -118331,21 +119411,21 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15" t="s">
-        <v>39043</v>
+        <v>39403</v>
       </c>
       <c r="I15" t="s">
-        <v>39074</v>
+        <v>39434</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>38935</v>
+        <v>39295</v>
       </c>
       <c r="B16" t="s">
-        <v>38966</v>
+        <v>39326</v>
       </c>
       <c r="C16" t="s">
-        <v>39018</v>
+        <v>39378</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
@@ -118358,21 +119438,21 @@
       </c>
       <c r="G16" s="1"/>
       <c r="H16" t="s">
-        <v>39043</v>
+        <v>39403</v>
       </c>
       <c r="I16" t="s">
-        <v>39075</v>
+        <v>39435</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>38935</v>
+        <v>39295</v>
       </c>
       <c r="B17" t="s">
-        <v>38967</v>
+        <v>39327</v>
       </c>
       <c r="C17" t="s">
-        <v>39018</v>
+        <v>39378</v>
       </c>
       <c r="D17" s="1">
         <v>0.70999997854232788</v>
@@ -118385,21 +119465,21 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" t="s">
-        <v>39043</v>
+        <v>39403</v>
       </c>
       <c r="I17" t="s">
-        <v>39076</v>
+        <v>39436</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>38936</v>
+        <v>39296</v>
       </c>
       <c r="B18" t="s">
-        <v>38968</v>
+        <v>39328</v>
       </c>
       <c r="C18" t="s">
-        <v>39019</v>
+        <v>39379</v>
       </c>
       <c r="D18" s="1">
         <v>0.69999998807907104</v>
@@ -118412,21 +119492,21 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" t="s">
-        <v>39044</v>
+        <v>39404</v>
       </c>
       <c r="I18" t="s">
-        <v>39077</v>
+        <v>39437</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>38936</v>
+        <v>39296</v>
       </c>
       <c r="B19" t="s">
-        <v>38969</v>
+        <v>39329</v>
       </c>
       <c r="C19" t="s">
-        <v>39019</v>
+        <v>39379</v>
       </c>
       <c r="D19" s="1">
         <v>0.6600000262260437</v>
@@ -118439,21 +119519,21 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19" t="s">
-        <v>39044</v>
+        <v>39404</v>
       </c>
       <c r="I19" t="s">
-        <v>39078</v>
+        <v>39438</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>38936</v>
+        <v>39296</v>
       </c>
       <c r="B20" t="s">
-        <v>38970</v>
+        <v>39330</v>
       </c>
       <c r="C20" t="s">
-        <v>39019</v>
+        <v>39379</v>
       </c>
       <c r="D20" s="1">
         <v>0.40000000596046448</v>
@@ -118466,21 +119546,21 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" t="s">
-        <v>39044</v>
+        <v>39404</v>
       </c>
       <c r="I20" t="s">
-        <v>39079</v>
+        <v>39439</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>38937</v>
+        <v>39297</v>
       </c>
       <c r="B21" t="s">
-        <v>38971</v>
+        <v>39331</v>
       </c>
       <c r="C21" t="s">
-        <v>39019</v>
+        <v>39379</v>
       </c>
       <c r="D21" s="1">
         <v>0.62999999523162842</v>
@@ -118493,21 +119573,21 @@
       </c>
       <c r="G21" s="1"/>
       <c r="H21" t="s">
-        <v>39045</v>
+        <v>39405</v>
       </c>
       <c r="I21" t="s">
-        <v>39080</v>
+        <v>39440</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>38937</v>
+        <v>39297</v>
       </c>
       <c r="B22" t="s">
-        <v>38972</v>
+        <v>39332</v>
       </c>
       <c r="C22" t="s">
-        <v>39019</v>
+        <v>39379</v>
       </c>
       <c r="D22" s="1">
         <v>0.64999997615814209</v>
@@ -118520,21 +119600,21 @@
       </c>
       <c r="G22" s="1"/>
       <c r="H22" t="s">
-        <v>39045</v>
+        <v>39405</v>
       </c>
       <c r="I22" t="s">
-        <v>39081</v>
+        <v>39441</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>38937</v>
+        <v>39297</v>
       </c>
       <c r="B23" t="s">
-        <v>38973</v>
+        <v>39333</v>
       </c>
       <c r="C23" t="s">
-        <v>39019</v>
+        <v>39379</v>
       </c>
       <c r="D23" s="1">
         <v>0.81999999284744263</v>
@@ -118547,21 +119627,21 @@
       </c>
       <c r="G23" s="1"/>
       <c r="H23" t="s">
-        <v>39045</v>
+        <v>39405</v>
       </c>
       <c r="I23" t="s">
-        <v>39082</v>
+        <v>39442</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>38938</v>
+        <v>39298</v>
       </c>
       <c r="B24" t="s">
-        <v>38974</v>
+        <v>39334</v>
       </c>
       <c r="C24" t="s">
-        <v>39019</v>
+        <v>39379</v>
       </c>
       <c r="D24" s="1">
         <v>0.84700000286102295</v>
@@ -118574,21 +119654,21 @@
       </c>
       <c r="G24" s="1"/>
       <c r="H24" t="s">
-        <v>39046</v>
+        <v>39406</v>
       </c>
       <c r="I24" t="s">
-        <v>39083</v>
+        <v>39443</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>38938</v>
+        <v>39298</v>
       </c>
       <c r="B25" t="s">
-        <v>38975</v>
+        <v>39335</v>
       </c>
       <c r="C25" t="s">
-        <v>39019</v>
+        <v>39379</v>
       </c>
       <c r="D25" s="1">
         <v>0.37000000476837158</v>
@@ -118601,21 +119681,21 @@
       </c>
       <c r="G25" s="1"/>
       <c r="H25" t="s">
-        <v>39046</v>
+        <v>39406</v>
       </c>
       <c r="I25" t="s">
-        <v>39084</v>
+        <v>39444</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>38938</v>
+        <v>39298</v>
       </c>
       <c r="B26" t="s">
-        <v>38976</v>
+        <v>39336</v>
       </c>
       <c r="C26" t="s">
-        <v>39019</v>
+        <v>39379</v>
       </c>
       <c r="D26" s="1">
         <v>0.70200002193450928</v>
@@ -118628,21 +119708,21 @@
       </c>
       <c r="G26" s="1"/>
       <c r="H26" t="s">
-        <v>39046</v>
+        <v>39406</v>
       </c>
       <c r="I26" t="s">
-        <v>39085</v>
+        <v>39445</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>38938</v>
+        <v>39298</v>
       </c>
       <c r="B27" t="s">
-        <v>38977</v>
+        <v>39337</v>
       </c>
       <c r="C27" t="s">
-        <v>39020</v>
+        <v>39380</v>
       </c>
       <c r="D27" s="1">
         <v>0.52100002765655518</v>
@@ -118655,21 +119735,21 @@
       </c>
       <c r="G27" s="1"/>
       <c r="H27" t="s">
-        <v>39047</v>
+        <v>39407</v>
       </c>
       <c r="I27" t="s">
-        <v>39086</v>
+        <v>39446</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>38938</v>
+        <v>39298</v>
       </c>
       <c r="B28" t="s">
-        <v>38978</v>
+        <v>39338</v>
       </c>
       <c r="C28" t="s">
-        <v>39020</v>
+        <v>39380</v>
       </c>
       <c r="D28" s="1">
         <v>0.38600000739097595</v>
@@ -118682,21 +119762,21 @@
       </c>
       <c r="G28" s="1"/>
       <c r="H28" t="s">
-        <v>39047</v>
+        <v>39407</v>
       </c>
       <c r="I28" t="s">
-        <v>39087</v>
+        <v>39447</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>38938</v>
+        <v>39298</v>
       </c>
       <c r="B29" t="s">
-        <v>38979</v>
+        <v>39339</v>
       </c>
       <c r="C29" t="s">
-        <v>39020</v>
+        <v>39380</v>
       </c>
       <c r="D29" s="1">
         <v>0.335999995470047</v>
@@ -118709,21 +119789,21 @@
       </c>
       <c r="G29" s="1"/>
       <c r="H29" t="s">
-        <v>39047</v>
+        <v>39407</v>
       </c>
       <c r="I29" t="s">
-        <v>39088</v>
+        <v>39448</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>38939</v>
+        <v>39299</v>
       </c>
       <c r="B30" t="s">
-        <v>38980</v>
+        <v>39340</v>
       </c>
       <c r="C30" t="s">
-        <v>39021</v>
+        <v>39381</v>
       </c>
       <c r="D30" s="1">
         <v>0.68000000715255737</v>
@@ -118736,21 +119816,21 @@
       </c>
       <c r="G30" s="1"/>
       <c r="H30" t="s">
-        <v>39048</v>
+        <v>39408</v>
       </c>
       <c r="I30" t="s">
-        <v>39089</v>
+        <v>39449</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>38939</v>
+        <v>39299</v>
       </c>
       <c r="B31" t="s">
-        <v>38981</v>
+        <v>39341</v>
       </c>
       <c r="C31" t="s">
-        <v>39021</v>
+        <v>39381</v>
       </c>
       <c r="D31" s="1">
         <v>0.72000002861022949</v>
@@ -118763,21 +119843,21 @@
       </c>
       <c r="G31" s="1"/>
       <c r="H31" t="s">
-        <v>39048</v>
+        <v>39408</v>
       </c>
       <c r="I31" t="s">
-        <v>39090</v>
+        <v>39450</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>38940</v>
+        <v>39300</v>
       </c>
       <c r="B32" t="s">
-        <v>38982</v>
+        <v>39342</v>
       </c>
       <c r="C32" t="s">
-        <v>39021</v>
+        <v>39381</v>
       </c>
       <c r="D32" s="1">
         <v>0.75</v>
@@ -118790,21 +119870,21 @@
       </c>
       <c r="G32" s="1"/>
       <c r="H32" t="s">
-        <v>39049</v>
+        <v>39409</v>
       </c>
       <c r="I32" t="s">
-        <v>39091</v>
+        <v>39451</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>38940</v>
+        <v>39300</v>
       </c>
       <c r="B33" t="s">
-        <v>38983</v>
+        <v>39343</v>
       </c>
       <c r="C33" t="s">
-        <v>39021</v>
+        <v>39381</v>
       </c>
       <c r="D33" s="1">
         <v>0.54000002145767212</v>
@@ -118817,21 +119897,21 @@
       </c>
       <c r="G33" s="1"/>
       <c r="H33" t="s">
-        <v>39049</v>
+        <v>39409</v>
       </c>
       <c r="I33" t="s">
-        <v>39092</v>
+        <v>39452</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>38940</v>
+        <v>39300</v>
       </c>
       <c r="B34" t="s">
-        <v>38984</v>
+        <v>39344</v>
       </c>
       <c r="C34" t="s">
-        <v>39022</v>
+        <v>39382</v>
       </c>
       <c r="D34" s="1">
         <v>1.6699999570846558</v>
@@ -118844,21 +119924,21 @@
       </c>
       <c r="G34" s="1"/>
       <c r="H34" t="s">
-        <v>39050</v>
+        <v>39410</v>
       </c>
       <c r="I34" t="s">
-        <v>39093</v>
+        <v>39453</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>38940</v>
+        <v>39300</v>
       </c>
       <c r="B35" t="s">
-        <v>38985</v>
+        <v>39345</v>
       </c>
       <c r="C35" t="s">
-        <v>39022</v>
+        <v>39382</v>
       </c>
       <c r="D35" s="1">
         <v>2.3299999237060547</v>
@@ -118871,21 +119951,21 @@
       </c>
       <c r="G35" s="1"/>
       <c r="H35" t="s">
-        <v>39050</v>
+        <v>39410</v>
       </c>
       <c r="I35" t="s">
-        <v>39094</v>
+        <v>39454</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>38941</v>
+        <v>39301</v>
       </c>
       <c r="B36" t="s">
-        <v>38986</v>
+        <v>39346</v>
       </c>
       <c r="C36" t="s">
-        <v>39023</v>
+        <v>39383</v>
       </c>
       <c r="D36" s="1">
         <v>0.15999999642372131</v>
@@ -118898,21 +119978,21 @@
       </c>
       <c r="G36" s="1"/>
       <c r="H36" t="s">
-        <v>39051</v>
+        <v>39411</v>
       </c>
       <c r="I36" t="s">
-        <v>39095</v>
+        <v>39455</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>38941</v>
+        <v>39301</v>
       </c>
       <c r="B37" t="s">
-        <v>38987</v>
+        <v>39347</v>
       </c>
       <c r="C37" t="s">
-        <v>39023</v>
+        <v>39383</v>
       </c>
       <c r="D37" s="1">
         <v>0.51999998092651367</v>
@@ -118925,21 +120005,21 @@
       </c>
       <c r="G37" s="1"/>
       <c r="H37" t="s">
-        <v>39051</v>
+        <v>39411</v>
       </c>
       <c r="I37" t="s">
-        <v>39096</v>
+        <v>39456</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>38941</v>
+        <v>39301</v>
       </c>
       <c r="B38" t="s">
-        <v>38988</v>
+        <v>39348</v>
       </c>
       <c r="C38" t="s">
-        <v>39023</v>
+        <v>39383</v>
       </c>
       <c r="D38" s="1">
         <v>0.62999999523162842</v>
@@ -118952,21 +120032,21 @@
       </c>
       <c r="G38" s="1"/>
       <c r="H38" t="s">
-        <v>39051</v>
+        <v>39411</v>
       </c>
       <c r="I38" t="s">
-        <v>39097</v>
+        <v>39457</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>38941</v>
+        <v>39301</v>
       </c>
       <c r="B39" t="s">
-        <v>38989</v>
+        <v>39349</v>
       </c>
       <c r="C39" t="s">
-        <v>39023</v>
+        <v>39383</v>
       </c>
       <c r="D39" s="1">
         <v>0.25999999046325684</v>
@@ -118979,21 +120059,21 @@
       </c>
       <c r="G39" s="1"/>
       <c r="H39" t="s">
-        <v>39051</v>
+        <v>39411</v>
       </c>
       <c r="I39" t="s">
-        <v>39098</v>
+        <v>39458</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>38942</v>
+        <v>39302</v>
       </c>
       <c r="B40" t="s">
-        <v>38990</v>
+        <v>39350</v>
       </c>
       <c r="C40" t="s">
-        <v>39023</v>
+        <v>39383</v>
       </c>
       <c r="D40" s="1">
         <v>0.2199999988079071</v>
@@ -119006,21 +120086,21 @@
       </c>
       <c r="G40" s="1"/>
       <c r="H40" t="s">
-        <v>39051</v>
+        <v>39411</v>
       </c>
       <c r="I40" t="s">
-        <v>39099</v>
+        <v>39459</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>38942</v>
+        <v>39302</v>
       </c>
       <c r="B41" t="s">
-        <v>38991</v>
+        <v>39351</v>
       </c>
       <c r="C41" t="s">
-        <v>39023</v>
+        <v>39383</v>
       </c>
       <c r="D41" s="1">
         <v>0.46000000834465027</v>
@@ -119033,21 +120113,21 @@
       </c>
       <c r="G41" s="1"/>
       <c r="H41" t="s">
-        <v>39051</v>
+        <v>39411</v>
       </c>
       <c r="I41" t="s">
-        <v>39100</v>
+        <v>39460</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>38942</v>
+        <v>39302</v>
       </c>
       <c r="B42" t="s">
-        <v>38992</v>
+        <v>39352</v>
       </c>
       <c r="C42" t="s">
-        <v>39023</v>
+        <v>39383</v>
       </c>
       <c r="D42" s="1">
         <v>0.60000002384185791</v>
@@ -119060,21 +120140,21 @@
       </c>
       <c r="G42" s="1"/>
       <c r="H42" t="s">
-        <v>39051</v>
+        <v>39411</v>
       </c>
       <c r="I42" t="s">
-        <v>39101</v>
+        <v>39461</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>38942</v>
+        <v>39302</v>
       </c>
       <c r="B43" t="s">
-        <v>38993</v>
+        <v>39353</v>
       </c>
       <c r="C43" t="s">
-        <v>39023</v>
+        <v>39383</v>
       </c>
       <c r="D43" s="1">
         <v>0.37000000476837158</v>
@@ -119087,21 +120167,21 @@
       </c>
       <c r="G43" s="1"/>
       <c r="H43" t="s">
-        <v>39051</v>
+        <v>39411</v>
       </c>
       <c r="I43" t="s">
-        <v>39102</v>
+        <v>39462</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>38943</v>
+        <v>39303</v>
       </c>
       <c r="B44" t="s">
-        <v>38994</v>
+        <v>39354</v>
       </c>
       <c r="C44" t="s">
-        <v>39023</v>
+        <v>39383</v>
       </c>
       <c r="D44" s="1">
         <v>0.5899999737739563</v>
@@ -119114,21 +120194,21 @@
       </c>
       <c r="G44" s="1"/>
       <c r="H44" t="s">
-        <v>39052</v>
+        <v>39412</v>
       </c>
       <c r="I44" t="s">
-        <v>39103</v>
+        <v>39463</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>38943</v>
+        <v>39303</v>
       </c>
       <c r="B45" t="s">
-        <v>38995</v>
+        <v>39355</v>
       </c>
       <c r="C45" t="s">
-        <v>39023</v>
+        <v>39383</v>
       </c>
       <c r="D45" s="1">
         <v>0.47999998927116394</v>
@@ -119141,21 +120221,21 @@
       </c>
       <c r="G45" s="1"/>
       <c r="H45" t="s">
-        <v>39052</v>
+        <v>39412</v>
       </c>
       <c r="I45" t="s">
-        <v>39104</v>
+        <v>39464</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>38944</v>
+        <v>39304</v>
       </c>
       <c r="B46" t="s">
-        <v>38996</v>
+        <v>39356</v>
       </c>
       <c r="C46" t="s">
-        <v>39024</v>
+        <v>39384</v>
       </c>
       <c r="D46" s="1">
         <v>0.77100002765655518</v>
@@ -119168,21 +120248,21 @@
       </c>
       <c r="G46" s="1"/>
       <c r="H46" t="s">
-        <v>39052</v>
+        <v>39412</v>
       </c>
       <c r="I46" t="s">
-        <v>39105</v>
+        <v>39465</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>38944</v>
+        <v>39304</v>
       </c>
       <c r="B47" t="s">
-        <v>38997</v>
+        <v>39357</v>
       </c>
       <c r="C47" t="s">
-        <v>39024</v>
+        <v>39384</v>
       </c>
       <c r="D47" s="1">
         <v>0.75199997425079346</v>
@@ -119195,21 +120275,21 @@
       </c>
       <c r="G47" s="1"/>
       <c r="H47" t="s">
-        <v>39052</v>
+        <v>39412</v>
       </c>
       <c r="I47" t="s">
-        <v>39106</v>
+        <v>39466</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>38945</v>
+        <v>39305</v>
       </c>
       <c r="B48" t="s">
-        <v>38998</v>
+        <v>39358</v>
       </c>
       <c r="C48" t="s">
-        <v>39025</v>
+        <v>39385</v>
       </c>
       <c r="D48" s="1">
         <v>0.54000002145767212</v>
@@ -119222,21 +120302,21 @@
       </c>
       <c r="G48" s="1"/>
       <c r="H48" t="s">
-        <v>39052</v>
+        <v>39412</v>
       </c>
       <c r="I48" t="s">
-        <v>39107</v>
+        <v>39467</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>38945</v>
+        <v>39305</v>
       </c>
       <c r="B49" t="s">
-        <v>38999</v>
+        <v>39359</v>
       </c>
       <c r="C49" t="s">
-        <v>39025</v>
+        <v>39385</v>
       </c>
       <c r="D49" s="1">
         <v>0.67000001668930054</v>
@@ -119249,21 +120329,21 @@
       </c>
       <c r="G49" s="1"/>
       <c r="H49" t="s">
-        <v>39052</v>
+        <v>39412</v>
       </c>
       <c r="I49" t="s">
-        <v>39108</v>
+        <v>39468</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>38945</v>
+        <v>39305</v>
       </c>
       <c r="B50" t="s">
-        <v>39000</v>
+        <v>39360</v>
       </c>
       <c r="C50" t="s">
-        <v>39025</v>
+        <v>39385</v>
       </c>
       <c r="D50" s="1">
         <v>0.60000002384185791</v>
@@ -119276,21 +120356,21 @@
       </c>
       <c r="G50" s="1"/>
       <c r="H50" t="s">
-        <v>39052</v>
+        <v>39412</v>
       </c>
       <c r="I50" t="s">
-        <v>39109</v>
+        <v>39469</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>38946</v>
+        <v>39306</v>
       </c>
       <c r="B51" t="s">
-        <v>39001</v>
+        <v>39361</v>
       </c>
       <c r="C51" t="s">
-        <v>39026</v>
+        <v>39386</v>
       </c>
       <c r="D51" s="1">
         <v>0.97600001096725464</v>
@@ -119303,21 +120383,21 @@
       </c>
       <c r="G51" s="1"/>
       <c r="H51" t="s">
-        <v>39053</v>
+        <v>39413</v>
       </c>
       <c r="I51" t="s">
-        <v>39110</v>
+        <v>39470</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>38946</v>
+        <v>39306</v>
       </c>
       <c r="B52" t="s">
-        <v>39002</v>
+        <v>39362</v>
       </c>
       <c r="C52" t="s">
-        <v>39026</v>
+        <v>39386</v>
       </c>
       <c r="D52" s="1">
         <v>0.92599999904632568</v>
@@ -119330,21 +120410,21 @@
       </c>
       <c r="G52" s="1"/>
       <c r="H52" t="s">
-        <v>39053</v>
+        <v>39413</v>
       </c>
       <c r="I52" t="s">
-        <v>39111</v>
+        <v>39471</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>38946</v>
+        <v>39306</v>
       </c>
       <c r="B53" t="s">
-        <v>39003</v>
+        <v>39363</v>
       </c>
       <c r="C53" t="s">
-        <v>39026</v>
+        <v>39386</v>
       </c>
       <c r="D53" s="1">
         <v>0.88300001621246338</v>
@@ -119357,21 +120437,21 @@
       </c>
       <c r="G53" s="1"/>
       <c r="H53" t="s">
-        <v>39053</v>
+        <v>39413</v>
       </c>
       <c r="I53" t="s">
-        <v>39112</v>
+        <v>39472</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>38947</v>
+        <v>39307</v>
       </c>
       <c r="B54" t="s">
-        <v>39004</v>
+        <v>39364</v>
       </c>
       <c r="C54" t="s">
-        <v>39027</v>
+        <v>39387</v>
       </c>
       <c r="D54" s="1">
         <v>0.6600000262260437</v>
@@ -119384,21 +120464,21 @@
       </c>
       <c r="G54" s="1"/>
       <c r="H54" t="s">
-        <v>39054</v>
+        <v>39414</v>
       </c>
       <c r="I54" t="s">
-        <v>39113</v>
+        <v>39473</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>38947</v>
+        <v>39307</v>
       </c>
       <c r="B55" t="s">
-        <v>39005</v>
+        <v>39365</v>
       </c>
       <c r="C55" t="s">
-        <v>39027</v>
+        <v>39387</v>
       </c>
       <c r="D55" s="1">
         <v>0.63999998569488525</v>
@@ -119411,21 +120491,21 @@
       </c>
       <c r="G55" s="1"/>
       <c r="H55" t="s">
-        <v>39054</v>
+        <v>39414</v>
       </c>
       <c r="I55" t="s">
-        <v>39114</v>
+        <v>39474</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>38948</v>
+        <v>39308</v>
       </c>
       <c r="B56" t="s">
-        <v>39006</v>
+        <v>39366</v>
       </c>
       <c r="C56" t="s">
-        <v>39028</v>
+        <v>39388</v>
       </c>
       <c r="D56" s="1">
         <v>0.89999997615814209</v>
@@ -119438,21 +120518,21 @@
       </c>
       <c r="G56" s="1"/>
       <c r="H56" t="s">
-        <v>39055</v>
+        <v>39415</v>
       </c>
       <c r="I56" t="s">
-        <v>39115</v>
+        <v>39475</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>38948</v>
+        <v>39308</v>
       </c>
       <c r="B57" t="s">
-        <v>39007</v>
+        <v>39367</v>
       </c>
       <c r="C57" t="s">
-        <v>39028</v>
+        <v>39388</v>
       </c>
       <c r="D57" s="1">
         <v>0.95999997854232788</v>
@@ -119465,21 +120545,21 @@
       </c>
       <c r="G57" s="1"/>
       <c r="H57" t="s">
-        <v>39055</v>
+        <v>39415</v>
       </c>
       <c r="I57" t="s">
-        <v>39116</v>
+        <v>39476</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>38949</v>
+        <v>39309</v>
       </c>
       <c r="B58" t="s">
-        <v>39008</v>
+        <v>39368</v>
       </c>
       <c r="C58" t="s">
-        <v>39029</v>
+        <v>39389</v>
       </c>
       <c r="D58" s="1">
         <v>0.4699999988079071</v>
@@ -119492,21 +120572,21 @@
       </c>
       <c r="G58" s="1"/>
       <c r="H58" t="s">
-        <v>39056</v>
+        <v>39416</v>
       </c>
       <c r="I58" t="s">
-        <v>39117</v>
+        <v>39477</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>38949</v>
+        <v>39309</v>
       </c>
       <c r="B59" t="s">
-        <v>39009</v>
+        <v>39369</v>
       </c>
       <c r="C59" t="s">
-        <v>39029</v>
+        <v>39389</v>
       </c>
       <c r="D59" s="1">
         <v>0.47999998927116394</v>
@@ -119519,21 +120599,21 @@
       </c>
       <c r="G59" s="1"/>
       <c r="H59" t="s">
-        <v>39056</v>
+        <v>39416</v>
       </c>
       <c r="I59" t="s">
-        <v>39118</v>
+        <v>39478</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>38949</v>
+        <v>39309</v>
       </c>
       <c r="B60" t="s">
-        <v>39010</v>
+        <v>39370</v>
       </c>
       <c r="C60" t="s">
-        <v>39030</v>
+        <v>39390</v>
       </c>
       <c r="D60" s="1">
         <v>0.43999999761581421</v>
@@ -119546,21 +120626,21 @@
       </c>
       <c r="G60" s="1"/>
       <c r="H60" t="s">
-        <v>39057</v>
+        <v>39417</v>
       </c>
       <c r="I60" t="s">
-        <v>39119</v>
+        <v>39479</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>38949</v>
+        <v>39309</v>
       </c>
       <c r="B61" t="s">
-        <v>39011</v>
+        <v>39371</v>
       </c>
       <c r="C61" t="s">
-        <v>39030</v>
+        <v>39390</v>
       </c>
       <c r="D61" s="1">
         <v>0.75999999046325684</v>
@@ -119573,21 +120653,21 @@
       </c>
       <c r="G61" s="1"/>
       <c r="H61" t="s">
-        <v>39057</v>
+        <v>39417</v>
       </c>
       <c r="I61" t="s">
-        <v>39120</v>
+        <v>39480</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>38950</v>
+        <v>39310</v>
       </c>
       <c r="B62" t="s">
-        <v>39012</v>
+        <v>39372</v>
       </c>
       <c r="C62" t="s">
-        <v>39030</v>
+        <v>39390</v>
       </c>
       <c r="D62" s="1">
         <v>0.81000000238418579</v>
@@ -119600,21 +120680,21 @@
       </c>
       <c r="G62" s="1"/>
       <c r="H62" t="s">
-        <v>39058</v>
+        <v>39418</v>
       </c>
       <c r="I62" t="s">
-        <v>39121</v>
+        <v>39481</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>38950</v>
+        <v>39310</v>
       </c>
       <c r="B63" t="s">
-        <v>39013</v>
+        <v>39373</v>
       </c>
       <c r="C63" t="s">
-        <v>39030</v>
+        <v>39390</v>
       </c>
       <c r="D63" s="1">
         <v>0.79000002145767212</v>
@@ -119627,21 +120707,21 @@
       </c>
       <c r="G63" s="1"/>
       <c r="H63" t="s">
-        <v>39058</v>
+        <v>39418</v>
       </c>
       <c r="I63" t="s">
-        <v>39122</v>
+        <v>39482</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>38951</v>
+        <v>39311</v>
       </c>
       <c r="B64" t="s">
-        <v>39014</v>
+        <v>39374</v>
       </c>
       <c r="C64" t="s">
-        <v>39031</v>
+        <v>39391</v>
       </c>
       <c r="D64" s="1">
         <v>0.6600000262260437</v>
@@ -119654,21 +120734,21 @@
       </c>
       <c r="G64" s="1"/>
       <c r="H64" t="s">
-        <v>39059</v>
+        <v>39419</v>
       </c>
       <c r="I64" t="s">
-        <v>39123</v>
+        <v>39483</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>38951</v>
+        <v>39311</v>
       </c>
       <c r="B65" t="s">
-        <v>39015</v>
+        <v>39375</v>
       </c>
       <c r="C65" t="s">
-        <v>39031</v>
+        <v>39391</v>
       </c>
       <c r="D65" s="1">
         <v>0.55000001192092896</v>
@@ -119681,10 +120761,10 @@
       </c>
       <c r="G65" s="1"/>
       <c r="H65" t="s">
-        <v>39059</v>
+        <v>39419</v>
       </c>
       <c r="I65" t="s">
-        <v>39124</v>
+        <v>39484</v>
       </c>
     </row>
   </sheetData>
@@ -119698,42 +120778,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>39125</v>
+        <v>39485</v>
       </c>
       <c r="B1" t="s">
-        <v>39147</v>
+        <v>39507</v>
       </c>
       <c r="C1" t="s">
-        <v>39194</v>
+        <v>39554</v>
       </c>
       <c r="D1" t="s">
-        <v>39204</v>
+        <v>39564</v>
       </c>
       <c r="E1" t="s">
-        <v>39205</v>
+        <v>39565</v>
       </c>
       <c r="F1" t="s">
-        <v>39206</v>
+        <v>39566</v>
       </c>
       <c r="G1" t="s">
-        <v>39207</v>
+        <v>39567</v>
       </c>
       <c r="H1" t="s">
-        <v>39219</v>
+        <v>39579</v>
       </c>
       <c r="I1" t="s">
-        <v>39240</v>
+        <v>39600</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>39126</v>
+        <v>39486</v>
       </c>
       <c r="B2" t="s">
-        <v>39148</v>
+        <v>39508</v>
       </c>
       <c r="C2" t="s">
-        <v>39195</v>
+        <v>39555</v>
       </c>
       <c r="D2" s="1">
         <v>0.5899999737739563</v>
@@ -119745,24 +120825,24 @@
         <v>0.81999999284744263</v>
       </c>
       <c r="G2" t="s">
-        <v>39208</v>
+        <v>39568</v>
       </c>
       <c r="H2" t="s">
-        <v>39220</v>
+        <v>39580</v>
       </c>
       <c r="I2" t="s">
-        <v>39241</v>
+        <v>39601</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>39126</v>
+        <v>39486</v>
       </c>
       <c r="B3" t="s">
-        <v>39149</v>
+        <v>39509</v>
       </c>
       <c r="C3" t="s">
-        <v>39195</v>
+        <v>39555</v>
       </c>
       <c r="D3" s="1">
         <v>0.18000000715255737</v>
@@ -119774,24 +120854,24 @@
         <v>1.4900000095367432</v>
       </c>
       <c r="G3" t="s">
-        <v>39208</v>
+        <v>39568</v>
       </c>
       <c r="H3" t="s">
-        <v>39220</v>
+        <v>39580</v>
       </c>
       <c r="I3" t="s">
-        <v>39242</v>
+        <v>39602</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>39127</v>
+        <v>39487</v>
       </c>
       <c r="B4" t="s">
-        <v>39150</v>
+        <v>39510</v>
       </c>
       <c r="C4" t="s">
-        <v>39195</v>
+        <v>39555</v>
       </c>
       <c r="D4" s="1">
         <v>0.37999999523162842</v>
@@ -119803,24 +120883,24 @@
         <v>0.6600000262260437</v>
       </c>
       <c r="G4" t="s">
-        <v>39208</v>
+        <v>39568</v>
       </c>
       <c r="H4" t="s">
-        <v>39221</v>
+        <v>39581</v>
       </c>
       <c r="I4" t="s">
-        <v>39243</v>
+        <v>39603</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>39127</v>
+        <v>39487</v>
       </c>
       <c r="B5" t="s">
-        <v>39151</v>
+        <v>39511</v>
       </c>
       <c r="C5" t="s">
-        <v>39195</v>
+        <v>39555</v>
       </c>
       <c r="D5" s="1">
         <v>0.44999998807907104</v>
@@ -119832,24 +120912,24 @@
         <v>0.57999998331069946</v>
       </c>
       <c r="G5" t="s">
-        <v>39208</v>
+        <v>39568</v>
       </c>
       <c r="H5" t="s">
-        <v>39221</v>
+        <v>39581</v>
       </c>
       <c r="I5" t="s">
-        <v>39244</v>
+        <v>39604</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>39128</v>
+        <v>39488</v>
       </c>
       <c r="B6" t="s">
-        <v>39152</v>
+        <v>39512</v>
       </c>
       <c r="C6" t="s">
-        <v>39195</v>
+        <v>39555</v>
       </c>
       <c r="D6" s="1">
         <v>0.75700002908706665</v>
@@ -119861,24 +120941,24 @@
         <v>0.96299999952316284</v>
       </c>
       <c r="G6" t="s">
-        <v>39209</v>
+        <v>39569</v>
       </c>
       <c r="H6" t="s">
-        <v>39222</v>
+        <v>39582</v>
       </c>
       <c r="I6" t="s">
-        <v>39245</v>
+        <v>39605</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>39128</v>
+        <v>39488</v>
       </c>
       <c r="B7" t="s">
-        <v>39153</v>
+        <v>39513</v>
       </c>
       <c r="C7" t="s">
-        <v>39195</v>
+        <v>39555</v>
       </c>
       <c r="D7" s="1">
         <v>0.92599999904632568</v>
@@ -119890,24 +120970,24 @@
         <v>1.2790000438690186</v>
       </c>
       <c r="G7" t="s">
-        <v>39210</v>
+        <v>39570</v>
       </c>
       <c r="H7" t="s">
-        <v>39222</v>
+        <v>39582</v>
       </c>
       <c r="I7" t="s">
-        <v>39246</v>
+        <v>39606</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>39129</v>
+        <v>39489</v>
       </c>
       <c r="B8" t="s">
-        <v>39154</v>
+        <v>39514</v>
       </c>
       <c r="C8" t="s">
-        <v>39195</v>
+        <v>39555</v>
       </c>
       <c r="D8" s="1">
         <v>0.43999999761581421</v>
@@ -119919,24 +120999,24 @@
         <v>0.56000000238418579</v>
       </c>
       <c r="G8" t="s">
-        <v>39211</v>
+        <v>39571</v>
       </c>
       <c r="H8" t="s">
-        <v>39223</v>
+        <v>39583</v>
       </c>
       <c r="I8" t="s">
-        <v>39247</v>
+        <v>39607</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>39129</v>
+        <v>39489</v>
       </c>
       <c r="B9" t="s">
-        <v>39155</v>
+        <v>39515</v>
       </c>
       <c r="C9" t="s">
-        <v>39195</v>
+        <v>39555</v>
       </c>
       <c r="D9" s="1">
         <v>0.80000001192092896</v>
@@ -119948,24 +121028,24 @@
         <v>1.1100000143051147</v>
       </c>
       <c r="G9" t="s">
-        <v>39211</v>
+        <v>39571</v>
       </c>
       <c r="H9" t="s">
-        <v>39223</v>
+        <v>39583</v>
       </c>
       <c r="I9" t="s">
-        <v>39248</v>
+        <v>39608</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>39130</v>
+        <v>39490</v>
       </c>
       <c r="B10" t="s">
-        <v>39156</v>
+        <v>39516</v>
       </c>
       <c r="C10" t="s">
-        <v>39195</v>
+        <v>39555</v>
       </c>
       <c r="D10" s="1">
         <v>0.56000000238418579</v>
@@ -119977,24 +121057,24 @@
         <v>0.97000002861022949</v>
       </c>
       <c r="G10" t="s">
-        <v>39211</v>
+        <v>39571</v>
       </c>
       <c r="H10" t="s">
-        <v>39224</v>
+        <v>39584</v>
       </c>
       <c r="I10" t="s">
-        <v>39249</v>
+        <v>39609</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>39130</v>
+        <v>39490</v>
       </c>
       <c r="B11" t="s">
-        <v>39157</v>
+        <v>39517</v>
       </c>
       <c r="C11" t="s">
-        <v>39195</v>
+        <v>39555</v>
       </c>
       <c r="D11" s="1">
         <v>0.50999999046325684</v>
@@ -120006,24 +121086,24 @@
         <v>1.190000057220459</v>
       </c>
       <c r="G11" t="s">
-        <v>39211</v>
+        <v>39571</v>
       </c>
       <c r="H11" t="s">
-        <v>39224</v>
+        <v>39584</v>
       </c>
       <c r="I11" t="s">
-        <v>39250</v>
+        <v>39610</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>39131</v>
+        <v>39491</v>
       </c>
       <c r="B12" t="s">
-        <v>39158</v>
+        <v>39518</v>
       </c>
       <c r="C12" t="s">
-        <v>39195</v>
+        <v>39555</v>
       </c>
       <c r="D12" s="1">
         <v>0.6600000262260437</v>
@@ -120035,24 +121115,24 @@
         <v>0.89999997615814209</v>
       </c>
       <c r="G12" t="s">
-        <v>39211</v>
+        <v>39571</v>
       </c>
       <c r="H12" t="s">
-        <v>39225</v>
+        <v>39585</v>
       </c>
       <c r="I12" t="s">
-        <v>39251</v>
+        <v>39611</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>39131</v>
+        <v>39491</v>
       </c>
       <c r="B13" t="s">
-        <v>39159</v>
+        <v>39519</v>
       </c>
       <c r="C13" t="s">
-        <v>39195</v>
+        <v>39555</v>
       </c>
       <c r="D13" s="1">
         <v>0.36000001430511475</v>
@@ -120064,24 +121144,24 @@
         <v>0.82999998331069946</v>
       </c>
       <c r="G13" t="s">
-        <v>39211</v>
+        <v>39571</v>
       </c>
       <c r="H13" t="s">
-        <v>39225</v>
+        <v>39585</v>
       </c>
       <c r="I13" t="s">
-        <v>39252</v>
+        <v>39612</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>39132</v>
+        <v>39492</v>
       </c>
       <c r="B14" t="s">
-        <v>39160</v>
+        <v>39520</v>
       </c>
       <c r="C14" t="s">
-        <v>39195</v>
+        <v>39555</v>
       </c>
       <c r="D14" s="1">
         <v>0.55299997329711914</v>
@@ -120093,24 +121173,24 @@
         <v>0.9309999942779541</v>
       </c>
       <c r="G14" t="s">
-        <v>39212</v>
+        <v>39572</v>
       </c>
       <c r="H14" t="s">
-        <v>39226</v>
+        <v>39586</v>
       </c>
       <c r="I14" t="s">
-        <v>39253</v>
+        <v>39613</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>39132</v>
+        <v>39492</v>
       </c>
       <c r="B15" t="s">
-        <v>39161</v>
+        <v>39521</v>
       </c>
       <c r="C15" t="s">
-        <v>39195</v>
+        <v>39555</v>
       </c>
       <c r="D15" s="1">
         <v>0.76599997282028198</v>
@@ -120122,24 +121202,24 @@
         <v>3.9639999866485596</v>
       </c>
       <c r="G15" t="s">
-        <v>39212</v>
+        <v>39572</v>
       </c>
       <c r="H15" t="s">
-        <v>39226</v>
+        <v>39586</v>
       </c>
       <c r="I15" t="s">
-        <v>39254</v>
+        <v>39614</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>39132</v>
+        <v>39492</v>
       </c>
       <c r="B16" t="s">
-        <v>39162</v>
+        <v>39522</v>
       </c>
       <c r="C16" t="s">
-        <v>39196</v>
+        <v>39556</v>
       </c>
       <c r="D16" s="1">
         <v>0.39800000190734863</v>
@@ -120151,24 +121231,24 @@
         <v>0.71899998188018799</v>
       </c>
       <c r="G16" t="s">
-        <v>39212</v>
+        <v>39572</v>
       </c>
       <c r="H16" t="s">
-        <v>39227</v>
+        <v>39587</v>
       </c>
       <c r="I16" t="s">
-        <v>39255</v>
+        <v>39615</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>39132</v>
+        <v>39492</v>
       </c>
       <c r="B17" t="s">
-        <v>39163</v>
+        <v>39523</v>
       </c>
       <c r="C17" t="s">
-        <v>39196</v>
+        <v>39556</v>
       </c>
       <c r="D17" s="1">
         <v>0.49799999594688416</v>
@@ -120180,24 +121260,24 @@
         <v>2.4030001163482666</v>
       </c>
       <c r="G17" t="s">
-        <v>39212</v>
+        <v>39572</v>
       </c>
       <c r="H17" t="s">
-        <v>39227</v>
+        <v>39587</v>
       </c>
       <c r="I17" t="s">
-        <v>39256</v>
+        <v>39616</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>39133</v>
+        <v>39493</v>
       </c>
       <c r="B18" t="s">
-        <v>39164</v>
+        <v>39524</v>
       </c>
       <c r="C18" t="s">
-        <v>39197</v>
+        <v>39557</v>
       </c>
       <c r="D18" s="1">
         <v>0.87000000476837158</v>
@@ -120209,24 +121289,24 @@
         <v>1.2899999618530273</v>
       </c>
       <c r="G18" t="s">
-        <v>39213</v>
+        <v>39573</v>
       </c>
       <c r="H18" t="s">
-        <v>39228</v>
+        <v>39588</v>
       </c>
       <c r="I18" t="s">
-        <v>39257</v>
+        <v>39617</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>39133</v>
+        <v>39493</v>
       </c>
       <c r="B19" t="s">
-        <v>39165</v>
+        <v>39525</v>
       </c>
       <c r="C19" t="s">
-        <v>39197</v>
+        <v>39557</v>
       </c>
       <c r="D19" s="1">
         <v>0.38999998569488525</v>
@@ -120238,24 +121318,24 @@
         <v>0.80000001192092896</v>
       </c>
       <c r="G19" t="s">
-        <v>39213</v>
+        <v>39573</v>
       </c>
       <c r="H19" t="s">
-        <v>39228</v>
+        <v>39588</v>
       </c>
       <c r="I19" t="s">
-        <v>39258</v>
+        <v>39618</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>39134</v>
+        <v>39494</v>
       </c>
       <c r="B20" t="s">
-        <v>39166</v>
+        <v>39526</v>
       </c>
       <c r="C20" t="s">
-        <v>39197</v>
+        <v>39557</v>
       </c>
       <c r="D20" s="1">
         <v>0.61000001430511475</v>
@@ -120267,24 +121347,24 @@
         <v>1.1699999570846558</v>
       </c>
       <c r="G20" t="s">
-        <v>39213</v>
+        <v>39573</v>
       </c>
       <c r="H20" t="s">
-        <v>39229</v>
+        <v>39589</v>
       </c>
       <c r="I20" t="s">
-        <v>39259</v>
+        <v>39619</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>39134</v>
+        <v>39494</v>
       </c>
       <c r="B21" t="s">
-        <v>39167</v>
+        <v>39527</v>
       </c>
       <c r="C21" t="s">
-        <v>39197</v>
+        <v>39557</v>
       </c>
       <c r="D21" s="1">
         <v>0.75</v>
@@ -120296,24 +121376,24 @@
         <v>1.3600000143051147</v>
       </c>
       <c r="G21" t="s">
-        <v>39213</v>
+        <v>39573</v>
       </c>
       <c r="H21" t="s">
-        <v>39229</v>
+        <v>39589</v>
       </c>
       <c r="I21" t="s">
-        <v>39260</v>
+        <v>39620</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>39134</v>
+        <v>39494</v>
       </c>
       <c r="B22" t="s">
-        <v>39168</v>
+        <v>39528</v>
       </c>
       <c r="C22" t="s">
-        <v>39198</v>
+        <v>39558</v>
       </c>
       <c r="D22" s="1">
         <v>5.9000000953674316</v>
@@ -120325,24 +121405,24 @@
         <v>46.099998474121094</v>
       </c>
       <c r="G22" t="s">
-        <v>39213</v>
+        <v>39573</v>
       </c>
       <c r="H22" t="s">
-        <v>39230</v>
+        <v>39590</v>
       </c>
       <c r="I22" t="s">
-        <v>39261</v>
+        <v>39621</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>39134</v>
+        <v>39494</v>
       </c>
       <c r="B23" t="s">
-        <v>39169</v>
+        <v>39529</v>
       </c>
       <c r="C23" t="s">
-        <v>39198</v>
+        <v>39558</v>
       </c>
       <c r="D23" s="1">
         <v>1.8200000524520874</v>
@@ -120354,24 +121434,24 @@
         <v>5.1399998664855957</v>
       </c>
       <c r="G23" t="s">
-        <v>39213</v>
+        <v>39573</v>
       </c>
       <c r="H23" t="s">
-        <v>39230</v>
+        <v>39590</v>
       </c>
       <c r="I23" t="s">
-        <v>39262</v>
+        <v>39622</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>39135</v>
+        <v>39495</v>
       </c>
       <c r="B24" t="s">
-        <v>39170</v>
+        <v>39530</v>
       </c>
       <c r="C24" t="s">
-        <v>39199</v>
+        <v>39559</v>
       </c>
       <c r="D24" s="1">
         <v>0.5899999737739563</v>
@@ -120383,24 +121463,24 @@
         <v>1.3999999761581421</v>
       </c>
       <c r="G24" t="s">
-        <v>39213</v>
+        <v>39573</v>
       </c>
       <c r="H24" t="s">
-        <v>39231</v>
+        <v>39591</v>
       </c>
       <c r="I24" t="s">
-        <v>39263</v>
+        <v>39623</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>39135</v>
+        <v>39495</v>
       </c>
       <c r="B25" t="s">
-        <v>39171</v>
+        <v>39531</v>
       </c>
       <c r="C25" t="s">
-        <v>39199</v>
+        <v>39559</v>
       </c>
       <c r="D25" s="1">
         <v>0.69999998807907104</v>
@@ -120412,24 +121492,24 @@
         <v>0.87000000476837158</v>
       </c>
       <c r="G25" t="s">
-        <v>39213</v>
+        <v>39573</v>
       </c>
       <c r="H25" t="s">
-        <v>39231</v>
+        <v>39591</v>
       </c>
       <c r="I25" t="s">
-        <v>39264</v>
+        <v>39624</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>39136</v>
+        <v>39496</v>
       </c>
       <c r="B26" t="s">
-        <v>39172</v>
+        <v>39532</v>
       </c>
       <c r="C26" t="s">
-        <v>39199</v>
+        <v>39559</v>
       </c>
       <c r="D26" s="1">
         <v>0.38999998569488525</v>
@@ -120441,24 +121521,24 @@
         <v>0.68999999761581421</v>
       </c>
       <c r="G26" t="s">
-        <v>39213</v>
+        <v>39573</v>
       </c>
       <c r="H26" t="s">
-        <v>39232</v>
+        <v>39592</v>
       </c>
       <c r="I26" t="s">
-        <v>39265</v>
+        <v>39625</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>39136</v>
+        <v>39496</v>
       </c>
       <c r="B27" t="s">
-        <v>39173</v>
+        <v>39533</v>
       </c>
       <c r="C27" t="s">
-        <v>39199</v>
+        <v>39559</v>
       </c>
       <c r="D27" s="1">
         <v>0.15999999642372131</v>
@@ -120470,24 +121550,24 @@
         <v>0.40000000596046448</v>
       </c>
       <c r="G27" t="s">
-        <v>39213</v>
+        <v>39573</v>
       </c>
       <c r="H27" t="s">
-        <v>39232</v>
+        <v>39592</v>
       </c>
       <c r="I27" t="s">
-        <v>39266</v>
+        <v>39626</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>39137</v>
+        <v>39497</v>
       </c>
       <c r="B28" t="s">
-        <v>39174</v>
+        <v>39534</v>
       </c>
       <c r="C28" t="s">
-        <v>39199</v>
+        <v>39559</v>
       </c>
       <c r="D28" s="1">
         <v>0.46000000834465027</v>
@@ -120499,24 +121579,24 @@
         <v>0.6600000262260437</v>
       </c>
       <c r="G28" t="s">
-        <v>39213</v>
+        <v>39573</v>
       </c>
       <c r="H28" t="s">
-        <v>39232</v>
+        <v>39592</v>
       </c>
       <c r="I28" t="s">
-        <v>39267</v>
+        <v>39627</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>39137</v>
+        <v>39497</v>
       </c>
       <c r="B29" t="s">
-        <v>39175</v>
+        <v>39535</v>
       </c>
       <c r="C29" t="s">
-        <v>39199</v>
+        <v>39559</v>
       </c>
       <c r="D29" s="1">
         <v>0.30000001192092896</v>
@@ -120528,24 +121608,24 @@
         <v>0.44999998807907104</v>
       </c>
       <c r="G29" t="s">
-        <v>39213</v>
+        <v>39573</v>
       </c>
       <c r="H29" t="s">
-        <v>39232</v>
+        <v>39592</v>
       </c>
       <c r="I29" t="s">
-        <v>39268</v>
+        <v>39628</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>39138</v>
+        <v>39498</v>
       </c>
       <c r="B30" t="s">
-        <v>39176</v>
+        <v>39536</v>
       </c>
       <c r="C30" t="s">
-        <v>39199</v>
+        <v>39559</v>
       </c>
       <c r="D30" s="1">
         <v>0.60000002384185791</v>
@@ -120557,24 +121637,24 @@
         <v>1.059999942779541</v>
       </c>
       <c r="G30" t="s">
-        <v>39213</v>
+        <v>39573</v>
       </c>
       <c r="H30" t="s">
-        <v>39233</v>
+        <v>39593</v>
       </c>
       <c r="I30" t="s">
-        <v>39269</v>
+        <v>39629</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>39138</v>
+        <v>39498</v>
       </c>
       <c r="B31" t="s">
-        <v>39177</v>
+        <v>39537</v>
       </c>
       <c r="C31" t="s">
-        <v>39199</v>
+        <v>39559</v>
       </c>
       <c r="D31" s="1">
         <v>0.47999998927116394</v>
@@ -120586,24 +121666,24 @@
         <v>0.81999999284744263</v>
       </c>
       <c r="G31" t="s">
-        <v>39213</v>
+        <v>39573</v>
       </c>
       <c r="H31" t="s">
-        <v>39233</v>
+        <v>39593</v>
       </c>
       <c r="I31" t="s">
-        <v>39270</v>
+        <v>39630</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>39139</v>
+        <v>39499</v>
       </c>
       <c r="B32" t="s">
-        <v>39178</v>
+        <v>39538</v>
       </c>
       <c r="C32" t="s">
-        <v>39199</v>
+        <v>39559</v>
       </c>
       <c r="D32" s="1">
         <v>1.6200000047683716</v>
@@ -120615,24 +121695,24 @@
         <v>2.4100000858306885</v>
       </c>
       <c r="G32" t="s">
-        <v>39213</v>
+        <v>39573</v>
       </c>
       <c r="H32" t="s">
-        <v>39233</v>
+        <v>39593</v>
       </c>
       <c r="I32" t="s">
-        <v>39271</v>
+        <v>39631</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>39139</v>
+        <v>39499</v>
       </c>
       <c r="B33" t="s">
-        <v>39179</v>
+        <v>39539</v>
       </c>
       <c r="C33" t="s">
-        <v>39199</v>
+        <v>39559</v>
       </c>
       <c r="D33" s="1">
         <v>2.0099999904632568</v>
@@ -120644,24 +121724,24 @@
         <v>2.8399999141693115</v>
       </c>
       <c r="G33" t="s">
-        <v>39213</v>
+        <v>39573</v>
       </c>
       <c r="H33" t="s">
-        <v>39233</v>
+        <v>39593</v>
       </c>
       <c r="I33" t="s">
-        <v>39272</v>
+        <v>39632</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>39140</v>
+        <v>39500</v>
       </c>
       <c r="B34" t="s">
-        <v>39180</v>
+        <v>39540</v>
       </c>
       <c r="C34" t="s">
-        <v>39200</v>
+        <v>39560</v>
       </c>
       <c r="D34" s="1">
         <v>0.95999997854232788</v>
@@ -120673,24 +121753,24 @@
         <v>1.2560000419616699</v>
       </c>
       <c r="G34" t="s">
-        <v>39214</v>
+        <v>39574</v>
       </c>
       <c r="H34" t="s">
-        <v>39234</v>
+        <v>39594</v>
       </c>
       <c r="I34" t="s">
-        <v>39273</v>
+        <v>39633</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>39140</v>
+        <v>39500</v>
       </c>
       <c r="B35" t="s">
-        <v>39181</v>
+        <v>39541</v>
       </c>
       <c r="C35" t="s">
-        <v>39200</v>
+        <v>39560</v>
       </c>
       <c r="D35" s="1">
         <v>1.0800000429153442</v>
@@ -120702,24 +121782,24 @@
         <v>1.3609999418258667</v>
       </c>
       <c r="G35" t="s">
-        <v>39214</v>
+        <v>39574</v>
       </c>
       <c r="H35" t="s">
-        <v>39234</v>
+        <v>39594</v>
       </c>
       <c r="I35" t="s">
-        <v>39274</v>
+        <v>39634</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>39141</v>
+        <v>39501</v>
       </c>
       <c r="B36" t="s">
-        <v>39182</v>
+        <v>39542</v>
       </c>
       <c r="C36" t="s">
-        <v>39200</v>
+        <v>39560</v>
       </c>
       <c r="D36" s="1">
         <v>0.87699997425079346</v>
@@ -120731,24 +121811,24 @@
         <v>1.156000018119812</v>
       </c>
       <c r="G36" t="s">
-        <v>39215</v>
+        <v>39575</v>
       </c>
       <c r="H36" t="s">
-        <v>39235</v>
+        <v>39595</v>
       </c>
       <c r="I36" t="s">
-        <v>39275</v>
+        <v>39635</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>39141</v>
+        <v>39501</v>
       </c>
       <c r="B37" t="s">
-        <v>39183</v>
+        <v>39543</v>
       </c>
       <c r="C37" t="s">
-        <v>39200</v>
+        <v>39560</v>
       </c>
       <c r="D37" s="1">
         <v>0.68400001525878906</v>
@@ -120760,24 +121840,24 @@
         <v>0.875</v>
       </c>
       <c r="G37" t="s">
-        <v>39215</v>
+        <v>39575</v>
       </c>
       <c r="H37" t="s">
-        <v>39235</v>
+        <v>39595</v>
       </c>
       <c r="I37" t="s">
-        <v>39276</v>
+        <v>39636</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>39141</v>
+        <v>39501</v>
       </c>
       <c r="B38" t="s">
-        <v>39184</v>
+        <v>39544</v>
       </c>
       <c r="C38" t="s">
-        <v>39200</v>
+        <v>39560</v>
       </c>
       <c r="D38" s="1">
         <v>0.85699999332427979</v>
@@ -120789,24 +121869,24 @@
         <v>1.1779999732971191</v>
       </c>
       <c r="G38" t="s">
-        <v>39215</v>
+        <v>39575</v>
       </c>
       <c r="H38" t="s">
-        <v>39235</v>
+        <v>39595</v>
       </c>
       <c r="I38" t="s">
-        <v>39277</v>
+        <v>39637</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>39142</v>
+        <v>39502</v>
       </c>
       <c r="B39" t="s">
-        <v>39184</v>
+        <v>39544</v>
       </c>
       <c r="C39" t="s">
-        <v>39201</v>
+        <v>39561</v>
       </c>
       <c r="D39" s="1">
         <v>0.64999997615814209</v>
@@ -120818,24 +121898,24 @@
         <v>0.8399999737739563</v>
       </c>
       <c r="G39" t="s">
-        <v>39216</v>
+        <v>39576</v>
       </c>
       <c r="H39" t="s">
-        <v>39235</v>
+        <v>39595</v>
       </c>
       <c r="I39" t="s">
-        <v>39278</v>
+        <v>39638</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>39142</v>
+        <v>39502</v>
       </c>
       <c r="B40" t="s">
-        <v>39185</v>
+        <v>39545</v>
       </c>
       <c r="C40" t="s">
-        <v>39201</v>
+        <v>39561</v>
       </c>
       <c r="D40" s="1">
         <v>0.47999998927116394</v>
@@ -120847,24 +121927,24 @@
         <v>0.75</v>
       </c>
       <c r="G40" t="s">
-        <v>39216</v>
+        <v>39576</v>
       </c>
       <c r="H40" t="s">
-        <v>39235</v>
+        <v>39595</v>
       </c>
       <c r="I40" t="s">
-        <v>39279</v>
+        <v>39639</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>39143</v>
+        <v>39503</v>
       </c>
       <c r="B41" t="s">
-        <v>39186</v>
+        <v>39546</v>
       </c>
       <c r="C41" t="s">
-        <v>39202</v>
+        <v>39562</v>
       </c>
       <c r="D41" s="1">
         <v>0.78100001811981201</v>
@@ -120876,24 +121956,24 @@
         <v>1.3220000267028809</v>
       </c>
       <c r="G41" t="s">
-        <v>39217</v>
+        <v>39577</v>
       </c>
       <c r="H41" t="s">
-        <v>39236</v>
+        <v>39596</v>
       </c>
       <c r="I41" t="s">
-        <v>39280</v>
+        <v>39640</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>39143</v>
+        <v>39503</v>
       </c>
       <c r="B42" t="s">
-        <v>39187</v>
+        <v>39547</v>
       </c>
       <c r="C42" t="s">
-        <v>39202</v>
+        <v>39562</v>
       </c>
       <c r="D42" s="1">
         <v>0.97500002384185791</v>
@@ -120905,24 +121985,24 @@
         <v>1.1829999685287476</v>
       </c>
       <c r="G42" t="s">
-        <v>39217</v>
+        <v>39577</v>
       </c>
       <c r="H42" t="s">
-        <v>39236</v>
+        <v>39596</v>
       </c>
       <c r="I42" t="s">
-        <v>39281</v>
+        <v>39641</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>39144</v>
+        <v>39504</v>
       </c>
       <c r="B43" t="s">
-        <v>39188</v>
+        <v>39548</v>
       </c>
       <c r="C43" t="s">
-        <v>39202</v>
+        <v>39562</v>
       </c>
       <c r="D43" s="1">
         <v>0.93999999761581421</v>
@@ -120934,24 +122014,24 @@
         <v>1.190000057220459</v>
       </c>
       <c r="G43" t="s">
-        <v>39218</v>
+        <v>39578</v>
       </c>
       <c r="H43" t="s">
-        <v>39237</v>
+        <v>39597</v>
       </c>
       <c r="I43" t="s">
-        <v>39282</v>
+        <v>39642</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>39144</v>
+        <v>39504</v>
       </c>
       <c r="B44" t="s">
-        <v>39189</v>
+        <v>39549</v>
       </c>
       <c r="C44" t="s">
-        <v>39202</v>
+        <v>39562</v>
       </c>
       <c r="D44" s="1">
         <v>0.93000000715255737</v>
@@ -120963,24 +122043,24 @@
         <v>1.309999942779541</v>
       </c>
       <c r="G44" t="s">
-        <v>39218</v>
+        <v>39578</v>
       </c>
       <c r="H44" t="s">
-        <v>39237</v>
+        <v>39597</v>
       </c>
       <c r="I44" t="s">
-        <v>39283</v>
+        <v>39643</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>39145</v>
+        <v>39505</v>
       </c>
       <c r="B45" t="s">
-        <v>39190</v>
+        <v>39550</v>
       </c>
       <c r="C45" t="s">
-        <v>39203</v>
+        <v>39563</v>
       </c>
       <c r="D45" s="1">
         <v>0.63999998569488525</v>
@@ -120992,24 +122072,24 @@
         <v>0.9100000262260437</v>
       </c>
       <c r="G45" t="s">
-        <v>39218</v>
+        <v>39578</v>
       </c>
       <c r="H45" t="s">
-        <v>39238</v>
+        <v>39598</v>
       </c>
       <c r="I45" t="s">
-        <v>39284</v>
+        <v>39644</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>39145</v>
+        <v>39505</v>
       </c>
       <c r="B46" t="s">
-        <v>39191</v>
+        <v>39551</v>
       </c>
       <c r="C46" t="s">
-        <v>39203</v>
+        <v>39563</v>
       </c>
       <c r="D46" s="1">
         <v>0.72000002861022949</v>
@@ -121021,24 +122101,24 @@
         <v>0.89999997615814209</v>
       </c>
       <c r="G46" t="s">
-        <v>39218</v>
+        <v>39578</v>
       </c>
       <c r="H46" t="s">
-        <v>39238</v>
+        <v>39598</v>
       </c>
       <c r="I46" t="s">
-        <v>39285</v>
+        <v>39645</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>39146</v>
+        <v>39506</v>
       </c>
       <c r="B47" t="s">
-        <v>39192</v>
+        <v>39552</v>
       </c>
       <c r="C47" t="s">
-        <v>39203</v>
+        <v>39563</v>
       </c>
       <c r="D47" s="1">
         <v>0.46000000834465027</v>
@@ -121050,24 +122130,24 @@
         <v>0.73000001907348633</v>
       </c>
       <c r="G47" t="s">
-        <v>39218</v>
+        <v>39578</v>
       </c>
       <c r="H47" t="s">
-        <v>39239</v>
+        <v>39599</v>
       </c>
       <c r="I47" t="s">
-        <v>39286</v>
+        <v>39646</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>39146</v>
+        <v>39506</v>
       </c>
       <c r="B48" t="s">
-        <v>39193</v>
+        <v>39553</v>
       </c>
       <c r="C48" t="s">
-        <v>39203</v>
+        <v>39563</v>
       </c>
       <c r="D48" s="1">
         <v>0.62999999523162842</v>
@@ -121079,13 +122159,13 @@
         <v>0.89999997615814209</v>
       </c>
       <c r="G48" t="s">
-        <v>39218</v>
+        <v>39578</v>
       </c>
       <c r="H48" t="s">
-        <v>39239</v>
+        <v>39599</v>
       </c>
       <c r="I48" t="s">
-        <v>39287</v>
+        <v>39647</v>
       </c>
     </row>
   </sheetData>

</xml_diff>